<commit_message>
adding heliostat interaction limit input
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C58C90D-A838-4B59-AAE4-5742A2B2984E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33407DEE-4EF9-46F1-B065-BD188AFA0F44}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="907">
   <si>
     <t>String name</t>
   </si>
@@ -2724,6 +2724,18 @@
   </si>
   <si>
     <t>USA CA Daggett (TMY2).csv</t>
+  </si>
+  <si>
+    <t>interaction_limit</t>
+  </si>
+  <si>
+    <t>Multiply the heliostat height to determine the radius of possible interaction with other heliostats</t>
+  </si>
+  <si>
+    <t>Heliostat shading interaction limit</t>
+  </si>
+  <si>
+    <t>helio-ht</t>
   </si>
 </sst>
 </file>
@@ -2962,10 +2974,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L296" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L296" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:L306">
-    <sortCondition ref="A1:A306"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L297" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L297" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:L307">
+    <sortCondition ref="A1:A307"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain" dataDxfId="11"/>
@@ -3306,11 +3318,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L296"/>
+  <dimension ref="A1:L297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:L296"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G292" sqref="G292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12754,31 +12766,31 @@
         <v>4</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>828</v>
+        <v>903</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D292" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E292" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F292" s="11" t="s">
-        <v>308</v>
+        <v>906</v>
       </c>
       <c r="G292" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H292" s="10"/>
       <c r="I292" s="10"/>
       <c r="J292" s="10"/>
       <c r="K292" s="10" t="s">
-        <v>831</v>
+        <v>905</v>
       </c>
       <c r="L292" s="10" t="s">
-        <v>832</v>
+        <v>904</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
@@ -12786,7 +12798,7 @@
         <v>4</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C293" s="9" t="s">
         <v>816</v>
@@ -12807,10 +12819,10 @@
       <c r="I293" s="10"/>
       <c r="J293" s="10"/>
       <c r="K293" s="10" t="s">
-        <v>801</v>
+        <v>831</v>
       </c>
       <c r="L293" s="10" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
@@ -12818,17 +12830,19 @@
         <v>4</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>389</v>
+        <v>827</v>
       </c>
       <c r="C294" s="9" t="s">
         <v>816</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>813</v>
-      </c>
-      <c r="E294" s="12"/>
+        <v>806</v>
+      </c>
+      <c r="E294" s="12">
+        <v>0</v>
+      </c>
       <c r="F294" s="11" t="s">
-        <v>21</v>
+        <v>308</v>
       </c>
       <c r="G294" s="11" t="b">
         <v>0</v>
@@ -12837,10 +12851,10 @@
       <c r="I294" s="10"/>
       <c r="J294" s="10"/>
       <c r="K294" s="10" t="s">
-        <v>390</v>
+        <v>801</v>
       </c>
       <c r="L294" s="10" t="s">
-        <v>390</v>
+        <v>833</v>
       </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
@@ -12848,19 +12862,17 @@
         <v>4</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>856</v>
+        <v>389</v>
       </c>
       <c r="C295" s="9" t="s">
         <v>816</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E295" s="12">
-        <v>0</v>
-      </c>
+        <v>813</v>
+      </c>
+      <c r="E295" s="12"/>
       <c r="F295" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G295" s="11" t="b">
         <v>0</v>
@@ -12869,10 +12881,10 @@
       <c r="I295" s="10"/>
       <c r="J295" s="10"/>
       <c r="K295" s="10" t="s">
-        <v>859</v>
+        <v>390</v>
       </c>
       <c r="L295" s="10" t="s">
-        <v>859</v>
+        <v>390</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
@@ -12880,7 +12892,7 @@
         <v>4</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="C296" s="9" t="s">
         <v>816</v>
@@ -12901,9 +12913,41 @@
       <c r="I296" s="10"/>
       <c r="J296" s="10"/>
       <c r="K296" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="L296" s="10" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A297" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B297" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="C297" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D297" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E297" s="12">
+        <v>0</v>
+      </c>
+      <c r="F297" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G297" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H297" s="10"/>
+      <c r="I297" s="10"/>
+      <c r="J297" s="10"/>
+      <c r="K297" s="10" t="s">
         <v>860</v>
       </c>
-      <c r="L296" s="10" t="s">
+      <c r="L297" s="10" t="s">
         <v>860</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix to scripting window to allow messages from the program to output to the log
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33407DEE-4EF9-46F1-B065-BD188AFA0F44}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E416C80-ABF0-4C6A-956A-3981FEC94781}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3321,8 +3321,8 @@
   <dimension ref="A1:L297"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G292" sqref="G292"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5607,7 +5607,7 @@
         <v>21</v>
       </c>
       <c r="G71" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
adding input control for specifying receiver power fractions
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E416C80-ABF0-4C6A-956A-3981FEC94781}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C5E650-6B7D-4199-9A48-FADCA6769DB7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="913">
   <si>
     <t>String name</t>
   </si>
@@ -2736,6 +2736,24 @@
   </si>
   <si>
     <t>helio-ht</t>
+  </si>
+  <si>
+    <t>power_fraction</t>
+  </si>
+  <si>
+    <t>Multi-receiver power fraction</t>
+  </si>
+  <si>
+    <t>Target fraction of absorbed energy delivered by the heliostat field in configurations with multiple receivers</t>
+  </si>
+  <si>
+    <t>is_multirec_powfrac</t>
+  </si>
+  <si>
+    <t>Specify multi-receiver power fractions</t>
+  </si>
+  <si>
+    <t>Enables the user to specify the fraction of power delivered from the heliostat to each receiver</t>
   </si>
 </sst>
 </file>
@@ -2974,10 +2992,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L297" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L297" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:L307">
-    <sortCondition ref="A1:A307"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L299" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L299" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:L309">
+    <sortCondition ref="A1:A309"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain" dataDxfId="11"/>
@@ -3318,11 +3336,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L297"/>
+  <dimension ref="A1:L299"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A268" sqref="A268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10710,7 +10728,7 @@
         <v>8</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>307</v>
+        <v>907</v>
       </c>
       <c r="C229" s="9" t="s">
         <v>815</v>
@@ -10719,10 +10737,10 @@
         <v>806</v>
       </c>
       <c r="E229" s="12">
-        <v>10.199999999999999</v>
+        <v>1</v>
       </c>
       <c r="F229" s="11" t="s">
-        <v>567</v>
+        <v>21</v>
       </c>
       <c r="G229" s="11" t="b">
         <v>1</v>
@@ -10731,10 +10749,10 @@
       <c r="I229" s="10"/>
       <c r="J229" s="10"/>
       <c r="K229" s="10" t="s">
-        <v>568</v>
+        <v>908</v>
       </c>
       <c r="L229" s="10" t="s">
-        <v>569</v>
+        <v>909</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.25">
@@ -10742,7 +10760,7 @@
         <v>8</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>570</v>
+        <v>307</v>
       </c>
       <c r="C230" s="9" t="s">
         <v>815</v>
@@ -10751,10 +10769,10 @@
         <v>806</v>
       </c>
       <c r="E230" s="12">
-        <v>0</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F230" s="11" t="s">
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="G230" s="11" t="b">
         <v>1</v>
@@ -10763,10 +10781,10 @@
       <c r="I230" s="10"/>
       <c r="J230" s="10"/>
       <c r="K230" s="10" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="L230" s="10" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.25">
@@ -10774,7 +10792,7 @@
         <v>8</v>
       </c>
       <c r="B231" s="9" t="s">
-        <v>15</v>
+        <v>570</v>
       </c>
       <c r="C231" s="9" t="s">
         <v>815</v>
@@ -10786,7 +10804,7 @@
         <v>0</v>
       </c>
       <c r="F231" s="11" t="s">
-        <v>56</v>
+        <v>558</v>
       </c>
       <c r="G231" s="11" t="b">
         <v>1</v>
@@ -10794,11 +10812,11 @@
       <c r="H231" s="10"/>
       <c r="I231" s="10"/>
       <c r="J231" s="10"/>
-      <c r="K231" s="9" t="s">
-        <v>145</v>
+      <c r="K231" s="10" t="s">
+        <v>571</v>
       </c>
       <c r="L231" s="10" t="s">
-        <v>422</v>
+        <v>572</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
@@ -10806,7 +10824,7 @@
         <v>8</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>298</v>
+        <v>15</v>
       </c>
       <c r="C232" s="9" t="s">
         <v>815</v>
@@ -10818,21 +10836,19 @@
         <v>0</v>
       </c>
       <c r="F232" s="11" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G232" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H232" s="10"/>
       <c r="I232" s="10"/>
-      <c r="J232" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="K232" s="10" t="s">
-        <v>300</v>
+      <c r="J232" s="10"/>
+      <c r="K232" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="L232" s="10" t="s">
-        <v>301</v>
+        <v>422</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
@@ -10840,7 +10856,7 @@
         <v>8</v>
       </c>
       <c r="B233" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C233" s="9" t="s">
         <v>815</v>
@@ -10849,7 +10865,7 @@
         <v>806</v>
       </c>
       <c r="E233" s="12">
-        <v>7.75</v>
+        <v>0</v>
       </c>
       <c r="F233" s="11" t="s">
         <v>23</v>
@@ -10863,10 +10879,10 @@
         <v>640</v>
       </c>
       <c r="K233" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L233" s="10" t="s">
-        <v>423</v>
+        <v>301</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
@@ -10874,7 +10890,7 @@
         <v>8</v>
       </c>
       <c r="B234" s="9" t="s">
-        <v>11</v>
+        <v>297</v>
       </c>
       <c r="C234" s="9" t="s">
         <v>815</v>
@@ -10883,7 +10899,7 @@
         <v>806</v>
       </c>
       <c r="E234" s="12">
-        <v>17.649999999999999</v>
+        <v>7.75</v>
       </c>
       <c r="F234" s="11" t="s">
         <v>23</v>
@@ -10893,12 +10909,14 @@
       </c>
       <c r="H234" s="10"/>
       <c r="I234" s="10"/>
-      <c r="J234" s="10"/>
-      <c r="K234" s="9" t="s">
-        <v>119</v>
+      <c r="J234" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K234" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="L234" s="10" t="s">
-        <v>142</v>
+        <v>423</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
@@ -10906,7 +10924,7 @@
         <v>8</v>
       </c>
       <c r="B235" s="9" t="s">
-        <v>431</v>
+        <v>11</v>
       </c>
       <c r="C235" s="9" t="s">
         <v>815</v>
@@ -10915,10 +10933,10 @@
         <v>806</v>
       </c>
       <c r="E235" s="12">
-        <v>0</v>
+        <v>17.649999999999999</v>
       </c>
       <c r="F235" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G235" s="11" t="b">
         <v>1</v>
@@ -10927,10 +10945,10 @@
       <c r="I235" s="10"/>
       <c r="J235" s="10"/>
       <c r="K235" s="9" t="s">
-        <v>429</v>
+        <v>119</v>
       </c>
       <c r="L235" s="10" t="s">
-        <v>430</v>
+        <v>142</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
@@ -10938,7 +10956,7 @@
         <v>8</v>
       </c>
       <c r="B236" s="9" t="s">
-        <v>12</v>
+        <v>431</v>
       </c>
       <c r="C236" s="9" t="s">
         <v>815</v>
@@ -10947,10 +10965,10 @@
         <v>806</v>
       </c>
       <c r="E236" s="12">
-        <v>21.6</v>
+        <v>0</v>
       </c>
       <c r="F236" s="11" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G236" s="11" t="b">
         <v>1</v>
@@ -10959,10 +10977,10 @@
       <c r="I236" s="10"/>
       <c r="J236" s="10"/>
       <c r="K236" s="9" t="s">
-        <v>120</v>
+        <v>429</v>
       </c>
       <c r="L236" s="10" t="s">
-        <v>143</v>
+        <v>430</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
@@ -10970,29 +10988,31 @@
         <v>8</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>313</v>
+        <v>12</v>
       </c>
       <c r="C237" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E237" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="F237" s="11"/>
+        <v>806</v>
+      </c>
+      <c r="E237" s="12">
+        <v>21.6</v>
+      </c>
+      <c r="F237" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G237" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H237" s="10"/>
       <c r="I237" s="10"/>
       <c r="J237" s="10"/>
-      <c r="K237" s="10" t="s">
-        <v>315</v>
+      <c r="K237" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="L237" s="10" t="s">
-        <v>315</v>
+        <v>143</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.25">
@@ -11000,31 +11020,29 @@
         <v>8</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>16</v>
+        <v>313</v>
       </c>
       <c r="C238" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E238" s="12">
-        <v>0</v>
-      </c>
-      <c r="F238" s="11" t="s">
-        <v>23</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="E238" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="F238" s="11"/>
       <c r="G238" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H238" s="10"/>
       <c r="I238" s="10"/>
       <c r="J238" s="10"/>
-      <c r="K238" s="9" t="s">
-        <v>146</v>
+      <c r="K238" s="10" t="s">
+        <v>315</v>
       </c>
       <c r="L238" s="10" t="s">
-        <v>148</v>
+        <v>315</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
@@ -11032,7 +11050,7 @@
         <v>8</v>
       </c>
       <c r="B239" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C239" s="9" t="s">
         <v>815</v>
@@ -11053,10 +11071,10 @@
       <c r="I239" s="10"/>
       <c r="J239" s="10"/>
       <c r="K239" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L239" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
@@ -11064,7 +11082,7 @@
         <v>8</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C240" s="9" t="s">
         <v>815</v>
@@ -11085,10 +11103,10 @@
       <c r="I240" s="10"/>
       <c r="J240" s="10"/>
       <c r="K240" s="9" t="s">
-        <v>303</v>
+        <v>147</v>
       </c>
       <c r="L240" s="10" t="s">
-        <v>426</v>
+        <v>149</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
@@ -11096,35 +11114,31 @@
         <v>8</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>20</v>
+        <v>302</v>
       </c>
       <c r="C241" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D241" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E241" s="12">
         <v>0</v>
       </c>
       <c r="F241" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G241" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H241" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I241" s="10" t="s">
-        <v>771</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H241" s="10"/>
+      <c r="I241" s="10"/>
       <c r="J241" s="10"/>
       <c r="K241" s="9" t="s">
-        <v>24</v>
+        <v>303</v>
       </c>
       <c r="L241" s="10" t="s">
-        <v>150</v>
+        <v>426</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
@@ -11132,31 +11146,35 @@
         <v>8</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E242" s="12">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F242" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G242" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H242" s="10"/>
-      <c r="I242" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H242" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I242" s="10" t="s">
+        <v>771</v>
+      </c>
       <c r="J242" s="10"/>
       <c r="K242" s="9" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="L242" s="10" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
@@ -11164,7 +11182,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>417</v>
+        <v>10</v>
       </c>
       <c r="C243" s="9" t="s">
         <v>815</v>
@@ -11173,24 +11191,22 @@
         <v>806</v>
       </c>
       <c r="E243" s="12">
-        <v>180</v>
+        <v>17</v>
       </c>
       <c r="F243" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G243" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H243" s="10"/>
       <c r="I243" s="10"/>
-      <c r="J243" s="10" t="s">
-        <v>640</v>
-      </c>
+      <c r="J243" s="10"/>
       <c r="K243" s="9" t="s">
-        <v>420</v>
+        <v>118</v>
       </c>
       <c r="L243" s="10" t="s">
-        <v>421</v>
+        <v>141</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
@@ -11198,7 +11214,7 @@
         <v>8</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C244" s="9" t="s">
         <v>815</v>
@@ -11207,7 +11223,7 @@
         <v>806</v>
       </c>
       <c r="E244" s="12">
-        <v>-180</v>
+        <v>180</v>
       </c>
       <c r="F244" s="11" t="s">
         <v>56</v>
@@ -11221,10 +11237,10 @@
         <v>640</v>
       </c>
       <c r="K244" s="9" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="L244" s="10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
@@ -11232,7 +11248,7 @@
         <v>8</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>561</v>
+        <v>416</v>
       </c>
       <c r="C245" s="9" t="s">
         <v>815</v>
@@ -11241,22 +11257,24 @@
         <v>806</v>
       </c>
       <c r="E245" s="12">
-        <v>30</v>
+        <v>-180</v>
       </c>
       <c r="F245" s="11" t="s">
-        <v>291</v>
+        <v>56</v>
       </c>
       <c r="G245" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H245" s="10"/>
       <c r="I245" s="10"/>
-      <c r="J245" s="10"/>
-      <c r="K245" s="10" t="s">
-        <v>562</v>
+      <c r="J245" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K245" s="9" t="s">
+        <v>418</v>
       </c>
       <c r="L245" s="10" t="s">
-        <v>563</v>
+        <v>419</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
@@ -11264,31 +11282,31 @@
         <v>8</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C246" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>803</v>
-      </c>
-      <c r="E246" s="10" t="s">
-        <v>309</v>
+        <v>806</v>
+      </c>
+      <c r="E246" s="12">
+        <v>30</v>
       </c>
       <c r="F246" s="11" t="s">
-        <v>21</v>
+        <v>291</v>
       </c>
       <c r="G246" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H246" s="10"/>
       <c r="I246" s="10"/>
       <c r="J246" s="10"/>
       <c r="K246" s="10" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="L246" s="10" t="s">
-        <v>305</v>
+        <v>563</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
@@ -11296,7 +11314,7 @@
         <v>8</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>304</v>
+        <v>564</v>
       </c>
       <c r="C247" s="9" t="s">
         <v>815</v>
@@ -11317,10 +11335,10 @@
       <c r="I247" s="10"/>
       <c r="J247" s="10"/>
       <c r="K247" s="10" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L247" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
@@ -11328,19 +11346,19 @@
         <v>8</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E248" s="12">
-        <v>0</v>
+        <v>803</v>
+      </c>
+      <c r="E248" s="10" t="s">
+        <v>309</v>
       </c>
       <c r="F248" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G248" s="11" t="b">
         <v>0</v>
@@ -11349,10 +11367,10 @@
       <c r="I248" s="10"/>
       <c r="J248" s="10"/>
       <c r="K248" s="10" t="s">
-        <v>311</v>
+        <v>566</v>
       </c>
       <c r="L248" s="10" t="s">
-        <v>424</v>
+        <v>306</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
@@ -11360,7 +11378,7 @@
         <v>8</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>25</v>
+        <v>310</v>
       </c>
       <c r="C249" s="9" t="s">
         <v>816</v>
@@ -11369,10 +11387,10 @@
         <v>806</v>
       </c>
       <c r="E249" s="12">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="F249" s="11" t="s">
-        <v>23</v>
+        <v>308</v>
       </c>
       <c r="G249" s="11" t="b">
         <v>0</v>
@@ -11380,11 +11398,11 @@
       <c r="H249" s="10"/>
       <c r="I249" s="10"/>
       <c r="J249" s="10"/>
-      <c r="K249" s="9" t="s">
-        <v>140</v>
+      <c r="K249" s="10" t="s">
+        <v>311</v>
       </c>
       <c r="L249" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
@@ -11392,7 +11410,7 @@
         <v>8</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>577</v>
+        <v>25</v>
       </c>
       <c r="C250" s="9" t="s">
         <v>816</v>
@@ -11401,10 +11419,10 @@
         <v>806</v>
       </c>
       <c r="E250" s="12">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="F250" s="11" t="s">
-        <v>574</v>
+        <v>23</v>
       </c>
       <c r="G250" s="11" t="b">
         <v>0</v>
@@ -11412,11 +11430,11 @@
       <c r="H250" s="10"/>
       <c r="I250" s="10"/>
       <c r="J250" s="10"/>
-      <c r="K250" s="10" t="s">
-        <v>578</v>
+      <c r="K250" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="L250" s="10" t="s">
-        <v>579</v>
+        <v>425</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
@@ -11424,7 +11442,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>294</v>
+        <v>577</v>
       </c>
       <c r="C251" s="9" t="s">
         <v>816</v>
@@ -11433,22 +11451,22 @@
         <v>806</v>
       </c>
       <c r="E251" s="12">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="F251" s="11" t="s">
-        <v>21</v>
+        <v>574</v>
       </c>
       <c r="G251" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H251" s="10"/>
       <c r="I251" s="10"/>
       <c r="J251" s="10"/>
       <c r="K251" s="10" t="s">
-        <v>295</v>
+        <v>578</v>
       </c>
       <c r="L251" s="10" t="s">
-        <v>296</v>
+        <v>579</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
@@ -11456,7 +11474,7 @@
         <v>8</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>824</v>
+        <v>294</v>
       </c>
       <c r="C252" s="9" t="s">
         <v>816</v>
@@ -11465,22 +11483,22 @@
         <v>806</v>
       </c>
       <c r="E252" s="12">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F252" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G252" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H252" s="10"/>
       <c r="I252" s="10"/>
       <c r="J252" s="10"/>
       <c r="K252" s="10" t="s">
-        <v>825</v>
+        <v>295</v>
       </c>
       <c r="L252" s="10" t="s">
-        <v>825</v>
+        <v>296</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
@@ -11488,7 +11506,7 @@
         <v>8</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>573</v>
+        <v>824</v>
       </c>
       <c r="C253" s="9" t="s">
         <v>816</v>
@@ -11500,7 +11518,7 @@
         <v>0</v>
       </c>
       <c r="F253" s="11" t="s">
-        <v>574</v>
+        <v>21</v>
       </c>
       <c r="G253" s="11" t="b">
         <v>0</v>
@@ -11509,42 +11527,42 @@
       <c r="I253" s="10"/>
       <c r="J253" s="10"/>
       <c r="K253" s="10" t="s">
-        <v>575</v>
+        <v>825</v>
       </c>
       <c r="L253" s="10" t="s">
-        <v>576</v>
+        <v>825</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>19</v>
+        <v>573</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D254" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E254" s="12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F254" s="11" t="s">
-        <v>56</v>
+        <v>574</v>
       </c>
       <c r="G254" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H254" s="10"/>
       <c r="I254" s="10"/>
       <c r="J254" s="10"/>
       <c r="K254" s="10" t="s">
-        <v>138</v>
+        <v>575</v>
       </c>
       <c r="L254" s="10" t="s">
-        <v>110</v>
+        <v>576</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">
@@ -11552,7 +11570,7 @@
         <v>4</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C255" s="9" t="s">
         <v>815</v>
@@ -11561,7 +11579,7 @@
         <v>806</v>
       </c>
       <c r="E255" s="12">
-        <v>-180</v>
+        <v>180</v>
       </c>
       <c r="F255" s="11" t="s">
         <v>56</v>
@@ -11573,10 +11591,10 @@
       <c r="I255" s="10"/>
       <c r="J255" s="10"/>
       <c r="K255" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L255" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
@@ -11584,7 +11602,7 @@
         <v>4</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C256" s="9" t="s">
         <v>815</v>
@@ -11593,10 +11611,10 @@
         <v>806</v>
       </c>
       <c r="E256" s="12">
-        <v>2</v>
+        <v>-180</v>
       </c>
       <c r="F256" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G256" s="11" t="b">
         <v>1</v>
@@ -11604,11 +11622,11 @@
       <c r="H256" s="10"/>
       <c r="I256" s="10"/>
       <c r="J256" s="10"/>
-      <c r="K256" s="9" t="s">
-        <v>127</v>
+      <c r="K256" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="L256" s="10" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
@@ -11616,31 +11634,31 @@
         <v>4</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>545</v>
+        <v>99</v>
       </c>
       <c r="C257" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E257" s="12" t="s">
-        <v>546</v>
+        <v>806</v>
+      </c>
+      <c r="E257" s="12">
+        <v>2</v>
       </c>
       <c r="F257" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G257" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H257" s="10"/>
       <c r="I257" s="10"/>
       <c r="J257" s="10"/>
-      <c r="K257" s="10" t="s">
-        <v>547</v>
+      <c r="K257" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="L257" s="10" t="s">
-        <v>547</v>
+        <v>213</v>
       </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
@@ -11648,7 +11666,7 @@
         <v>4</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>104</v>
+        <v>545</v>
       </c>
       <c r="C258" s="9" t="s">
         <v>815</v>
@@ -11656,27 +11674,23 @@
       <c r="D258" s="9" t="s">
         <v>805</v>
       </c>
-      <c r="E258" s="12">
-        <v>5</v>
+      <c r="E258" s="12" t="s">
+        <v>546</v>
       </c>
       <c r="F258" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G258" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H258" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I258" s="10" t="s">
-        <v>556</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H258" s="10"/>
+      <c r="I258" s="10"/>
       <c r="J258" s="10"/>
-      <c r="K258" s="9" t="s">
-        <v>135</v>
+      <c r="K258" s="10" t="s">
+        <v>547</v>
       </c>
       <c r="L258" s="10" t="s">
-        <v>105</v>
+        <v>547</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
@@ -11684,16 +11698,16 @@
         <v>4</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
       <c r="C259" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E259" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F259" s="11" t="s">
         <v>21</v>
@@ -11701,14 +11715,18 @@
       <c r="G259" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H259" s="10"/>
-      <c r="I259" s="10"/>
+      <c r="H259" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I259" s="10" t="s">
+        <v>556</v>
+      </c>
       <c r="J259" s="10"/>
-      <c r="K259" s="10" t="s">
-        <v>193</v>
+      <c r="K259" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="L259" s="10" t="s">
-        <v>194</v>
+        <v>105</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
@@ -11716,7 +11734,7 @@
         <v>4</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>582</v>
+        <v>192</v>
       </c>
       <c r="C260" s="9" t="s">
         <v>815</v>
@@ -11725,7 +11743,7 @@
         <v>804</v>
       </c>
       <c r="E260" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F260" s="11" t="s">
         <v>21</v>
@@ -11737,10 +11755,10 @@
       <c r="I260" s="10"/>
       <c r="J260" s="10"/>
       <c r="K260" s="10" t="s">
-        <v>583</v>
+        <v>193</v>
       </c>
       <c r="L260" s="10" t="s">
-        <v>584</v>
+        <v>194</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
@@ -11748,19 +11766,19 @@
         <v>4</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>188</v>
+        <v>582</v>
       </c>
       <c r="C261" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D261" s="9" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E261" s="12">
-        <v>950</v>
+        <v>2</v>
       </c>
       <c r="F261" s="11" t="s">
-        <v>189</v>
+        <v>21</v>
       </c>
       <c r="G261" s="11" t="b">
         <v>1</v>
@@ -11769,10 +11787,10 @@
       <c r="I261" s="10"/>
       <c r="J261" s="10"/>
       <c r="K261" s="10" t="s">
-        <v>190</v>
+        <v>583</v>
       </c>
       <c r="L261" s="10" t="s">
-        <v>191</v>
+        <v>584</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
@@ -11780,35 +11798,31 @@
         <v>4</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>521</v>
+        <v>188</v>
       </c>
       <c r="C262" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D262" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E262" s="12">
-        <v>7</v>
+        <v>950</v>
       </c>
       <c r="F262" s="11" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="G262" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H262" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I262" s="10" t="s">
-        <v>523</v>
-      </c>
+      <c r="H262" s="10"/>
+      <c r="I262" s="10"/>
       <c r="J262" s="10"/>
       <c r="K262" s="10" t="s">
-        <v>555</v>
+        <v>190</v>
       </c>
       <c r="L262" s="10" t="s">
-        <v>522</v>
+        <v>191</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
@@ -11816,16 +11830,16 @@
         <v>4</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>891</v>
+        <v>521</v>
       </c>
       <c r="C263" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E263" s="12" t="b">
-        <v>0</v>
+        <v>805</v>
+      </c>
+      <c r="E263" s="12">
+        <v>7</v>
       </c>
       <c r="F263" s="11" t="s">
         <v>21</v>
@@ -11834,15 +11848,17 @@
         <v>1</v>
       </c>
       <c r="H263" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="I263" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="I263" s="10" t="s">
+        <v>523</v>
+      </c>
       <c r="J263" s="10"/>
       <c r="K263" s="10" t="s">
-        <v>892</v>
+        <v>555</v>
       </c>
       <c r="L263" s="10" t="s">
-        <v>893</v>
+        <v>522</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
@@ -11850,7 +11866,7 @@
         <v>4</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>636</v>
+        <v>891</v>
       </c>
       <c r="C264" s="9" t="s">
         <v>815</v>
@@ -11859,13 +11875,13 @@
         <v>807</v>
       </c>
       <c r="E264" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F264" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G264" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H264" s="10" t="s">
         <v>202</v>
@@ -11873,10 +11889,10 @@
       <c r="I264" s="10"/>
       <c r="J264" s="10"/>
       <c r="K264" s="10" t="s">
-        <v>637</v>
+        <v>892</v>
       </c>
       <c r="L264" s="10" t="s">
-        <v>638</v>
+        <v>893</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
@@ -11884,7 +11900,7 @@
         <v>4</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>612</v>
+        <v>636</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>815</v>
@@ -11893,13 +11909,13 @@
         <v>807</v>
       </c>
       <c r="E265" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F265" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G265" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H265" s="10" t="s">
         <v>202</v>
@@ -11907,10 +11923,10 @@
       <c r="I265" s="10"/>
       <c r="J265" s="10"/>
       <c r="K265" s="10" t="s">
-        <v>610</v>
+        <v>637</v>
       </c>
       <c r="L265" s="10" t="s">
-        <v>611</v>
+        <v>638</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
@@ -11918,7 +11934,7 @@
         <v>4</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>209</v>
+        <v>612</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>815</v>
@@ -11927,13 +11943,13 @@
         <v>807</v>
       </c>
       <c r="E266" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F266" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G266" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H266" s="10" t="s">
         <v>202</v>
@@ -11941,10 +11957,10 @@
       <c r="I266" s="10"/>
       <c r="J266" s="10"/>
       <c r="K266" s="10" t="s">
-        <v>210</v>
+        <v>610</v>
       </c>
       <c r="L266" s="10" t="s">
-        <v>211</v>
+        <v>611</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
@@ -11952,27 +11968,33 @@
         <v>4</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>387</v>
+        <v>209</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E267" s="12"/>
-      <c r="F267" s="11"/>
+        <v>807</v>
+      </c>
+      <c r="E267" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F267" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G267" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H267" s="10"/>
+      <c r="H267" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I267" s="10"/>
       <c r="J267" s="10"/>
       <c r="K267" s="10" t="s">
-        <v>388</v>
+        <v>210</v>
       </c>
       <c r="L267" s="10" t="s">
-        <v>388</v>
+        <v>211</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
@@ -11980,35 +12002,33 @@
         <v>4</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>6</v>
+        <v>910</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E268" s="12">
+        <v>807</v>
+      </c>
+      <c r="E268" s="12" t="b">
         <v>0</v>
       </c>
       <c r="F268" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G268" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H268" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I268" s="10" t="s">
-        <v>132</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="I268" s="10"/>
       <c r="J268" s="10"/>
-      <c r="K268" s="9" t="s">
-        <v>133</v>
+      <c r="K268" s="10" t="s">
+        <v>911</v>
       </c>
       <c r="L268" s="10" t="s">
-        <v>65</v>
+        <v>912</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
@@ -12016,31 +12036,27 @@
         <v>4</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>623</v>
+        <v>387</v>
       </c>
       <c r="C269" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E269" s="12">
-        <v>1</v>
-      </c>
-      <c r="F269" s="11" t="s">
-        <v>625</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="E269" s="12"/>
+      <c r="F269" s="11"/>
       <c r="G269" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H269" s="10"/>
       <c r="I269" s="10"/>
       <c r="J269" s="10"/>
       <c r="K269" s="10" t="s">
-        <v>627</v>
+        <v>388</v>
       </c>
       <c r="L269" s="10" t="s">
-        <v>632</v>
+        <v>388</v>
       </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
@@ -12048,31 +12064,35 @@
         <v>4</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>621</v>
+        <v>6</v>
       </c>
       <c r="C270" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E270" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F270" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G270" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H270" s="10"/>
-      <c r="I270" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H270" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I270" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="J270" s="10"/>
-      <c r="K270" s="10" t="s">
-        <v>626</v>
+      <c r="K270" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="L270" s="10" t="s">
-        <v>631</v>
+        <v>65</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
@@ -12080,7 +12100,7 @@
         <v>4</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C271" s="9" t="s">
         <v>815</v>
@@ -12089,7 +12109,7 @@
         <v>806</v>
       </c>
       <c r="E271" s="12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F271" s="11" t="s">
         <v>625</v>
@@ -12101,10 +12121,10 @@
       <c r="I271" s="10"/>
       <c r="J271" s="10"/>
       <c r="K271" s="10" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L271" s="10" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
@@ -12112,7 +12132,7 @@
         <v>4</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C272" s="9" t="s">
         <v>815</v>
@@ -12121,7 +12141,7 @@
         <v>806</v>
       </c>
       <c r="E272" s="12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F272" s="11" t="s">
         <v>625</v>
@@ -12133,10 +12153,10 @@
       <c r="I272" s="10"/>
       <c r="J272" s="10"/>
       <c r="K272" s="10" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="L272" s="10" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
@@ -12144,7 +12164,7 @@
         <v>4</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>613</v>
+        <v>624</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>815</v>
@@ -12153,10 +12173,10 @@
         <v>806</v>
       </c>
       <c r="E273" s="12">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F273" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G273" s="11" t="b">
         <v>1</v>
@@ -12165,10 +12185,10 @@
       <c r="I273" s="10"/>
       <c r="J273" s="10"/>
       <c r="K273" s="10" t="s">
-        <v>614</v>
+        <v>629</v>
       </c>
       <c r="L273" s="10" t="s">
-        <v>615</v>
+        <v>634</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
@@ -12176,7 +12196,7 @@
         <v>4</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>5</v>
+        <v>622</v>
       </c>
       <c r="C274" s="9" t="s">
         <v>815</v>
@@ -12185,10 +12205,10 @@
         <v>806</v>
       </c>
       <c r="E274" s="12">
-        <v>670</v>
+        <v>0.1</v>
       </c>
       <c r="F274" s="11" t="s">
-        <v>212</v>
+        <v>625</v>
       </c>
       <c r="G274" s="11" t="b">
         <v>1</v>
@@ -12196,11 +12216,11 @@
       <c r="H274" s="10"/>
       <c r="I274" s="10"/>
       <c r="J274" s="10"/>
-      <c r="K274" s="9" t="s">
-        <v>126</v>
+      <c r="K274" s="10" t="s">
+        <v>628</v>
       </c>
       <c r="L274" s="10" t="s">
-        <v>64</v>
+        <v>633</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">
@@ -12208,16 +12228,16 @@
         <v>4</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>100</v>
+        <v>613</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E275" s="12">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F275" s="11" t="s">
         <v>21</v>
@@ -12225,18 +12245,14 @@
       <c r="G275" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H275" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I275" s="10" t="s">
-        <v>786</v>
-      </c>
+      <c r="H275" s="10"/>
+      <c r="I275" s="10"/>
       <c r="J275" s="10"/>
-      <c r="K275" s="9" t="s">
-        <v>134</v>
+      <c r="K275" s="10" t="s">
+        <v>614</v>
       </c>
       <c r="L275" s="10" t="s">
-        <v>101</v>
+        <v>615</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
@@ -12244,7 +12260,7 @@
         <v>4</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>531</v>
+        <v>5</v>
       </c>
       <c r="C276" s="9" t="s">
         <v>815</v>
@@ -12253,10 +12269,10 @@
         <v>806</v>
       </c>
       <c r="E276" s="12">
-        <v>1.1000000000000001</v>
+        <v>670</v>
       </c>
       <c r="F276" s="11" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="G276" s="11" t="b">
         <v>1</v>
@@ -12264,11 +12280,11 @@
       <c r="H276" s="10"/>
       <c r="I276" s="10"/>
       <c r="J276" s="10"/>
-      <c r="K276" s="10" t="s">
-        <v>535</v>
+      <c r="K276" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="L276" s="10" t="s">
-        <v>538</v>
+        <v>64</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
@@ -12276,16 +12292,16 @@
         <v>4</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>532</v>
+        <v>100</v>
       </c>
       <c r="C277" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E277" s="12">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F277" s="11" t="s">
         <v>21</v>
@@ -12293,14 +12309,18 @@
       <c r="G277" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H277" s="10"/>
-      <c r="I277" s="10"/>
+      <c r="H277" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I277" s="10" t="s">
+        <v>786</v>
+      </c>
       <c r="J277" s="10"/>
-      <c r="K277" s="10" t="s">
-        <v>536</v>
+      <c r="K277" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="L277" s="10" t="s">
-        <v>539</v>
+        <v>101</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
@@ -12308,7 +12328,7 @@
         <v>4</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>14</v>
+        <v>531</v>
       </c>
       <c r="C278" s="9" t="s">
         <v>815</v>
@@ -12317,22 +12337,22 @@
         <v>806</v>
       </c>
       <c r="E278" s="12">
-        <v>195</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F278" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G278" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H278" s="10"/>
       <c r="I278" s="10"/>
       <c r="J278" s="10"/>
-      <c r="K278" s="9" t="s">
-        <v>137</v>
+      <c r="K278" s="10" t="s">
+        <v>535</v>
       </c>
       <c r="L278" s="10" t="s">
-        <v>68</v>
+        <v>538</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
@@ -12340,7 +12360,7 @@
         <v>4</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>13</v>
+        <v>532</v>
       </c>
       <c r="C279" s="9" t="s">
         <v>815</v>
@@ -12349,22 +12369,22 @@
         <v>806</v>
       </c>
       <c r="E279" s="12">
-        <v>16</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F279" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G279" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H279" s="10"/>
       <c r="I279" s="10"/>
       <c r="J279" s="10"/>
-      <c r="K279" s="9" t="s">
-        <v>136</v>
+      <c r="K279" s="10" t="s">
+        <v>536</v>
       </c>
       <c r="L279" s="10" t="s">
-        <v>67</v>
+        <v>539</v>
       </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.25">
@@ -12372,7 +12392,7 @@
         <v>4</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>894</v>
+        <v>14</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>815</v>
@@ -12381,22 +12401,22 @@
         <v>806</v>
       </c>
       <c r="E280" s="12">
-        <v>0.5</v>
+        <v>195</v>
       </c>
       <c r="F280" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G280" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H280" s="10"/>
       <c r="I280" s="10"/>
       <c r="J280" s="10"/>
-      <c r="K280" s="10" t="s">
-        <v>895</v>
+      <c r="K280" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="L280" s="10" t="s">
-        <v>895</v>
+        <v>68</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">
@@ -12404,7 +12424,7 @@
         <v>4</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C281" s="9" t="s">
         <v>815</v>
@@ -12413,22 +12433,22 @@
         <v>806</v>
       </c>
       <c r="E281" s="12">
-        <v>1.33</v>
+        <v>16</v>
       </c>
       <c r="F281" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G281" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H281" s="10"/>
       <c r="I281" s="10"/>
       <c r="J281" s="10"/>
       <c r="K281" s="9" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="L281" s="10" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.25">
@@ -12436,7 +12456,7 @@
         <v>4</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>854</v>
+        <v>894</v>
       </c>
       <c r="C282" s="9" t="s">
         <v>815</v>
@@ -12445,10 +12465,10 @@
         <v>806</v>
       </c>
       <c r="E282" s="12">
-        <v>180</v>
+        <v>0.5</v>
       </c>
       <c r="F282" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G282" s="11" t="b">
         <v>1</v>
@@ -12457,10 +12477,10 @@
       <c r="I282" s="10"/>
       <c r="J282" s="10"/>
       <c r="K282" s="10" t="s">
-        <v>857</v>
+        <v>895</v>
       </c>
       <c r="L282" s="10" t="s">
-        <v>500</v>
+        <v>895</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.25">
@@ -12468,7 +12488,7 @@
         <v>4</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>855</v>
+        <v>97</v>
       </c>
       <c r="C283" s="9" t="s">
         <v>815</v>
@@ -12477,10 +12497,10 @@
         <v>806</v>
       </c>
       <c r="E283" s="12">
-        <v>85</v>
+        <v>1.33</v>
       </c>
       <c r="F283" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G283" s="11" t="b">
         <v>1</v>
@@ -12488,11 +12508,11 @@
       <c r="H283" s="10"/>
       <c r="I283" s="10"/>
       <c r="J283" s="10"/>
-      <c r="K283" s="10" t="s">
-        <v>858</v>
+      <c r="K283" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="L283" s="10" t="s">
-        <v>501</v>
+        <v>98</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.25">
@@ -12500,35 +12520,31 @@
         <v>4</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>497</v>
+        <v>854</v>
       </c>
       <c r="C284" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D284" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E284" s="12">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F284" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G284" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H284" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I284" s="10" t="s">
-        <v>520</v>
-      </c>
+      <c r="H284" s="10"/>
+      <c r="I284" s="10"/>
       <c r="J284" s="10"/>
       <c r="K284" s="10" t="s">
-        <v>498</v>
+        <v>857</v>
       </c>
       <c r="L284" s="10" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.25">
@@ -12536,33 +12552,31 @@
         <v>4</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>774</v>
+        <v>855</v>
       </c>
       <c r="C285" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D285" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E285" s="12">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F285" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G285" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H285" s="10" t="s">
-        <v>131</v>
-      </c>
+      <c r="H285" s="10"/>
       <c r="I285" s="10"/>
       <c r="J285" s="10"/>
       <c r="K285" s="10" t="s">
-        <v>775</v>
+        <v>858</v>
       </c>
       <c r="L285" s="10" t="s">
-        <v>776</v>
+        <v>501</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
@@ -12570,7 +12584,7 @@
         <v>4</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>269</v>
+        <v>497</v>
       </c>
       <c r="C286" s="9" t="s">
         <v>815</v>
@@ -12581,7 +12595,9 @@
       <c r="E286" s="12">
         <v>0</v>
       </c>
-      <c r="F286" s="11"/>
+      <c r="F286" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G286" s="11" t="b">
         <v>1</v>
       </c>
@@ -12589,14 +12605,14 @@
         <v>131</v>
       </c>
       <c r="I286" s="10" t="s">
-        <v>271</v>
+        <v>520</v>
       </c>
       <c r="J286" s="10"/>
       <c r="K286" s="10" t="s">
-        <v>270</v>
+        <v>498</v>
       </c>
       <c r="L286" s="10" t="s">
-        <v>284</v>
+        <v>499</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
@@ -12604,31 +12620,33 @@
         <v>4</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>9</v>
+        <v>774</v>
       </c>
       <c r="C287" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E287" s="12">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="F287" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G287" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H287" s="10"/>
+      <c r="H287" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="I287" s="10"/>
       <c r="J287" s="10"/>
-      <c r="K287" s="9" t="s">
-        <v>285</v>
+      <c r="K287" s="10" t="s">
+        <v>775</v>
       </c>
       <c r="L287" s="10" t="s">
-        <v>286</v>
+        <v>776</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
@@ -12636,31 +12654,33 @@
         <v>4</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>787</v>
+        <v>269</v>
       </c>
       <c r="C288" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D288" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E288" s="12">
-        <v>1</v>
-      </c>
-      <c r="F288" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F288" s="11"/>
       <c r="G288" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H288" s="10"/>
-      <c r="I288" s="10"/>
+      <c r="H288" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I288" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="J288" s="10"/>
       <c r="K288" s="10" t="s">
-        <v>788</v>
+        <v>270</v>
       </c>
       <c r="L288" s="10" t="s">
-        <v>789</v>
+        <v>284</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -12668,33 +12688,31 @@
         <v>4</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>533</v>
+        <v>9</v>
       </c>
       <c r="C289" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D289" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E289" s="12">
-        <v>0</v>
-      </c>
-      <c r="F289" s="11"/>
+        <v>195</v>
+      </c>
+      <c r="F289" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G289" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H289" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I289" s="10" t="s">
-        <v>534</v>
-      </c>
+      <c r="H289" s="10"/>
+      <c r="I289" s="10"/>
       <c r="J289" s="10"/>
-      <c r="K289" s="10" t="s">
-        <v>537</v>
+      <c r="K289" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="L289" s="10" t="s">
-        <v>540</v>
+        <v>286</v>
       </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
@@ -12702,7 +12720,7 @@
         <v>4</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>541</v>
+        <v>787</v>
       </c>
       <c r="C290" s="9" t="s">
         <v>815</v>
@@ -12723,10 +12741,10 @@
       <c r="I290" s="10"/>
       <c r="J290" s="10"/>
       <c r="K290" s="10" t="s">
-        <v>542</v>
+        <v>788</v>
       </c>
       <c r="L290" s="10" t="s">
-        <v>543</v>
+        <v>789</v>
       </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
@@ -12734,31 +12752,33 @@
         <v>4</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>620</v>
+        <v>533</v>
       </c>
       <c r="C291" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E291" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="F291" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F291" s="11"/>
       <c r="G291" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H291" s="10"/>
-      <c r="I291" s="10"/>
+      <c r="H291" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I291" s="10" t="s">
+        <v>534</v>
+      </c>
       <c r="J291" s="10"/>
       <c r="K291" s="10" t="s">
-        <v>630</v>
+        <v>537</v>
       </c>
       <c r="L291" s="10" t="s">
-        <v>635</v>
+        <v>540</v>
       </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
@@ -12766,7 +12786,7 @@
         <v>4</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>903</v>
+        <v>541</v>
       </c>
       <c r="C292" s="9" t="s">
         <v>815</v>
@@ -12775,10 +12795,10 @@
         <v>806</v>
       </c>
       <c r="E292" s="12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F292" s="11" t="s">
-        <v>906</v>
+        <v>21</v>
       </c>
       <c r="G292" s="11" t="b">
         <v>1</v>
@@ -12787,10 +12807,10 @@
       <c r="I292" s="10"/>
       <c r="J292" s="10"/>
       <c r="K292" s="10" t="s">
-        <v>905</v>
+        <v>542</v>
       </c>
       <c r="L292" s="10" t="s">
-        <v>904</v>
+        <v>543</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
@@ -12798,31 +12818,31 @@
         <v>4</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>828</v>
+        <v>620</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D293" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E293" s="12">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F293" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G293" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H293" s="10"/>
       <c r="I293" s="10"/>
       <c r="J293" s="10"/>
       <c r="K293" s="10" t="s">
-        <v>831</v>
+        <v>630</v>
       </c>
       <c r="L293" s="10" t="s">
-        <v>832</v>
+        <v>635</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
@@ -12830,31 +12850,31 @@
         <v>4</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>827</v>
+        <v>903</v>
       </c>
       <c r="C294" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D294" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E294" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F294" s="11" t="s">
-        <v>308</v>
+        <v>906</v>
       </c>
       <c r="G294" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H294" s="10"/>
       <c r="I294" s="10"/>
       <c r="J294" s="10"/>
       <c r="K294" s="10" t="s">
-        <v>801</v>
+        <v>905</v>
       </c>
       <c r="L294" s="10" t="s">
-        <v>833</v>
+        <v>904</v>
       </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
@@ -12862,17 +12882,19 @@
         <v>4</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>389</v>
+        <v>828</v>
       </c>
       <c r="C295" s="9" t="s">
         <v>816</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>813</v>
-      </c>
-      <c r="E295" s="12"/>
+        <v>806</v>
+      </c>
+      <c r="E295" s="12">
+        <v>0</v>
+      </c>
       <c r="F295" s="11" t="s">
-        <v>21</v>
+        <v>308</v>
       </c>
       <c r="G295" s="11" t="b">
         <v>0</v>
@@ -12881,10 +12903,10 @@
       <c r="I295" s="10"/>
       <c r="J295" s="10"/>
       <c r="K295" s="10" t="s">
-        <v>390</v>
+        <v>831</v>
       </c>
       <c r="L295" s="10" t="s">
-        <v>390</v>
+        <v>832</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
@@ -12892,7 +12914,7 @@
         <v>4</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>856</v>
+        <v>827</v>
       </c>
       <c r="C296" s="9" t="s">
         <v>816</v>
@@ -12904,7 +12926,7 @@
         <v>0</v>
       </c>
       <c r="F296" s="11" t="s">
-        <v>56</v>
+        <v>308</v>
       </c>
       <c r="G296" s="11" t="b">
         <v>0</v>
@@ -12913,10 +12935,10 @@
       <c r="I296" s="10"/>
       <c r="J296" s="10"/>
       <c r="K296" s="10" t="s">
-        <v>859</v>
+        <v>801</v>
       </c>
       <c r="L296" s="10" t="s">
-        <v>859</v>
+        <v>833</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.25">
@@ -12924,19 +12946,17 @@
         <v>4</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>861</v>
+        <v>389</v>
       </c>
       <c r="C297" s="9" t="s">
         <v>816</v>
       </c>
       <c r="D297" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E297" s="12">
-        <v>0</v>
-      </c>
+        <v>813</v>
+      </c>
+      <c r="E297" s="12"/>
       <c r="F297" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G297" s="11" t="b">
         <v>0</v>
@@ -12945,9 +12965,73 @@
       <c r="I297" s="10"/>
       <c r="J297" s="10"/>
       <c r="K297" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="L297" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A298" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B298" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="C298" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D298" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E298" s="12">
+        <v>0</v>
+      </c>
+      <c r="F298" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G298" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H298" s="10"/>
+      <c r="I298" s="10"/>
+      <c r="J298" s="10"/>
+      <c r="K298" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="L298" s="10" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A299" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B299" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="C299" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D299" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E299" s="12">
+        <v>0</v>
+      </c>
+      <c r="F299" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G299" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H299" s="10"/>
+      <c r="I299" s="10"/>
+      <c r="J299" s="10"/>
+      <c r="K299" s="10" t="s">
         <v>860</v>
       </c>
-      <c r="L297" s="10" t="s">
+      <c r="L299" s="10" t="s">
         <v>860</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding parameters for multi-receiver optimization settings
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C5E650-6B7D-4199-9A48-FADCA6769DB7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545333F-24FD-4244-A031-09AAA7851C90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="926">
   <si>
     <t>String name</t>
   </si>
@@ -2754,6 +2754,45 @@
   </si>
   <si>
     <t>Enables the user to specify the fraction of power delivered from the heliostat to each receiver</t>
+  </si>
+  <si>
+    <t>q_rec_des</t>
+  </si>
+  <si>
+    <t>Design-point thermal power</t>
+  </si>
+  <si>
+    <t>Power produced by the receiver at design after thermal losses</t>
+  </si>
+  <si>
+    <t>rec_offset_reference</t>
+  </si>
+  <si>
+    <t>Receiver offset reference</t>
+  </si>
+  <si>
+    <t>Tower=0</t>
+  </si>
+  <si>
+    <t>Receiver offset is relative to the position of the selected item. Options include tower or other receivers.</t>
+  </si>
+  <si>
+    <t>multirec_opt_timeout</t>
+  </si>
+  <si>
+    <t>Multi-receiver optimization solver time</t>
+  </si>
+  <si>
+    <t>Maximum allowable solver time for multiple receiver heliostat position and aimpoint optimization</t>
+  </si>
+  <si>
+    <t>multirec_screen_mult</t>
+  </si>
+  <si>
+    <t>Multi-receiver heliostat screen fraction</t>
+  </si>
+  <si>
+    <t>The number of heliostats required to meet this value times the design power of each receiver are considered for layout</t>
   </si>
 </sst>
 </file>
@@ -2992,10 +3031,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L299" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L299" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:L309">
-    <sortCondition ref="A1:A309"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L303" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L303" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:L313">
+    <sortCondition ref="A1:A313"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain" dataDxfId="11"/>
@@ -3336,11 +3375,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L299"/>
+  <dimension ref="A1:L303"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A268" sqref="A268"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E202" sqref="E202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9584,17 +9623,19 @@
         <v>714</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>737</v>
+        <v>920</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>806</v>
       </c>
-      <c r="E194" s="12"/>
+      <c r="E194" s="12">
+        <v>60</v>
+      </c>
       <c r="F194" s="11" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="G194" s="11" t="b">
         <v>0</v>
@@ -9603,10 +9644,10 @@
       <c r="I194" s="10"/>
       <c r="J194" s="10"/>
       <c r="K194" s="10" t="s">
-        <v>738</v>
+        <v>921</v>
       </c>
       <c r="L194" s="10" t="s">
-        <v>738</v>
+        <v>922</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.25">
@@ -9614,15 +9655,17 @@
         <v>714</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>720</v>
+        <v>923</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>806</v>
       </c>
-      <c r="E195" s="12"/>
+      <c r="E195" s="12">
+        <v>1.25</v>
+      </c>
       <c r="F195" s="11" t="s">
         <v>21</v>
       </c>
@@ -9631,32 +9674,28 @@
       </c>
       <c r="H195" s="10"/>
       <c r="I195" s="10"/>
-      <c r="J195" s="10" t="s">
-        <v>640</v>
-      </c>
+      <c r="J195" s="10"/>
       <c r="K195" s="10" t="s">
-        <v>731</v>
+        <v>924</v>
       </c>
       <c r="L195" s="10" t="s">
-        <v>732</v>
+        <v>925</v>
       </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="9" t="s">
-        <v>503</v>
+        <v>714</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>545</v>
+        <v>737</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E196" s="12" t="s">
-        <v>553</v>
-      </c>
+        <v>806</v>
+      </c>
+      <c r="E196" s="12"/>
       <c r="F196" s="11" t="s">
         <v>21</v>
       </c>
@@ -9667,40 +9706,42 @@
       <c r="I196" s="10"/>
       <c r="J196" s="10"/>
       <c r="K196" s="10" t="s">
-        <v>547</v>
+        <v>738</v>
       </c>
       <c r="L196" s="10" t="s">
-        <v>547</v>
+        <v>738</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="9" t="s">
-        <v>503</v>
+        <v>714</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>504</v>
+        <v>720</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E197" s="12" t="s">
-        <v>876</v>
-      </c>
-      <c r="F197" s="11"/>
+        <v>806</v>
+      </c>
+      <c r="E197" s="12"/>
+      <c r="F197" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G197" s="11" t="b">
         <v>0</v>
       </c>
       <c r="H197" s="10"/>
       <c r="I197" s="10"/>
-      <c r="J197" s="10"/>
+      <c r="J197" s="10" t="s">
+        <v>640</v>
+      </c>
       <c r="K197" s="10" t="s">
-        <v>510</v>
+        <v>731</v>
       </c>
       <c r="L197" s="10" t="s">
-        <v>512</v>
+        <v>732</v>
       </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.25">
@@ -9708,7 +9749,7 @@
         <v>503</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>505</v>
+        <v>545</v>
       </c>
       <c r="C198" s="9" t="s">
         <v>815</v>
@@ -9717,9 +9758,11 @@
         <v>805</v>
       </c>
       <c r="E198" s="12" t="s">
-        <v>508</v>
-      </c>
-      <c r="F198" s="11"/>
+        <v>553</v>
+      </c>
+      <c r="F198" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G198" s="11" t="b">
         <v>0</v>
       </c>
@@ -9727,10 +9770,10 @@
       <c r="I198" s="10"/>
       <c r="J198" s="10"/>
       <c r="K198" s="10" t="s">
-        <v>511</v>
+        <v>547</v>
       </c>
       <c r="L198" s="10" t="s">
-        <v>513</v>
+        <v>547</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.25">
@@ -9738,7 +9781,7 @@
         <v>503</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>815</v>
@@ -9746,25 +9789,21 @@
       <c r="D199" s="9" t="s">
         <v>805</v>
       </c>
-      <c r="E199" s="12">
-        <v>0</v>
+      <c r="E199" s="12" t="s">
+        <v>876</v>
       </c>
       <c r="F199" s="11"/>
       <c r="G199" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H199" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I199" s="10" t="s">
-        <v>515</v>
-      </c>
+      <c r="H199" s="10"/>
+      <c r="I199" s="10"/>
       <c r="J199" s="10"/>
       <c r="K199" s="10" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="L199" s="10" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.25">
@@ -9772,31 +9811,29 @@
         <v>503</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C200" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E200" s="12" t="b">
-        <v>1</v>
+        <v>805</v>
+      </c>
+      <c r="E200" s="12" t="s">
+        <v>508</v>
       </c>
       <c r="F200" s="11"/>
       <c r="G200" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H200" s="10" t="s">
-        <v>202</v>
-      </c>
+      <c r="H200" s="10"/>
       <c r="I200" s="10"/>
       <c r="J200" s="10"/>
       <c r="K200" s="10" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="L200" s="10" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.25">
@@ -9804,33 +9841,33 @@
         <v>503</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>696</v>
+        <v>507</v>
       </c>
       <c r="C201" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E201" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F201" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="E201" s="12">
+        <v>0</v>
+      </c>
+      <c r="F201" s="11"/>
       <c r="G201" s="11" t="b">
         <v>0</v>
       </c>
       <c r="H201" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="I201" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="I201" s="10" t="s">
+        <v>515</v>
+      </c>
       <c r="J201" s="10"/>
       <c r="K201" s="10" t="s">
-        <v>697</v>
+        <v>516</v>
       </c>
       <c r="L201" s="10" t="s">
-        <v>697</v>
+        <v>517</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.25">
@@ -9838,7 +9875,7 @@
         <v>503</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>700</v>
+        <v>509</v>
       </c>
       <c r="C202" s="9" t="s">
         <v>815</v>
@@ -9847,11 +9884,9 @@
         <v>807</v>
       </c>
       <c r="E202" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F202" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F202" s="11"/>
       <c r="G202" s="11" t="b">
         <v>0</v>
       </c>
@@ -9861,10 +9896,10 @@
       <c r="I202" s="10"/>
       <c r="J202" s="10"/>
       <c r="K202" s="10" t="s">
-        <v>701</v>
+        <v>518</v>
       </c>
       <c r="L202" s="10" t="s">
-        <v>701</v>
+        <v>519</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.25">
@@ -9872,7 +9907,7 @@
         <v>503</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C203" s="9" t="s">
         <v>815</v>
@@ -9895,10 +9930,10 @@
       <c r="I203" s="10"/>
       <c r="J203" s="10"/>
       <c r="K203" s="10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="L203" s="10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.25">
@@ -9906,7 +9941,7 @@
         <v>503</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="C204" s="9" t="s">
         <v>815</v>
@@ -9929,10 +9964,10 @@
       <c r="I204" s="10"/>
       <c r="J204" s="10"/>
       <c r="K204" s="10" t="s">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="L204" s="10" t="s">
-        <v>652</v>
+        <v>701</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.25">
@@ -9940,7 +9975,7 @@
         <v>503</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>653</v>
+        <v>698</v>
       </c>
       <c r="C205" s="9" t="s">
         <v>815</v>
@@ -9963,10 +9998,10 @@
       <c r="I205" s="10"/>
       <c r="J205" s="10"/>
       <c r="K205" s="10" t="s">
-        <v>654</v>
+        <v>699</v>
       </c>
       <c r="L205" s="10" t="s">
-        <v>655</v>
+        <v>699</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.25">
@@ -9974,7 +10009,7 @@
         <v>503</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>881</v>
+        <v>650</v>
       </c>
       <c r="C206" s="9" t="s">
         <v>815</v>
@@ -9997,10 +10032,10 @@
       <c r="I206" s="10"/>
       <c r="J206" s="10"/>
       <c r="K206" s="10" t="s">
-        <v>886</v>
+        <v>651</v>
       </c>
       <c r="L206" s="10" t="s">
-        <v>697</v>
+        <v>652</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.25">
@@ -10008,7 +10043,7 @@
         <v>503</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>882</v>
+        <v>653</v>
       </c>
       <c r="C207" s="9" t="s">
         <v>815</v>
@@ -10031,10 +10066,10 @@
       <c r="I207" s="10"/>
       <c r="J207" s="10"/>
       <c r="K207" s="10" t="s">
-        <v>887</v>
+        <v>654</v>
       </c>
       <c r="L207" s="10" t="s">
-        <v>701</v>
+        <v>655</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.25">
@@ -10042,7 +10077,7 @@
         <v>503</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="C208" s="9" t="s">
         <v>815</v>
@@ -10065,10 +10100,10 @@
       <c r="I208" s="10"/>
       <c r="J208" s="10"/>
       <c r="K208" s="10" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L208" s="10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.25">
@@ -10076,7 +10111,7 @@
         <v>503</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>815</v>
@@ -10099,10 +10134,10 @@
       <c r="I209" s="10"/>
       <c r="J209" s="10"/>
       <c r="K209" s="10" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="L209" s="10" t="s">
-        <v>652</v>
+        <v>701</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.25">
@@ -10110,7 +10145,7 @@
         <v>503</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="C210" s="9" t="s">
         <v>815</v>
@@ -10133,10 +10168,10 @@
       <c r="I210" s="10"/>
       <c r="J210" s="10"/>
       <c r="K210" s="10" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="L210" s="10" t="s">
-        <v>655</v>
+        <v>699</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.25">
@@ -10144,27 +10179,33 @@
         <v>503</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>506</v>
+        <v>884</v>
       </c>
       <c r="C211" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E211" s="12"/>
-      <c r="F211" s="11"/>
+        <v>807</v>
+      </c>
+      <c r="E211" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F211" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G211" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H211" s="10"/>
+      <c r="H211" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I211" s="10"/>
       <c r="J211" s="10"/>
       <c r="K211" s="10" t="s">
-        <v>514</v>
+        <v>889</v>
       </c>
       <c r="L211" s="10" t="s">
-        <v>514</v>
+        <v>652</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.25">
@@ -10172,29 +10213,33 @@
         <v>503</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>559</v>
+        <v>885</v>
       </c>
       <c r="C212" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E212" s="12"/>
+        <v>807</v>
+      </c>
+      <c r="E212" s="12" t="b">
+        <v>0</v>
+      </c>
       <c r="F212" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G212" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H212" s="10"/>
+      <c r="H212" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I212" s="10"/>
       <c r="J212" s="10"/>
       <c r="K212" s="10" t="s">
-        <v>560</v>
+        <v>890</v>
       </c>
       <c r="L212" s="10" t="s">
-        <v>560</v>
+        <v>655</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.25">
@@ -10202,7 +10247,7 @@
         <v>503</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>873</v>
+        <v>506</v>
       </c>
       <c r="C213" s="9" t="s">
         <v>815</v>
@@ -10210,67 +10255,57 @@
       <c r="D213" s="9" t="s">
         <v>805</v>
       </c>
-      <c r="E213" s="12">
-        <v>0</v>
-      </c>
-      <c r="F213" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="E213" s="12"/>
+      <c r="F213" s="11"/>
       <c r="G213" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H213" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I213" s="10" t="s">
-        <v>874</v>
-      </c>
+      <c r="H213" s="10"/>
+      <c r="I213" s="10"/>
       <c r="J213" s="10"/>
       <c r="K213" s="10" t="s">
-        <v>875</v>
+        <v>514</v>
       </c>
       <c r="L213" s="10" t="s">
-        <v>875</v>
+        <v>514</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" s="9" t="s">
-        <v>8</v>
+        <v>503</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>287</v>
+        <v>559</v>
       </c>
       <c r="C214" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E214" s="12">
-        <v>0.94</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="E214" s="12"/>
       <c r="F214" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G214" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H214" s="10"/>
       <c r="I214" s="10"/>
       <c r="J214" s="10"/>
       <c r="K214" s="10" t="s">
-        <v>289</v>
+        <v>560</v>
       </c>
       <c r="L214" s="10" t="s">
-        <v>290</v>
+        <v>560</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" s="9" t="s">
-        <v>8</v>
+        <v>503</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>702</v>
+        <v>873</v>
       </c>
       <c r="C215" s="9" t="s">
         <v>815</v>
@@ -10285,20 +10320,20 @@
         <v>21</v>
       </c>
       <c r="G215" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H215" s="10" t="s">
         <v>131</v>
       </c>
       <c r="I215" s="10" t="s">
-        <v>413</v>
+        <v>874</v>
       </c>
       <c r="J215" s="10"/>
       <c r="K215" s="10" t="s">
-        <v>705</v>
+        <v>875</v>
       </c>
       <c r="L215" s="10" t="s">
-        <v>706</v>
+        <v>875</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.25">
@@ -10306,7 +10341,7 @@
         <v>8</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>703</v>
+        <v>287</v>
       </c>
       <c r="C216" s="9" t="s">
         <v>815</v>
@@ -10315,10 +10350,10 @@
         <v>806</v>
       </c>
       <c r="E216" s="12">
-        <v>180</v>
+        <v>0.94</v>
       </c>
       <c r="F216" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G216" s="11" t="b">
         <v>1</v>
@@ -10327,10 +10362,10 @@
       <c r="I216" s="10"/>
       <c r="J216" s="10"/>
       <c r="K216" s="10" t="s">
-        <v>707</v>
+        <v>289</v>
       </c>
       <c r="L216" s="10" t="s">
-        <v>708</v>
+        <v>290</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.25">
@@ -10338,31 +10373,35 @@
         <v>8</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C217" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E217" s="12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F217" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G217" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H217" s="10"/>
-      <c r="I217" s="10"/>
+      <c r="H217" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I217" s="10" t="s">
+        <v>413</v>
+      </c>
       <c r="J217" s="10"/>
       <c r="K217" s="10" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="L217" s="10" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.25">
@@ -10370,33 +10409,31 @@
         <v>8</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>412</v>
+        <v>703</v>
       </c>
       <c r="C218" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E218" s="12">
-        <v>0</v>
-      </c>
-      <c r="F218" s="11"/>
+        <v>180</v>
+      </c>
+      <c r="F218" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="G218" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H218" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I218" s="10" t="s">
-        <v>770</v>
-      </c>
+      <c r="H218" s="10"/>
+      <c r="I218" s="10"/>
       <c r="J218" s="10"/>
       <c r="K218" s="10" t="s">
-        <v>414</v>
+        <v>707</v>
       </c>
       <c r="L218" s="10" t="s">
-        <v>415</v>
+        <v>708</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.25">
@@ -10404,31 +10441,31 @@
         <v>8</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>835</v>
+        <v>704</v>
       </c>
       <c r="C219" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>836</v>
-      </c>
-      <c r="E219" s="14">
-        <v>0</v>
+        <v>806</v>
+      </c>
+      <c r="E219" s="12">
+        <v>180</v>
       </c>
       <c r="F219" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G219" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H219" s="10"/>
       <c r="I219" s="10"/>
       <c r="J219" s="10"/>
       <c r="K219" s="10" t="s">
-        <v>834</v>
+        <v>709</v>
       </c>
       <c r="L219" s="10" t="s">
-        <v>834</v>
+        <v>710</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
@@ -10436,7 +10473,7 @@
         <v>8</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>545</v>
+        <v>412</v>
       </c>
       <c r="C220" s="9" t="s">
         <v>815</v>
@@ -10444,23 +10481,25 @@
       <c r="D220" s="9" t="s">
         <v>805</v>
       </c>
-      <c r="E220" s="12" t="s">
-        <v>548</v>
-      </c>
-      <c r="F220" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="E220" s="12">
+        <v>0</v>
+      </c>
+      <c r="F220" s="11"/>
       <c r="G220" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H220" s="10"/>
-      <c r="I220" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="H220" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I220" s="10" t="s">
+        <v>770</v>
+      </c>
       <c r="J220" s="10"/>
       <c r="K220" s="10" t="s">
-        <v>547</v>
+        <v>414</v>
       </c>
       <c r="L220" s="10" t="s">
-        <v>547</v>
+        <v>415</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.25">
@@ -10468,18 +10507,20 @@
         <v>8</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>29</v>
+        <v>835</v>
       </c>
       <c r="C221" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E221" s="12">
-        <v>-1</v>
-      </c>
-      <c r="F221" s="11"/>
+        <v>836</v>
+      </c>
+      <c r="E221" s="14">
+        <v>0</v>
+      </c>
+      <c r="F221" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G221" s="11" t="b">
         <v>0</v>
       </c>
@@ -10487,10 +10528,10 @@
       <c r="I221" s="10"/>
       <c r="J221" s="10"/>
       <c r="K221" s="10" t="s">
-        <v>320</v>
+        <v>834</v>
       </c>
       <c r="L221" s="10" t="s">
-        <v>320</v>
+        <v>834</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.25">
@@ -10498,31 +10539,31 @@
         <v>8</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>711</v>
+        <v>545</v>
       </c>
       <c r="C222" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E222" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F222" s="11"/>
+        <v>805</v>
+      </c>
+      <c r="E222" s="12" t="s">
+        <v>548</v>
+      </c>
+      <c r="F222" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G222" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H222" s="10" t="s">
-        <v>202</v>
-      </c>
+      <c r="H222" s="10"/>
       <c r="I222" s="10"/>
       <c r="J222" s="10"/>
       <c r="K222" s="10" t="s">
-        <v>712</v>
+        <v>547</v>
       </c>
       <c r="L222" s="10" t="s">
-        <v>713</v>
+        <v>547</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.25">
@@ -10530,16 +10571,16 @@
         <v>8</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>319</v>
+        <v>29</v>
       </c>
       <c r="C223" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D223" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E223" s="12" t="b">
-        <v>1</v>
+        <v>804</v>
+      </c>
+      <c r="E223" s="12">
+        <v>-1</v>
       </c>
       <c r="F223" s="11"/>
       <c r="G223" s="11" t="b">
@@ -10549,10 +10590,10 @@
       <c r="I223" s="10"/>
       <c r="J223" s="10"/>
       <c r="K223" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L223" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.25">
@@ -10560,7 +10601,7 @@
         <v>8</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>406</v>
+        <v>711</v>
       </c>
       <c r="C224" s="9" t="s">
         <v>815</v>
@@ -10569,7 +10610,7 @@
         <v>807</v>
       </c>
       <c r="E224" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F224" s="11"/>
       <c r="G224" s="11" t="b">
@@ -10579,14 +10620,12 @@
         <v>202</v>
       </c>
       <c r="I224" s="10"/>
-      <c r="J224" s="10" t="s">
-        <v>640</v>
-      </c>
+      <c r="J224" s="10"/>
       <c r="K224" s="10" t="s">
-        <v>407</v>
+        <v>712</v>
       </c>
       <c r="L224" s="10" t="s">
-        <v>408</v>
+        <v>713</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.25">
@@ -10594,7 +10633,7 @@
         <v>8</v>
       </c>
       <c r="B225" s="9" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="C225" s="9" t="s">
         <v>815</v>
@@ -10603,24 +10642,20 @@
         <v>807</v>
       </c>
       <c r="E225" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F225" s="11"/>
       <c r="G225" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H225" s="10" t="s">
-        <v>202</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H225" s="10"/>
       <c r="I225" s="10"/>
-      <c r="J225" s="10" t="s">
-        <v>640</v>
-      </c>
+      <c r="J225" s="10"/>
       <c r="K225" s="10" t="s">
-        <v>410</v>
+        <v>321</v>
       </c>
       <c r="L225" s="10" t="s">
-        <v>411</v>
+        <v>321</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.25">
@@ -10628,33 +10663,33 @@
         <v>8</v>
       </c>
       <c r="B226" s="9" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C226" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E226" s="12">
-        <v>12</v>
-      </c>
-      <c r="F226" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>807</v>
+      </c>
+      <c r="E226" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F226" s="11"/>
       <c r="G226" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H226" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H226" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I226" s="10"/>
       <c r="J226" s="10" t="s">
         <v>640</v>
       </c>
       <c r="K226" s="10" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="L226" s="10" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.25">
@@ -10662,33 +10697,33 @@
         <v>8</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="C227" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D227" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E227" s="12">
-        <v>0</v>
-      </c>
-      <c r="F227" s="11" t="s">
-        <v>56</v>
-      </c>
+        <v>807</v>
+      </c>
+      <c r="E227" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F227" s="11"/>
       <c r="G227" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H227" s="10"/>
+      <c r="H227" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I227" s="10"/>
       <c r="J227" s="10" t="s">
         <v>640</v>
       </c>
       <c r="K227" s="10" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="L227" s="10" t="s">
-        <v>641</v>
+        <v>411</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.25">
@@ -10696,31 +10731,33 @@
         <v>8</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>288</v>
+        <v>403</v>
       </c>
       <c r="C228" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E228" s="12">
-        <v>1000</v>
+        <v>12</v>
       </c>
       <c r="F228" s="11" t="s">
-        <v>291</v>
+        <v>21</v>
       </c>
       <c r="G228" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H228" s="10"/>
       <c r="I228" s="10"/>
-      <c r="J228" s="10"/>
+      <c r="J228" s="10" t="s">
+        <v>640</v>
+      </c>
       <c r="K228" s="10" t="s">
-        <v>292</v>
+        <v>404</v>
       </c>
       <c r="L228" s="10" t="s">
-        <v>293</v>
+        <v>405</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.25">
@@ -10728,7 +10765,7 @@
         <v>8</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>907</v>
+        <v>427</v>
       </c>
       <c r="C229" s="9" t="s">
         <v>815</v>
@@ -10737,22 +10774,24 @@
         <v>806</v>
       </c>
       <c r="E229" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F229" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G229" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H229" s="10"/>
       <c r="I229" s="10"/>
-      <c r="J229" s="10"/>
+      <c r="J229" s="10" t="s">
+        <v>640</v>
+      </c>
       <c r="K229" s="10" t="s">
-        <v>908</v>
+        <v>428</v>
       </c>
       <c r="L229" s="10" t="s">
-        <v>909</v>
+        <v>641</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.25">
@@ -10760,7 +10799,7 @@
         <v>8</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="C230" s="9" t="s">
         <v>815</v>
@@ -10769,10 +10808,10 @@
         <v>806</v>
       </c>
       <c r="E230" s="12">
-        <v>10.199999999999999</v>
+        <v>1000</v>
       </c>
       <c r="F230" s="11" t="s">
-        <v>567</v>
+        <v>291</v>
       </c>
       <c r="G230" s="11" t="b">
         <v>1</v>
@@ -10781,10 +10820,10 @@
       <c r="I230" s="10"/>
       <c r="J230" s="10"/>
       <c r="K230" s="10" t="s">
-        <v>568</v>
+        <v>292</v>
       </c>
       <c r="L230" s="10" t="s">
-        <v>569</v>
+        <v>293</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.25">
@@ -10792,7 +10831,7 @@
         <v>8</v>
       </c>
       <c r="B231" s="9" t="s">
-        <v>570</v>
+        <v>907</v>
       </c>
       <c r="C231" s="9" t="s">
         <v>815</v>
@@ -10801,10 +10840,10 @@
         <v>806</v>
       </c>
       <c r="E231" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F231" s="11" t="s">
-        <v>558</v>
+        <v>21</v>
       </c>
       <c r="G231" s="11" t="b">
         <v>1</v>
@@ -10813,10 +10852,10 @@
       <c r="I231" s="10"/>
       <c r="J231" s="10"/>
       <c r="K231" s="10" t="s">
-        <v>571</v>
+        <v>908</v>
       </c>
       <c r="L231" s="10" t="s">
-        <v>572</v>
+        <v>909</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
@@ -10824,7 +10863,7 @@
         <v>8</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>15</v>
+        <v>307</v>
       </c>
       <c r="C232" s="9" t="s">
         <v>815</v>
@@ -10833,10 +10872,10 @@
         <v>806</v>
       </c>
       <c r="E232" s="12">
-        <v>0</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F232" s="11" t="s">
-        <v>56</v>
+        <v>567</v>
       </c>
       <c r="G232" s="11" t="b">
         <v>1</v>
@@ -10844,11 +10883,11 @@
       <c r="H232" s="10"/>
       <c r="I232" s="10"/>
       <c r="J232" s="10"/>
-      <c r="K232" s="9" t="s">
-        <v>145</v>
+      <c r="K232" s="10" t="s">
+        <v>568</v>
       </c>
       <c r="L232" s="10" t="s">
-        <v>422</v>
+        <v>569</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
@@ -10856,7 +10895,7 @@
         <v>8</v>
       </c>
       <c r="B233" s="9" t="s">
-        <v>298</v>
+        <v>570</v>
       </c>
       <c r="C233" s="9" t="s">
         <v>815</v>
@@ -10868,21 +10907,19 @@
         <v>0</v>
       </c>
       <c r="F233" s="11" t="s">
-        <v>23</v>
+        <v>558</v>
       </c>
       <c r="G233" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H233" s="10"/>
       <c r="I233" s="10"/>
-      <c r="J233" s="10" t="s">
-        <v>640</v>
-      </c>
+      <c r="J233" s="10"/>
       <c r="K233" s="10" t="s">
-        <v>300</v>
+        <v>571</v>
       </c>
       <c r="L233" s="10" t="s">
-        <v>301</v>
+        <v>572</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
@@ -10890,7 +10927,7 @@
         <v>8</v>
       </c>
       <c r="B234" s="9" t="s">
-        <v>297</v>
+        <v>15</v>
       </c>
       <c r="C234" s="9" t="s">
         <v>815</v>
@@ -10899,24 +10936,22 @@
         <v>806</v>
       </c>
       <c r="E234" s="12">
-        <v>7.75</v>
+        <v>0</v>
       </c>
       <c r="F234" s="11" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G234" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H234" s="10"/>
       <c r="I234" s="10"/>
-      <c r="J234" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="K234" s="10" t="s">
-        <v>299</v>
+      <c r="J234" s="10"/>
+      <c r="K234" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="L234" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
@@ -10924,7 +10959,7 @@
         <v>8</v>
       </c>
       <c r="B235" s="9" t="s">
-        <v>11</v>
+        <v>298</v>
       </c>
       <c r="C235" s="9" t="s">
         <v>815</v>
@@ -10933,7 +10968,7 @@
         <v>806</v>
       </c>
       <c r="E235" s="12">
-        <v>17.649999999999999</v>
+        <v>0</v>
       </c>
       <c r="F235" s="11" t="s">
         <v>23</v>
@@ -10943,12 +10978,14 @@
       </c>
       <c r="H235" s="10"/>
       <c r="I235" s="10"/>
-      <c r="J235" s="10"/>
-      <c r="K235" s="9" t="s">
-        <v>119</v>
+      <c r="J235" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K235" s="10" t="s">
+        <v>300</v>
       </c>
       <c r="L235" s="10" t="s">
-        <v>142</v>
+        <v>301</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
@@ -10956,7 +10993,7 @@
         <v>8</v>
       </c>
       <c r="B236" s="9" t="s">
-        <v>431</v>
+        <v>297</v>
       </c>
       <c r="C236" s="9" t="s">
         <v>815</v>
@@ -10965,22 +11002,24 @@
         <v>806</v>
       </c>
       <c r="E236" s="12">
-        <v>0</v>
+        <v>7.75</v>
       </c>
       <c r="F236" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G236" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H236" s="10"/>
       <c r="I236" s="10"/>
-      <c r="J236" s="10"/>
-      <c r="K236" s="9" t="s">
-        <v>429</v>
+      <c r="J236" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K236" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="L236" s="10" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
@@ -10988,7 +11027,7 @@
         <v>8</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C237" s="9" t="s">
         <v>815</v>
@@ -10997,7 +11036,7 @@
         <v>806</v>
       </c>
       <c r="E237" s="12">
-        <v>21.6</v>
+        <v>17.649999999999999</v>
       </c>
       <c r="F237" s="11" t="s">
         <v>23</v>
@@ -11009,10 +11048,10 @@
       <c r="I237" s="10"/>
       <c r="J237" s="10"/>
       <c r="K237" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L237" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.25">
@@ -11020,29 +11059,31 @@
         <v>8</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>313</v>
+        <v>431</v>
       </c>
       <c r="C238" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E238" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="F238" s="11"/>
+        <v>806</v>
+      </c>
+      <c r="E238" s="12">
+        <v>0</v>
+      </c>
+      <c r="F238" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="G238" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H238" s="10"/>
       <c r="I238" s="10"/>
       <c r="J238" s="10"/>
-      <c r="K238" s="10" t="s">
-        <v>315</v>
+      <c r="K238" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="L238" s="10" t="s">
-        <v>315</v>
+        <v>430</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
@@ -11050,7 +11091,7 @@
         <v>8</v>
       </c>
       <c r="B239" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C239" s="9" t="s">
         <v>815</v>
@@ -11059,7 +11100,7 @@
         <v>806</v>
       </c>
       <c r="E239" s="12">
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="F239" s="11" t="s">
         <v>23</v>
@@ -11071,10 +11112,10 @@
       <c r="I239" s="10"/>
       <c r="J239" s="10"/>
       <c r="K239" s="9" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="L239" s="10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
@@ -11082,31 +11123,29 @@
         <v>8</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>17</v>
+        <v>313</v>
       </c>
       <c r="C240" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E240" s="12">
-        <v>0</v>
-      </c>
-      <c r="F240" s="11" t="s">
-        <v>23</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="E240" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="F240" s="11"/>
       <c r="G240" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H240" s="10"/>
       <c r="I240" s="10"/>
       <c r="J240" s="10"/>
-      <c r="K240" s="9" t="s">
-        <v>147</v>
+      <c r="K240" s="10" t="s">
+        <v>315</v>
       </c>
       <c r="L240" s="10" t="s">
-        <v>149</v>
+        <v>315</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
@@ -11114,7 +11153,7 @@
         <v>8</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>302</v>
+        <v>16</v>
       </c>
       <c r="C241" s="9" t="s">
         <v>815</v>
@@ -11135,10 +11174,10 @@
       <c r="I241" s="10"/>
       <c r="J241" s="10"/>
       <c r="K241" s="9" t="s">
-        <v>303</v>
+        <v>146</v>
       </c>
       <c r="L241" s="10" t="s">
-        <v>426</v>
+        <v>148</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
@@ -11146,35 +11185,31 @@
         <v>8</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E242" s="12">
         <v>0</v>
       </c>
       <c r="F242" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G242" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H242" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I242" s="10" t="s">
-        <v>771</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H242" s="10"/>
+      <c r="I242" s="10"/>
       <c r="J242" s="10"/>
       <c r="K242" s="9" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="L242" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
@@ -11182,7 +11217,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>10</v>
+        <v>302</v>
       </c>
       <c r="C243" s="9" t="s">
         <v>815</v>
@@ -11191,7 +11226,7 @@
         <v>806</v>
       </c>
       <c r="E243" s="12">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F243" s="11" t="s">
         <v>23</v>
@@ -11203,10 +11238,10 @@
       <c r="I243" s="10"/>
       <c r="J243" s="10"/>
       <c r="K243" s="9" t="s">
-        <v>118</v>
+        <v>303</v>
       </c>
       <c r="L243" s="10" t="s">
-        <v>141</v>
+        <v>426</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
@@ -11214,33 +11249,35 @@
         <v>8</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>417</v>
+        <v>916</v>
       </c>
       <c r="C244" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E244" s="12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F244" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G244" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H244" s="10"/>
-      <c r="I244" s="10"/>
-      <c r="J244" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="K244" s="9" t="s">
-        <v>420</v>
+        <v>0</v>
+      </c>
+      <c r="H244" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I244" s="10" t="s">
+        <v>918</v>
+      </c>
+      <c r="J244" s="10"/>
+      <c r="K244" s="10" t="s">
+        <v>917</v>
       </c>
       <c r="L244" s="10" t="s">
-        <v>421</v>
+        <v>919</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
@@ -11248,33 +11285,35 @@
         <v>8</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>416</v>
+        <v>20</v>
       </c>
       <c r="C245" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E245" s="12">
-        <v>-180</v>
+        <v>0</v>
       </c>
       <c r="F245" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G245" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H245" s="10"/>
-      <c r="I245" s="10"/>
-      <c r="J245" s="10" t="s">
-        <v>640</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H245" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I245" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="J245" s="10"/>
       <c r="K245" s="9" t="s">
-        <v>418</v>
+        <v>24</v>
       </c>
       <c r="L245" s="10" t="s">
-        <v>419</v>
+        <v>150</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
@@ -11282,7 +11321,7 @@
         <v>8</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>561</v>
+        <v>10</v>
       </c>
       <c r="C246" s="9" t="s">
         <v>815</v>
@@ -11291,10 +11330,10 @@
         <v>806</v>
       </c>
       <c r="E246" s="12">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F246" s="11" t="s">
-        <v>291</v>
+        <v>23</v>
       </c>
       <c r="G246" s="11" t="b">
         <v>1</v>
@@ -11302,11 +11341,11 @@
       <c r="H246" s="10"/>
       <c r="I246" s="10"/>
       <c r="J246" s="10"/>
-      <c r="K246" s="10" t="s">
-        <v>562</v>
+      <c r="K246" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="L246" s="10" t="s">
-        <v>563</v>
+        <v>141</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
@@ -11314,31 +11353,33 @@
         <v>8</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>564</v>
+        <v>417</v>
       </c>
       <c r="C247" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D247" s="9" t="s">
-        <v>803</v>
-      </c>
-      <c r="E247" s="10" t="s">
-        <v>309</v>
+        <v>806</v>
+      </c>
+      <c r="E247" s="12">
+        <v>180</v>
       </c>
       <c r="F247" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G247" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H247" s="10"/>
       <c r="I247" s="10"/>
-      <c r="J247" s="10"/>
-      <c r="K247" s="10" t="s">
-        <v>565</v>
+      <c r="J247" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K247" s="9" t="s">
+        <v>420</v>
       </c>
       <c r="L247" s="10" t="s">
-        <v>305</v>
+        <v>421</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
@@ -11346,31 +11387,33 @@
         <v>8</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>304</v>
+        <v>416</v>
       </c>
       <c r="C248" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>803</v>
-      </c>
-      <c r="E248" s="10" t="s">
-        <v>309</v>
+        <v>806</v>
+      </c>
+      <c r="E248" s="12">
+        <v>-180</v>
       </c>
       <c r="F248" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G248" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H248" s="10"/>
       <c r="I248" s="10"/>
-      <c r="J248" s="10"/>
-      <c r="K248" s="10" t="s">
-        <v>566</v>
+      <c r="J248" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K248" s="9" t="s">
+        <v>418</v>
       </c>
       <c r="L248" s="10" t="s">
-        <v>306</v>
+        <v>419</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
@@ -11378,31 +11421,31 @@
         <v>8</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>310</v>
+        <v>561</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D249" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E249" s="12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F249" s="11" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="G249" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H249" s="10"/>
       <c r="I249" s="10"/>
       <c r="J249" s="10"/>
       <c r="K249" s="10" t="s">
-        <v>311</v>
+        <v>562</v>
       </c>
       <c r="L249" s="10" t="s">
-        <v>424</v>
+        <v>563</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
@@ -11410,19 +11453,19 @@
         <v>8</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>25</v>
+        <v>564</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E250" s="12">
-        <v>195</v>
+        <v>803</v>
+      </c>
+      <c r="E250" s="10" t="s">
+        <v>309</v>
       </c>
       <c r="F250" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G250" s="11" t="b">
         <v>0</v>
@@ -11430,11 +11473,11 @@
       <c r="H250" s="10"/>
       <c r="I250" s="10"/>
       <c r="J250" s="10"/>
-      <c r="K250" s="9" t="s">
-        <v>140</v>
+      <c r="K250" s="10" t="s">
+        <v>565</v>
       </c>
       <c r="L250" s="10" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
@@ -11442,19 +11485,19 @@
         <v>8</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>577</v>
+        <v>304</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E251" s="12">
-        <v>0</v>
+        <v>803</v>
+      </c>
+      <c r="E251" s="10" t="s">
+        <v>309</v>
       </c>
       <c r="F251" s="11" t="s">
-        <v>574</v>
+        <v>21</v>
       </c>
       <c r="G251" s="11" t="b">
         <v>0</v>
@@ -11463,10 +11506,10 @@
       <c r="I251" s="10"/>
       <c r="J251" s="10"/>
       <c r="K251" s="10" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="L251" s="10" t="s">
-        <v>579</v>
+        <v>306</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
@@ -11474,7 +11517,7 @@
         <v>8</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="C252" s="9" t="s">
         <v>816</v>
@@ -11483,22 +11526,22 @@
         <v>806</v>
       </c>
       <c r="E252" s="12">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="F252" s="11" t="s">
-        <v>21</v>
+        <v>308</v>
       </c>
       <c r="G252" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H252" s="10"/>
       <c r="I252" s="10"/>
       <c r="J252" s="10"/>
       <c r="K252" s="10" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="L252" s="10" t="s">
-        <v>296</v>
+        <v>424</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
@@ -11506,7 +11549,7 @@
         <v>8</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>824</v>
+        <v>25</v>
       </c>
       <c r="C253" s="9" t="s">
         <v>816</v>
@@ -11515,10 +11558,10 @@
         <v>806</v>
       </c>
       <c r="E253" s="12">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="F253" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G253" s="11" t="b">
         <v>0</v>
@@ -11526,11 +11569,11 @@
       <c r="H253" s="10"/>
       <c r="I253" s="10"/>
       <c r="J253" s="10"/>
-      <c r="K253" s="10" t="s">
-        <v>825</v>
+      <c r="K253" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="L253" s="10" t="s">
-        <v>825</v>
+        <v>425</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
@@ -11538,7 +11581,7 @@
         <v>8</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="C254" s="9" t="s">
         <v>816</v>
@@ -11559,30 +11602,30 @@
       <c r="I254" s="10"/>
       <c r="J254" s="10"/>
       <c r="K254" s="10" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="L254" s="10" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>19</v>
+        <v>294</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D255" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E255" s="12">
-        <v>180</v>
+        <v>1.2</v>
       </c>
       <c r="F255" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G255" s="11" t="b">
         <v>1</v>
@@ -11591,94 +11634,94 @@
       <c r="I255" s="10"/>
       <c r="J255" s="10"/>
       <c r="K255" s="10" t="s">
-        <v>138</v>
+        <v>295</v>
       </c>
       <c r="L255" s="10" t="s">
-        <v>110</v>
+        <v>296</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>18</v>
+        <v>824</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D256" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E256" s="12">
-        <v>-180</v>
+        <v>0</v>
       </c>
       <c r="F256" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G256" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H256" s="10"/>
       <c r="I256" s="10"/>
       <c r="J256" s="10"/>
       <c r="K256" s="10" t="s">
-        <v>139</v>
+        <v>825</v>
       </c>
       <c r="L256" s="10" t="s">
-        <v>111</v>
+        <v>825</v>
       </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>99</v>
+        <v>573</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E257" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F257" s="11" t="s">
-        <v>21</v>
+        <v>574</v>
       </c>
       <c r="G257" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H257" s="10"/>
       <c r="I257" s="10"/>
       <c r="J257" s="10"/>
-      <c r="K257" s="9" t="s">
-        <v>127</v>
+      <c r="K257" s="10" t="s">
+        <v>575</v>
       </c>
       <c r="L257" s="10" t="s">
-        <v>213</v>
+        <v>576</v>
       </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>545</v>
+        <v>913</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E258" s="12" t="s">
-        <v>546</v>
+        <v>806</v>
+      </c>
+      <c r="E258" s="12">
+        <v>0</v>
       </c>
       <c r="F258" s="11" t="s">
-        <v>21</v>
+        <v>574</v>
       </c>
       <c r="G258" s="11" t="b">
         <v>0</v>
@@ -11687,10 +11730,10 @@
       <c r="I258" s="10"/>
       <c r="J258" s="10"/>
       <c r="K258" s="10" t="s">
-        <v>547</v>
+        <v>914</v>
       </c>
       <c r="L258" s="10" t="s">
-        <v>547</v>
+        <v>915</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
@@ -11698,35 +11741,31 @@
         <v>4</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="C259" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E259" s="12">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="F259" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G259" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H259" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I259" s="10" t="s">
-        <v>556</v>
-      </c>
+      <c r="H259" s="10"/>
+      <c r="I259" s="10"/>
       <c r="J259" s="10"/>
-      <c r="K259" s="9" t="s">
-        <v>135</v>
+      <c r="K259" s="10" t="s">
+        <v>138</v>
       </c>
       <c r="L259" s="10" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
@@ -11734,19 +11773,19 @@
         <v>4</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>192</v>
+        <v>18</v>
       </c>
       <c r="C260" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="E260" s="12">
-        <v>4</v>
+        <v>-180</v>
       </c>
       <c r="F260" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G260" s="11" t="b">
         <v>1</v>
@@ -11755,10 +11794,10 @@
       <c r="I260" s="10"/>
       <c r="J260" s="10"/>
       <c r="K260" s="10" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
       <c r="L260" s="10" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
@@ -11766,13 +11805,13 @@
         <v>4</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>582</v>
+        <v>99</v>
       </c>
       <c r="C261" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D261" s="9" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="E261" s="12">
         <v>2</v>
@@ -11786,11 +11825,11 @@
       <c r="H261" s="10"/>
       <c r="I261" s="10"/>
       <c r="J261" s="10"/>
-      <c r="K261" s="10" t="s">
-        <v>583</v>
+      <c r="K261" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="L261" s="10" t="s">
-        <v>584</v>
+        <v>213</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
@@ -11798,31 +11837,31 @@
         <v>4</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>188</v>
+        <v>545</v>
       </c>
       <c r="C262" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D262" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E262" s="12">
-        <v>950</v>
+        <v>805</v>
+      </c>
+      <c r="E262" s="12" t="s">
+        <v>546</v>
       </c>
       <c r="F262" s="11" t="s">
-        <v>189</v>
+        <v>21</v>
       </c>
       <c r="G262" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H262" s="10"/>
       <c r="I262" s="10"/>
       <c r="J262" s="10"/>
       <c r="K262" s="10" t="s">
-        <v>190</v>
+        <v>547</v>
       </c>
       <c r="L262" s="10" t="s">
-        <v>191</v>
+        <v>547</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
@@ -11830,7 +11869,7 @@
         <v>4</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>521</v>
+        <v>104</v>
       </c>
       <c r="C263" s="9" t="s">
         <v>815</v>
@@ -11839,7 +11878,7 @@
         <v>805</v>
       </c>
       <c r="E263" s="12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F263" s="11" t="s">
         <v>21</v>
@@ -11851,14 +11890,14 @@
         <v>131</v>
       </c>
       <c r="I263" s="10" t="s">
-        <v>523</v>
+        <v>556</v>
       </c>
       <c r="J263" s="10"/>
-      <c r="K263" s="10" t="s">
-        <v>555</v>
+      <c r="K263" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="L263" s="10" t="s">
-        <v>522</v>
+        <v>105</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
@@ -11866,16 +11905,16 @@
         <v>4</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>891</v>
+        <v>192</v>
       </c>
       <c r="C264" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D264" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E264" s="12" t="b">
-        <v>0</v>
+        <v>804</v>
+      </c>
+      <c r="E264" s="12">
+        <v>4</v>
       </c>
       <c r="F264" s="11" t="s">
         <v>21</v>
@@ -11883,16 +11922,14 @@
       <c r="G264" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H264" s="10" t="s">
-        <v>202</v>
-      </c>
+      <c r="H264" s="10"/>
       <c r="I264" s="10"/>
       <c r="J264" s="10"/>
       <c r="K264" s="10" t="s">
-        <v>892</v>
+        <v>193</v>
       </c>
       <c r="L264" s="10" t="s">
-        <v>893</v>
+        <v>194</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
@@ -11900,33 +11937,31 @@
         <v>4</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>636</v>
+        <v>582</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D265" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E265" s="12" t="b">
-        <v>1</v>
+        <v>804</v>
+      </c>
+      <c r="E265" s="12">
+        <v>2</v>
       </c>
       <c r="F265" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G265" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H265" s="10" t="s">
-        <v>202</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H265" s="10"/>
       <c r="I265" s="10"/>
       <c r="J265" s="10"/>
       <c r="K265" s="10" t="s">
-        <v>637</v>
+        <v>583</v>
       </c>
       <c r="L265" s="10" t="s">
-        <v>638</v>
+        <v>584</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
@@ -11934,33 +11969,31 @@
         <v>4</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>612</v>
+        <v>188</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D266" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E266" s="12" t="b">
-        <v>0</v>
+        <v>806</v>
+      </c>
+      <c r="E266" s="12">
+        <v>950</v>
       </c>
       <c r="F266" s="11" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="G266" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H266" s="10" t="s">
-        <v>202</v>
-      </c>
+      <c r="H266" s="10"/>
       <c r="I266" s="10"/>
       <c r="J266" s="10"/>
       <c r="K266" s="10" t="s">
-        <v>610</v>
+        <v>190</v>
       </c>
       <c r="L266" s="10" t="s">
-        <v>611</v>
+        <v>191</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
@@ -11968,33 +12001,35 @@
         <v>4</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>209</v>
+        <v>521</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E267" s="12" t="b">
-        <v>1</v>
+        <v>805</v>
+      </c>
+      <c r="E267" s="12">
+        <v>7</v>
       </c>
       <c r="F267" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G267" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H267" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="I267" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="I267" s="10" t="s">
+        <v>523</v>
+      </c>
       <c r="J267" s="10"/>
       <c r="K267" s="10" t="s">
-        <v>210</v>
+        <v>555</v>
       </c>
       <c r="L267" s="10" t="s">
-        <v>211</v>
+        <v>522</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
@@ -12002,7 +12037,7 @@
         <v>4</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>910</v>
+        <v>891</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>815</v>
@@ -12025,10 +12060,10 @@
       <c r="I268" s="10"/>
       <c r="J268" s="10"/>
       <c r="K268" s="10" t="s">
-        <v>911</v>
+        <v>892</v>
       </c>
       <c r="L268" s="10" t="s">
-        <v>912</v>
+        <v>893</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
@@ -12036,27 +12071,33 @@
         <v>4</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>387</v>
+        <v>636</v>
       </c>
       <c r="C269" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E269" s="12"/>
-      <c r="F269" s="11"/>
+        <v>807</v>
+      </c>
+      <c r="E269" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F269" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G269" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H269" s="10"/>
+      <c r="H269" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I269" s="10"/>
       <c r="J269" s="10"/>
       <c r="K269" s="10" t="s">
-        <v>388</v>
+        <v>637</v>
       </c>
       <c r="L269" s="10" t="s">
-        <v>388</v>
+        <v>638</v>
       </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
@@ -12064,35 +12105,33 @@
         <v>4</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>6</v>
+        <v>612</v>
       </c>
       <c r="C270" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E270" s="12">
+        <v>807</v>
+      </c>
+      <c r="E270" s="12" t="b">
         <v>0</v>
       </c>
       <c r="F270" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G270" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H270" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I270" s="10" t="s">
-        <v>132</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="I270" s="10"/>
       <c r="J270" s="10"/>
-      <c r="K270" s="9" t="s">
-        <v>133</v>
+      <c r="K270" s="10" t="s">
+        <v>610</v>
       </c>
       <c r="L270" s="10" t="s">
-        <v>65</v>
+        <v>611</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
@@ -12100,31 +12139,33 @@
         <v>4</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>623</v>
+        <v>209</v>
       </c>
       <c r="C271" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E271" s="12">
+        <v>807</v>
+      </c>
+      <c r="E271" s="12" t="b">
         <v>1</v>
       </c>
       <c r="F271" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G271" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H271" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H271" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I271" s="10"/>
       <c r="J271" s="10"/>
       <c r="K271" s="10" t="s">
-        <v>627</v>
+        <v>210</v>
       </c>
       <c r="L271" s="10" t="s">
-        <v>632</v>
+        <v>211</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
@@ -12132,31 +12173,33 @@
         <v>4</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>621</v>
+        <v>910</v>
       </c>
       <c r="C272" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E272" s="12">
-        <v>1</v>
+        <v>807</v>
+      </c>
+      <c r="E272" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="F272" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G272" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H272" s="10"/>
+      <c r="H272" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I272" s="10"/>
       <c r="J272" s="10"/>
       <c r="K272" s="10" t="s">
-        <v>626</v>
+        <v>911</v>
       </c>
       <c r="L272" s="10" t="s">
-        <v>631</v>
+        <v>912</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
@@ -12164,31 +12207,27 @@
         <v>4</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>624</v>
+        <v>387</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E273" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="F273" s="11" t="s">
-        <v>625</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="E273" s="12"/>
+      <c r="F273" s="11"/>
       <c r="G273" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H273" s="10"/>
       <c r="I273" s="10"/>
       <c r="J273" s="10"/>
       <c r="K273" s="10" t="s">
-        <v>629</v>
+        <v>388</v>
       </c>
       <c r="L273" s="10" t="s">
-        <v>634</v>
+        <v>388</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
@@ -12196,31 +12235,35 @@
         <v>4</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>622</v>
+        <v>6</v>
       </c>
       <c r="C274" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D274" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E274" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F274" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G274" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H274" s="10"/>
-      <c r="I274" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H274" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I274" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="J274" s="10"/>
-      <c r="K274" s="10" t="s">
-        <v>628</v>
+      <c r="K274" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="L274" s="10" t="s">
-        <v>633</v>
+        <v>65</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">
@@ -12228,7 +12271,7 @@
         <v>4</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>815</v>
@@ -12237,10 +12280,10 @@
         <v>806</v>
       </c>
       <c r="E275" s="12">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="F275" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G275" s="11" t="b">
         <v>1</v>
@@ -12249,10 +12292,10 @@
       <c r="I275" s="10"/>
       <c r="J275" s="10"/>
       <c r="K275" s="10" t="s">
-        <v>614</v>
+        <v>627</v>
       </c>
       <c r="L275" s="10" t="s">
-        <v>615</v>
+        <v>632</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
@@ -12260,7 +12303,7 @@
         <v>4</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>5</v>
+        <v>621</v>
       </c>
       <c r="C276" s="9" t="s">
         <v>815</v>
@@ -12269,10 +12312,10 @@
         <v>806</v>
       </c>
       <c r="E276" s="12">
-        <v>670</v>
+        <v>1</v>
       </c>
       <c r="F276" s="11" t="s">
-        <v>212</v>
+        <v>625</v>
       </c>
       <c r="G276" s="11" t="b">
         <v>1</v>
@@ -12280,11 +12323,11 @@
       <c r="H276" s="10"/>
       <c r="I276" s="10"/>
       <c r="J276" s="10"/>
-      <c r="K276" s="9" t="s">
-        <v>126</v>
+      <c r="K276" s="10" t="s">
+        <v>626</v>
       </c>
       <c r="L276" s="10" t="s">
-        <v>64</v>
+        <v>631</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
@@ -12292,35 +12335,31 @@
         <v>4</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>100</v>
+        <v>624</v>
       </c>
       <c r="C277" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E277" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F277" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G277" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H277" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I277" s="10" t="s">
-        <v>786</v>
-      </c>
+      <c r="H277" s="10"/>
+      <c r="I277" s="10"/>
       <c r="J277" s="10"/>
-      <c r="K277" s="9" t="s">
-        <v>134</v>
+      <c r="K277" s="10" t="s">
+        <v>629</v>
       </c>
       <c r="L277" s="10" t="s">
-        <v>101</v>
+        <v>634</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
@@ -12328,7 +12367,7 @@
         <v>4</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>531</v>
+        <v>622</v>
       </c>
       <c r="C278" s="9" t="s">
         <v>815</v>
@@ -12337,10 +12376,10 @@
         <v>806</v>
       </c>
       <c r="E278" s="12">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F278" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G278" s="11" t="b">
         <v>1</v>
@@ -12349,10 +12388,10 @@
       <c r="I278" s="10"/>
       <c r="J278" s="10"/>
       <c r="K278" s="10" t="s">
-        <v>535</v>
+        <v>628</v>
       </c>
       <c r="L278" s="10" t="s">
-        <v>538</v>
+        <v>633</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
@@ -12360,7 +12399,7 @@
         <v>4</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>532</v>
+        <v>613</v>
       </c>
       <c r="C279" s="9" t="s">
         <v>815</v>
@@ -12369,7 +12408,7 @@
         <v>806</v>
       </c>
       <c r="E279" s="12">
-        <v>1.1000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="F279" s="11" t="s">
         <v>21</v>
@@ -12381,10 +12420,10 @@
       <c r="I279" s="10"/>
       <c r="J279" s="10"/>
       <c r="K279" s="10" t="s">
-        <v>536</v>
+        <v>614</v>
       </c>
       <c r="L279" s="10" t="s">
-        <v>539</v>
+        <v>615</v>
       </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.25">
@@ -12392,7 +12431,7 @@
         <v>4</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>815</v>
@@ -12401,22 +12440,22 @@
         <v>806</v>
       </c>
       <c r="E280" s="12">
-        <v>195</v>
+        <v>670</v>
       </c>
       <c r="F280" s="11" t="s">
-        <v>23</v>
+        <v>212</v>
       </c>
       <c r="G280" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H280" s="10"/>
       <c r="I280" s="10"/>
       <c r="J280" s="10"/>
       <c r="K280" s="9" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="L280" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">
@@ -12424,31 +12463,35 @@
         <v>4</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C281" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D281" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E281" s="12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F281" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G281" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H281" s="10"/>
-      <c r="I281" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="H281" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I281" s="10" t="s">
+        <v>786</v>
+      </c>
       <c r="J281" s="10"/>
       <c r="K281" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L281" s="10" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.25">
@@ -12456,7 +12499,7 @@
         <v>4</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>894</v>
+        <v>531</v>
       </c>
       <c r="C282" s="9" t="s">
         <v>815</v>
@@ -12465,7 +12508,7 @@
         <v>806</v>
       </c>
       <c r="E282" s="12">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F282" s="11" t="s">
         <v>21</v>
@@ -12477,10 +12520,10 @@
       <c r="I282" s="10"/>
       <c r="J282" s="10"/>
       <c r="K282" s="10" t="s">
-        <v>895</v>
+        <v>535</v>
       </c>
       <c r="L282" s="10" t="s">
-        <v>895</v>
+        <v>538</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.25">
@@ -12488,7 +12531,7 @@
         <v>4</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>97</v>
+        <v>532</v>
       </c>
       <c r="C283" s="9" t="s">
         <v>815</v>
@@ -12497,7 +12540,7 @@
         <v>806</v>
       </c>
       <c r="E283" s="12">
-        <v>1.33</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F283" s="11" t="s">
         <v>21</v>
@@ -12508,11 +12551,11 @@
       <c r="H283" s="10"/>
       <c r="I283" s="10"/>
       <c r="J283" s="10"/>
-      <c r="K283" s="9" t="s">
-        <v>128</v>
+      <c r="K283" s="10" t="s">
+        <v>536</v>
       </c>
       <c r="L283" s="10" t="s">
-        <v>98</v>
+        <v>539</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.25">
@@ -12520,7 +12563,7 @@
         <v>4</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>854</v>
+        <v>14</v>
       </c>
       <c r="C284" s="9" t="s">
         <v>815</v>
@@ -12529,22 +12572,22 @@
         <v>806</v>
       </c>
       <c r="E284" s="12">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="F284" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G284" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H284" s="10"/>
       <c r="I284" s="10"/>
       <c r="J284" s="10"/>
-      <c r="K284" s="10" t="s">
-        <v>857</v>
+      <c r="K284" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="L284" s="10" t="s">
-        <v>500</v>
+        <v>68</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.25">
@@ -12552,7 +12595,7 @@
         <v>4</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>855</v>
+        <v>13</v>
       </c>
       <c r="C285" s="9" t="s">
         <v>815</v>
@@ -12561,22 +12604,22 @@
         <v>806</v>
       </c>
       <c r="E285" s="12">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="F285" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G285" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H285" s="10"/>
       <c r="I285" s="10"/>
       <c r="J285" s="10"/>
-      <c r="K285" s="10" t="s">
-        <v>858</v>
+      <c r="K285" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="L285" s="10" t="s">
-        <v>501</v>
+        <v>67</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
@@ -12584,16 +12627,16 @@
         <v>4</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>497</v>
+        <v>894</v>
       </c>
       <c r="C286" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E286" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F286" s="11" t="s">
         <v>21</v>
@@ -12601,18 +12644,14 @@
       <c r="G286" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H286" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I286" s="10" t="s">
-        <v>520</v>
-      </c>
+      <c r="H286" s="10"/>
+      <c r="I286" s="10"/>
       <c r="J286" s="10"/>
       <c r="K286" s="10" t="s">
-        <v>498</v>
+        <v>895</v>
       </c>
       <c r="L286" s="10" t="s">
-        <v>499</v>
+        <v>895</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
@@ -12620,16 +12659,16 @@
         <v>4</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>774</v>
+        <v>97</v>
       </c>
       <c r="C287" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E287" s="12">
-        <v>0</v>
+        <v>1.33</v>
       </c>
       <c r="F287" s="11" t="s">
         <v>21</v>
@@ -12637,16 +12676,14 @@
       <c r="G287" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H287" s="10" t="s">
-        <v>131</v>
-      </c>
+      <c r="H287" s="10"/>
       <c r="I287" s="10"/>
       <c r="J287" s="10"/>
-      <c r="K287" s="10" t="s">
-        <v>775</v>
+      <c r="K287" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="L287" s="10" t="s">
-        <v>776</v>
+        <v>98</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
@@ -12654,33 +12691,31 @@
         <v>4</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>269</v>
+        <v>854</v>
       </c>
       <c r="C288" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D288" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E288" s="12">
-        <v>0</v>
-      </c>
-      <c r="F288" s="11"/>
+        <v>180</v>
+      </c>
+      <c r="F288" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="G288" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H288" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I288" s="10" t="s">
-        <v>271</v>
-      </c>
+      <c r="H288" s="10"/>
+      <c r="I288" s="10"/>
       <c r="J288" s="10"/>
       <c r="K288" s="10" t="s">
-        <v>270</v>
+        <v>857</v>
       </c>
       <c r="L288" s="10" t="s">
-        <v>284</v>
+        <v>500</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -12688,7 +12723,7 @@
         <v>4</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>9</v>
+        <v>855</v>
       </c>
       <c r="C289" s="9" t="s">
         <v>815</v>
@@ -12697,10 +12732,10 @@
         <v>806</v>
       </c>
       <c r="E289" s="12">
-        <v>195</v>
+        <v>85</v>
       </c>
       <c r="F289" s="11" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G289" s="11" t="b">
         <v>1</v>
@@ -12708,11 +12743,11 @@
       <c r="H289" s="10"/>
       <c r="I289" s="10"/>
       <c r="J289" s="10"/>
-      <c r="K289" s="9" t="s">
-        <v>285</v>
+      <c r="K289" s="10" t="s">
+        <v>858</v>
       </c>
       <c r="L289" s="10" t="s">
-        <v>286</v>
+        <v>501</v>
       </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
@@ -12720,16 +12755,16 @@
         <v>4</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>787</v>
+        <v>497</v>
       </c>
       <c r="C290" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D290" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E290" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F290" s="11" t="s">
         <v>21</v>
@@ -12737,14 +12772,18 @@
       <c r="G290" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H290" s="10"/>
-      <c r="I290" s="10"/>
+      <c r="H290" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I290" s="10" t="s">
+        <v>520</v>
+      </c>
       <c r="J290" s="10"/>
       <c r="K290" s="10" t="s">
-        <v>788</v>
+        <v>498</v>
       </c>
       <c r="L290" s="10" t="s">
-        <v>789</v>
+        <v>499</v>
       </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
@@ -12752,7 +12791,7 @@
         <v>4</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>533</v>
+        <v>774</v>
       </c>
       <c r="C291" s="9" t="s">
         <v>815</v>
@@ -12763,22 +12802,22 @@
       <c r="E291" s="12">
         <v>0</v>
       </c>
-      <c r="F291" s="11"/>
+      <c r="F291" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G291" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H291" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="I291" s="10" t="s">
-        <v>534</v>
-      </c>
+      <c r="I291" s="10"/>
       <c r="J291" s="10"/>
       <c r="K291" s="10" t="s">
-        <v>537</v>
+        <v>775</v>
       </c>
       <c r="L291" s="10" t="s">
-        <v>540</v>
+        <v>776</v>
       </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
@@ -12786,31 +12825,33 @@
         <v>4</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>541</v>
+        <v>269</v>
       </c>
       <c r="C292" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D292" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E292" s="12">
-        <v>1</v>
-      </c>
-      <c r="F292" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F292" s="11"/>
       <c r="G292" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H292" s="10"/>
-      <c r="I292" s="10"/>
+      <c r="H292" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I292" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="J292" s="10"/>
       <c r="K292" s="10" t="s">
-        <v>542</v>
+        <v>270</v>
       </c>
       <c r="L292" s="10" t="s">
-        <v>543</v>
+        <v>284</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
@@ -12818,7 +12859,7 @@
         <v>4</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>620</v>
+        <v>9</v>
       </c>
       <c r="C293" s="9" t="s">
         <v>815</v>
@@ -12827,10 +12868,10 @@
         <v>806</v>
       </c>
       <c r="E293" s="12">
-        <v>1E-3</v>
+        <v>195</v>
       </c>
       <c r="F293" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G293" s="11" t="b">
         <v>1</v>
@@ -12838,11 +12879,11 @@
       <c r="H293" s="10"/>
       <c r="I293" s="10"/>
       <c r="J293" s="10"/>
-      <c r="K293" s="10" t="s">
-        <v>630</v>
+      <c r="K293" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="L293" s="10" t="s">
-        <v>635</v>
+        <v>286</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
@@ -12850,7 +12891,7 @@
         <v>4</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>903</v>
+        <v>787</v>
       </c>
       <c r="C294" s="9" t="s">
         <v>815</v>
@@ -12859,10 +12900,10 @@
         <v>806</v>
       </c>
       <c r="E294" s="12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F294" s="11" t="s">
-        <v>906</v>
+        <v>21</v>
       </c>
       <c r="G294" s="11" t="b">
         <v>1</v>
@@ -12871,10 +12912,10 @@
       <c r="I294" s="10"/>
       <c r="J294" s="10"/>
       <c r="K294" s="10" t="s">
-        <v>905</v>
+        <v>788</v>
       </c>
       <c r="L294" s="10" t="s">
-        <v>904</v>
+        <v>789</v>
       </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
@@ -12882,31 +12923,33 @@
         <v>4</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>828</v>
+        <v>533</v>
       </c>
       <c r="C295" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E295" s="12">
         <v>0</v>
       </c>
-      <c r="F295" s="11" t="s">
-        <v>308</v>
-      </c>
+      <c r="F295" s="11"/>
       <c r="G295" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H295" s="10"/>
-      <c r="I295" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="H295" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I295" s="10" t="s">
+        <v>534</v>
+      </c>
       <c r="J295" s="10"/>
       <c r="K295" s="10" t="s">
-        <v>831</v>
+        <v>537</v>
       </c>
       <c r="L295" s="10" t="s">
-        <v>832</v>
+        <v>540</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
@@ -12914,31 +12957,31 @@
         <v>4</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>827</v>
+        <v>541</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D296" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E296" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F296" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G296" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H296" s="10"/>
       <c r="I296" s="10"/>
       <c r="J296" s="10"/>
       <c r="K296" s="10" t="s">
-        <v>801</v>
+        <v>542</v>
       </c>
       <c r="L296" s="10" t="s">
-        <v>833</v>
+        <v>543</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.25">
@@ -12946,29 +12989,31 @@
         <v>4</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>389</v>
+        <v>620</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D297" s="9" t="s">
-        <v>813</v>
-      </c>
-      <c r="E297" s="12"/>
+        <v>806</v>
+      </c>
+      <c r="E297" s="12">
+        <v>1E-3</v>
+      </c>
       <c r="F297" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G297" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H297" s="10"/>
       <c r="I297" s="10"/>
       <c r="J297" s="10"/>
       <c r="K297" s="10" t="s">
-        <v>390</v>
+        <v>630</v>
       </c>
       <c r="L297" s="10" t="s">
-        <v>390</v>
+        <v>635</v>
       </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.25">
@@ -12976,31 +13021,31 @@
         <v>4</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>856</v>
+        <v>903</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D298" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E298" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F298" s="11" t="s">
-        <v>56</v>
+        <v>906</v>
       </c>
       <c r="G298" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H298" s="10"/>
       <c r="I298" s="10"/>
       <c r="J298" s="10"/>
       <c r="K298" s="10" t="s">
-        <v>859</v>
+        <v>905</v>
       </c>
       <c r="L298" s="10" t="s">
-        <v>859</v>
+        <v>904</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
@@ -13008,7 +13053,7 @@
         <v>4</v>
       </c>
       <c r="B299" s="9" t="s">
-        <v>861</v>
+        <v>828</v>
       </c>
       <c r="C299" s="9" t="s">
         <v>816</v>
@@ -13020,7 +13065,7 @@
         <v>0</v>
       </c>
       <c r="F299" s="11" t="s">
-        <v>56</v>
+        <v>308</v>
       </c>
       <c r="G299" s="11" t="b">
         <v>0</v>
@@ -13029,9 +13074,135 @@
       <c r="I299" s="10"/>
       <c r="J299" s="10"/>
       <c r="K299" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="L299" s="10" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A300" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B300" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="C300" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D300" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E300" s="12">
+        <v>0</v>
+      </c>
+      <c r="F300" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="G300" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H300" s="10"/>
+      <c r="I300" s="10"/>
+      <c r="J300" s="10"/>
+      <c r="K300" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="L300" s="10" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A301" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B301" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C301" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D301" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="E301" s="12"/>
+      <c r="F301" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G301" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H301" s="10"/>
+      <c r="I301" s="10"/>
+      <c r="J301" s="10"/>
+      <c r="K301" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="L301" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A302" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B302" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="C302" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D302" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E302" s="12">
+        <v>0</v>
+      </c>
+      <c r="F302" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G302" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H302" s="10"/>
+      <c r="I302" s="10"/>
+      <c r="J302" s="10"/>
+      <c r="K302" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="L302" s="10" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A303" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B303" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="C303" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D303" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E303" s="12">
+        <v>0</v>
+      </c>
+      <c r="F303" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G303" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H303" s="10"/>
+      <c r="I303" s="10"/>
+      <c r="J303" s="10"/>
+      <c r="K303" s="10" t="s">
         <v>860</v>
       </c>
-      <c r="L299" s="10" t="s">
+      <c r="L303" s="10" t="s">
         <v>860</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding global receiver offset calculation and relative offset
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545333F-24FD-4244-A031-09AAA7851C90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AD1926-2AAC-49F1-AFAA-4E0BC801B0A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="935">
   <si>
     <t>String name</t>
   </si>
@@ -2771,9 +2771,6 @@
     <t>Receiver offset reference</t>
   </si>
   <si>
-    <t>Tower=0</t>
-  </si>
-  <si>
     <t>Receiver offset is relative to the position of the selected item. Options include tower or other receivers.</t>
   </si>
   <si>
@@ -2793,6 +2790,36 @@
   </si>
   <si>
     <t>The number of heliostats required to meet this value times the design power of each receiver are considered for layout</t>
+  </si>
+  <si>
+    <t>rec_offset_y_global</t>
+  </si>
+  <si>
+    <t>rec_offset_x_global</t>
+  </si>
+  <si>
+    <t>rec_offset_z_global</t>
+  </si>
+  <si>
+    <t>Receiver global positioning offset - X axis</t>
+  </si>
+  <si>
+    <t>Receiver global positioning offset - Y axis</t>
+  </si>
+  <si>
+    <t>Receiver global positioning offset - Z axis</t>
+  </si>
+  <si>
+    <t>Offset of receiver center in the East(+)/West(-) direction from the reference object</t>
+  </si>
+  <si>
+    <t>Offset of receiver center in the North(+)/South(-) direction from the reference object</t>
+  </si>
+  <si>
+    <t>Offset of the receiver center in the vertical direction from the reference object, positive upwards</t>
+  </si>
+  <si>
+    <t>Tower=-1</t>
   </si>
 </sst>
 </file>
@@ -3031,10 +3058,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L303" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L303" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:L313">
-    <sortCondition ref="A1:A313"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L306" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L306" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:L316">
+    <sortCondition ref="A1:A316"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain" dataDxfId="11"/>
@@ -3375,11 +3402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L303"/>
+  <dimension ref="A1:L306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E202" sqref="E202"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E244" sqref="E244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9623,7 +9650,7 @@
         <v>714</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C194" s="9" t="s">
         <v>815</v>
@@ -9644,10 +9671,10 @@
       <c r="I194" s="10"/>
       <c r="J194" s="10"/>
       <c r="K194" s="10" t="s">
+        <v>920</v>
+      </c>
+      <c r="L194" s="10" t="s">
         <v>921</v>
-      </c>
-      <c r="L194" s="10" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.25">
@@ -9655,7 +9682,7 @@
         <v>714</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C195" s="9" t="s">
         <v>815</v>
@@ -9676,10 +9703,10 @@
       <c r="I195" s="10"/>
       <c r="J195" s="10"/>
       <c r="K195" s="10" t="s">
+        <v>923</v>
+      </c>
+      <c r="L195" s="10" t="s">
         <v>924</v>
-      </c>
-      <c r="L195" s="10" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.25">
@@ -11177,7 +11204,7 @@
         <v>146</v>
       </c>
       <c r="L241" s="10" t="s">
-        <v>148</v>
+        <v>931</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
@@ -11209,7 +11236,7 @@
         <v>147</v>
       </c>
       <c r="L242" s="10" t="s">
-        <v>149</v>
+        <v>932</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
@@ -11241,7 +11268,7 @@
         <v>303</v>
       </c>
       <c r="L243" s="10" t="s">
-        <v>426</v>
+        <v>933</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
@@ -11270,14 +11297,14 @@
         <v>131</v>
       </c>
       <c r="I244" s="10" t="s">
-        <v>918</v>
+        <v>934</v>
       </c>
       <c r="J244" s="10"/>
       <c r="K244" s="10" t="s">
         <v>917</v>
       </c>
       <c r="L244" s="10" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
@@ -11738,98 +11765,98 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>19</v>
+        <v>926</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D259" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E259" s="12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F259" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G259" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H259" s="10"/>
       <c r="I259" s="10"/>
       <c r="J259" s="10"/>
-      <c r="K259" s="10" t="s">
-        <v>138</v>
+      <c r="K259" s="9" t="s">
+        <v>928</v>
       </c>
       <c r="L259" s="10" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>18</v>
+        <v>925</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D260" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E260" s="12">
-        <v>-180</v>
+        <v>0</v>
       </c>
       <c r="F260" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G260" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H260" s="10"/>
       <c r="I260" s="10"/>
       <c r="J260" s="10"/>
-      <c r="K260" s="10" t="s">
-        <v>139</v>
+      <c r="K260" s="9" t="s">
+        <v>929</v>
       </c>
       <c r="L260" s="10" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>99</v>
+        <v>927</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D261" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E261" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F261" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G261" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H261" s="10"/>
       <c r="I261" s="10"/>
       <c r="J261" s="10"/>
       <c r="K261" s="9" t="s">
-        <v>127</v>
+        <v>930</v>
       </c>
       <c r="L261" s="10" t="s">
-        <v>213</v>
+        <v>426</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
@@ -11837,31 +11864,31 @@
         <v>4</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>545</v>
+        <v>19</v>
       </c>
       <c r="C262" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D262" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E262" s="12" t="s">
-        <v>546</v>
+        <v>806</v>
+      </c>
+      <c r="E262" s="12">
+        <v>180</v>
       </c>
       <c r="F262" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G262" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H262" s="10"/>
       <c r="I262" s="10"/>
       <c r="J262" s="10"/>
       <c r="K262" s="10" t="s">
-        <v>547</v>
+        <v>138</v>
       </c>
       <c r="L262" s="10" t="s">
-        <v>547</v>
+        <v>110</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
@@ -11869,35 +11896,31 @@
         <v>4</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="C263" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E263" s="12">
-        <v>5</v>
+        <v>-180</v>
       </c>
       <c r="F263" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G263" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H263" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I263" s="10" t="s">
-        <v>556</v>
-      </c>
+      <c r="H263" s="10"/>
+      <c r="I263" s="10"/>
       <c r="J263" s="10"/>
-      <c r="K263" s="9" t="s">
-        <v>135</v>
+      <c r="K263" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="L263" s="10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
@@ -11905,16 +11928,16 @@
         <v>4</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>192</v>
+        <v>99</v>
       </c>
       <c r="C264" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D264" s="9" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="E264" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F264" s="11" t="s">
         <v>21</v>
@@ -11925,11 +11948,11 @@
       <c r="H264" s="10"/>
       <c r="I264" s="10"/>
       <c r="J264" s="10"/>
-      <c r="K264" s="10" t="s">
-        <v>193</v>
+      <c r="K264" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="L264" s="10" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
@@ -11937,31 +11960,31 @@
         <v>4</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>582</v>
+        <v>545</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D265" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E265" s="12">
-        <v>2</v>
+        <v>805</v>
+      </c>
+      <c r="E265" s="12" t="s">
+        <v>546</v>
       </c>
       <c r="F265" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G265" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H265" s="10"/>
       <c r="I265" s="10"/>
       <c r="J265" s="10"/>
       <c r="K265" s="10" t="s">
-        <v>583</v>
+        <v>547</v>
       </c>
       <c r="L265" s="10" t="s">
-        <v>584</v>
+        <v>547</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
@@ -11969,31 +11992,35 @@
         <v>4</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>188</v>
+        <v>104</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D266" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E266" s="12">
-        <v>950</v>
+        <v>5</v>
       </c>
       <c r="F266" s="11" t="s">
-        <v>189</v>
+        <v>21</v>
       </c>
       <c r="G266" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H266" s="10"/>
-      <c r="I266" s="10"/>
+      <c r="H266" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I266" s="10" t="s">
+        <v>556</v>
+      </c>
       <c r="J266" s="10"/>
-      <c r="K266" s="10" t="s">
-        <v>190</v>
+      <c r="K266" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="L266" s="10" t="s">
-        <v>191</v>
+        <v>105</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
@@ -12001,16 +12028,16 @@
         <v>4</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>521</v>
+        <v>192</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E267" s="12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F267" s="11" t="s">
         <v>21</v>
@@ -12018,18 +12045,14 @@
       <c r="G267" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H267" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I267" s="10" t="s">
-        <v>523</v>
-      </c>
+      <c r="H267" s="10"/>
+      <c r="I267" s="10"/>
       <c r="J267" s="10"/>
       <c r="K267" s="10" t="s">
-        <v>555</v>
+        <v>193</v>
       </c>
       <c r="L267" s="10" t="s">
-        <v>522</v>
+        <v>194</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
@@ -12037,16 +12060,16 @@
         <v>4</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>891</v>
+        <v>582</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E268" s="12" t="b">
-        <v>0</v>
+        <v>804</v>
+      </c>
+      <c r="E268" s="12">
+        <v>2</v>
       </c>
       <c r="F268" s="11" t="s">
         <v>21</v>
@@ -12054,16 +12077,14 @@
       <c r="G268" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H268" s="10" t="s">
-        <v>202</v>
-      </c>
+      <c r="H268" s="10"/>
       <c r="I268" s="10"/>
       <c r="J268" s="10"/>
       <c r="K268" s="10" t="s">
-        <v>892</v>
+        <v>583</v>
       </c>
       <c r="L268" s="10" t="s">
-        <v>893</v>
+        <v>584</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
@@ -12071,33 +12092,31 @@
         <v>4</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>636</v>
+        <v>188</v>
       </c>
       <c r="C269" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E269" s="12" t="b">
-        <v>1</v>
+        <v>806</v>
+      </c>
+      <c r="E269" s="12">
+        <v>950</v>
       </c>
       <c r="F269" s="11" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="G269" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H269" s="10" t="s">
-        <v>202</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H269" s="10"/>
       <c r="I269" s="10"/>
       <c r="J269" s="10"/>
       <c r="K269" s="10" t="s">
-        <v>637</v>
+        <v>190</v>
       </c>
       <c r="L269" s="10" t="s">
-        <v>638</v>
+        <v>191</v>
       </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
@@ -12105,16 +12124,16 @@
         <v>4</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>612</v>
+        <v>521</v>
       </c>
       <c r="C270" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>807</v>
-      </c>
-      <c r="E270" s="12" t="b">
-        <v>0</v>
+        <v>805</v>
+      </c>
+      <c r="E270" s="12">
+        <v>7</v>
       </c>
       <c r="F270" s="11" t="s">
         <v>21</v>
@@ -12123,15 +12142,17 @@
         <v>1</v>
       </c>
       <c r="H270" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="I270" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="I270" s="10" t="s">
+        <v>523</v>
+      </c>
       <c r="J270" s="10"/>
       <c r="K270" s="10" t="s">
-        <v>610</v>
+        <v>555</v>
       </c>
       <c r="L270" s="10" t="s">
-        <v>611</v>
+        <v>522</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
@@ -12139,7 +12160,7 @@
         <v>4</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>209</v>
+        <v>891</v>
       </c>
       <c r="C271" s="9" t="s">
         <v>815</v>
@@ -12148,13 +12169,13 @@
         <v>807</v>
       </c>
       <c r="E271" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F271" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G271" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H271" s="10" t="s">
         <v>202</v>
@@ -12162,10 +12183,10 @@
       <c r="I271" s="10"/>
       <c r="J271" s="10"/>
       <c r="K271" s="10" t="s">
-        <v>210</v>
+        <v>892</v>
       </c>
       <c r="L271" s="10" t="s">
-        <v>211</v>
+        <v>893</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
@@ -12173,7 +12194,7 @@
         <v>4</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>910</v>
+        <v>636</v>
       </c>
       <c r="C272" s="9" t="s">
         <v>815</v>
@@ -12182,13 +12203,13 @@
         <v>807</v>
       </c>
       <c r="E272" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F272" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G272" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H272" s="10" t="s">
         <v>202</v>
@@ -12196,10 +12217,10 @@
       <c r="I272" s="10"/>
       <c r="J272" s="10"/>
       <c r="K272" s="10" t="s">
-        <v>911</v>
+        <v>637</v>
       </c>
       <c r="L272" s="10" t="s">
-        <v>912</v>
+        <v>638</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
@@ -12207,27 +12228,33 @@
         <v>4</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>387</v>
+        <v>612</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E273" s="12"/>
-      <c r="F273" s="11"/>
+        <v>807</v>
+      </c>
+      <c r="E273" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F273" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G273" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H273" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="H273" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I273" s="10"/>
       <c r="J273" s="10"/>
       <c r="K273" s="10" t="s">
-        <v>388</v>
+        <v>610</v>
       </c>
       <c r="L273" s="10" t="s">
-        <v>388</v>
+        <v>611</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
@@ -12235,16 +12262,16 @@
         <v>4</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="C274" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D274" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E274" s="12">
-        <v>0</v>
+        <v>807</v>
+      </c>
+      <c r="E274" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="F274" s="11" t="s">
         <v>21</v>
@@ -12253,17 +12280,15 @@
         <v>0</v>
       </c>
       <c r="H274" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I274" s="10" t="s">
-        <v>132</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="I274" s="10"/>
       <c r="J274" s="10"/>
-      <c r="K274" s="9" t="s">
-        <v>133</v>
+      <c r="K274" s="10" t="s">
+        <v>210</v>
       </c>
       <c r="L274" s="10" t="s">
-        <v>65</v>
+        <v>211</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">
@@ -12271,31 +12296,33 @@
         <v>4</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>623</v>
+        <v>910</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E275" s="12">
-        <v>1</v>
+        <v>807</v>
+      </c>
+      <c r="E275" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="F275" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G275" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H275" s="10"/>
+      <c r="H275" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I275" s="10"/>
       <c r="J275" s="10"/>
       <c r="K275" s="10" t="s">
-        <v>627</v>
+        <v>911</v>
       </c>
       <c r="L275" s="10" t="s">
-        <v>632</v>
+        <v>912</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
@@ -12303,31 +12330,27 @@
         <v>4</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>621</v>
+        <v>387</v>
       </c>
       <c r="C276" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D276" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E276" s="12">
-        <v>1</v>
-      </c>
-      <c r="F276" s="11" t="s">
-        <v>625</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="E276" s="12"/>
+      <c r="F276" s="11"/>
       <c r="G276" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H276" s="10"/>
       <c r="I276" s="10"/>
       <c r="J276" s="10"/>
       <c r="K276" s="10" t="s">
-        <v>626</v>
+        <v>388</v>
       </c>
       <c r="L276" s="10" t="s">
-        <v>631</v>
+        <v>388</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
@@ -12335,31 +12358,35 @@
         <v>4</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>624</v>
+        <v>6</v>
       </c>
       <c r="C277" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E277" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F277" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G277" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H277" s="10"/>
-      <c r="I277" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H277" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I277" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="J277" s="10"/>
-      <c r="K277" s="10" t="s">
-        <v>629</v>
+      <c r="K277" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="L277" s="10" t="s">
-        <v>634</v>
+        <v>65</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
@@ -12367,7 +12394,7 @@
         <v>4</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C278" s="9" t="s">
         <v>815</v>
@@ -12376,7 +12403,7 @@
         <v>806</v>
       </c>
       <c r="E278" s="12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F278" s="11" t="s">
         <v>625</v>
@@ -12388,10 +12415,10 @@
       <c r="I278" s="10"/>
       <c r="J278" s="10"/>
       <c r="K278" s="10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="L278" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
@@ -12399,7 +12426,7 @@
         <v>4</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="C279" s="9" t="s">
         <v>815</v>
@@ -12408,10 +12435,10 @@
         <v>806</v>
       </c>
       <c r="E279" s="12">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="F279" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G279" s="11" t="b">
         <v>1</v>
@@ -12420,10 +12447,10 @@
       <c r="I279" s="10"/>
       <c r="J279" s="10"/>
       <c r="K279" s="10" t="s">
-        <v>614</v>
+        <v>626</v>
       </c>
       <c r="L279" s="10" t="s">
-        <v>615</v>
+        <v>631</v>
       </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.25">
@@ -12431,7 +12458,7 @@
         <v>4</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>5</v>
+        <v>624</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>815</v>
@@ -12440,10 +12467,10 @@
         <v>806</v>
       </c>
       <c r="E280" s="12">
-        <v>670</v>
+        <v>0.1</v>
       </c>
       <c r="F280" s="11" t="s">
-        <v>212</v>
+        <v>625</v>
       </c>
       <c r="G280" s="11" t="b">
         <v>1</v>
@@ -12451,11 +12478,11 @@
       <c r="H280" s="10"/>
       <c r="I280" s="10"/>
       <c r="J280" s="10"/>
-      <c r="K280" s="9" t="s">
-        <v>126</v>
+      <c r="K280" s="10" t="s">
+        <v>629</v>
       </c>
       <c r="L280" s="10" t="s">
-        <v>64</v>
+        <v>634</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">
@@ -12463,35 +12490,31 @@
         <v>4</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>100</v>
+        <v>622</v>
       </c>
       <c r="C281" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D281" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E281" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F281" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G281" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H281" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I281" s="10" t="s">
-        <v>786</v>
-      </c>
+      <c r="H281" s="10"/>
+      <c r="I281" s="10"/>
       <c r="J281" s="10"/>
-      <c r="K281" s="9" t="s">
-        <v>134</v>
+      <c r="K281" s="10" t="s">
+        <v>628</v>
       </c>
       <c r="L281" s="10" t="s">
-        <v>101</v>
+        <v>633</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.25">
@@ -12499,7 +12522,7 @@
         <v>4</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>531</v>
+        <v>613</v>
       </c>
       <c r="C282" s="9" t="s">
         <v>815</v>
@@ -12508,7 +12531,7 @@
         <v>806</v>
       </c>
       <c r="E282" s="12">
-        <v>1.1000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="F282" s="11" t="s">
         <v>21</v>
@@ -12520,10 +12543,10 @@
       <c r="I282" s="10"/>
       <c r="J282" s="10"/>
       <c r="K282" s="10" t="s">
-        <v>535</v>
+        <v>614</v>
       </c>
       <c r="L282" s="10" t="s">
-        <v>538</v>
+        <v>615</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.25">
@@ -12531,7 +12554,7 @@
         <v>4</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>532</v>
+        <v>5</v>
       </c>
       <c r="C283" s="9" t="s">
         <v>815</v>
@@ -12540,10 +12563,10 @@
         <v>806</v>
       </c>
       <c r="E283" s="12">
-        <v>1.1000000000000001</v>
+        <v>670</v>
       </c>
       <c r="F283" s="11" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="G283" s="11" t="b">
         <v>1</v>
@@ -12551,11 +12574,11 @@
       <c r="H283" s="10"/>
       <c r="I283" s="10"/>
       <c r="J283" s="10"/>
-      <c r="K283" s="10" t="s">
-        <v>536</v>
+      <c r="K283" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="L283" s="10" t="s">
-        <v>539</v>
+        <v>64</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.25">
@@ -12563,31 +12586,35 @@
         <v>4</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C284" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D284" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E284" s="12">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="F284" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G284" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H284" s="10"/>
-      <c r="I284" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="H284" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I284" s="10" t="s">
+        <v>786</v>
+      </c>
       <c r="J284" s="10"/>
       <c r="K284" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L284" s="10" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.25">
@@ -12595,7 +12622,7 @@
         <v>4</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>13</v>
+        <v>531</v>
       </c>
       <c r="C285" s="9" t="s">
         <v>815</v>
@@ -12604,22 +12631,22 @@
         <v>806</v>
       </c>
       <c r="E285" s="12">
-        <v>16</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F285" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G285" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H285" s="10"/>
       <c r="I285" s="10"/>
       <c r="J285" s="10"/>
-      <c r="K285" s="9" t="s">
-        <v>136</v>
+      <c r="K285" s="10" t="s">
+        <v>535</v>
       </c>
       <c r="L285" s="10" t="s">
-        <v>67</v>
+        <v>538</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
@@ -12627,7 +12654,7 @@
         <v>4</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>894</v>
+        <v>532</v>
       </c>
       <c r="C286" s="9" t="s">
         <v>815</v>
@@ -12636,7 +12663,7 @@
         <v>806</v>
       </c>
       <c r="E286" s="12">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F286" s="11" t="s">
         <v>21</v>
@@ -12648,10 +12675,10 @@
       <c r="I286" s="10"/>
       <c r="J286" s="10"/>
       <c r="K286" s="10" t="s">
-        <v>895</v>
+        <v>536</v>
       </c>
       <c r="L286" s="10" t="s">
-        <v>895</v>
+        <v>539</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
@@ -12659,7 +12686,7 @@
         <v>4</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="C287" s="9" t="s">
         <v>815</v>
@@ -12668,22 +12695,22 @@
         <v>806</v>
       </c>
       <c r="E287" s="12">
-        <v>1.33</v>
+        <v>195</v>
       </c>
       <c r="F287" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G287" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H287" s="10"/>
       <c r="I287" s="10"/>
       <c r="J287" s="10"/>
       <c r="K287" s="9" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="L287" s="10" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
@@ -12691,7 +12718,7 @@
         <v>4</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>854</v>
+        <v>13</v>
       </c>
       <c r="C288" s="9" t="s">
         <v>815</v>
@@ -12700,22 +12727,22 @@
         <v>806</v>
       </c>
       <c r="E288" s="12">
-        <v>180</v>
+        <v>16</v>
       </c>
       <c r="F288" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G288" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H288" s="10"/>
       <c r="I288" s="10"/>
       <c r="J288" s="10"/>
-      <c r="K288" s="10" t="s">
-        <v>857</v>
+      <c r="K288" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="L288" s="10" t="s">
-        <v>500</v>
+        <v>67</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -12723,7 +12750,7 @@
         <v>4</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>855</v>
+        <v>894</v>
       </c>
       <c r="C289" s="9" t="s">
         <v>815</v>
@@ -12732,10 +12759,10 @@
         <v>806</v>
       </c>
       <c r="E289" s="12">
-        <v>85</v>
+        <v>0.5</v>
       </c>
       <c r="F289" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G289" s="11" t="b">
         <v>1</v>
@@ -12744,10 +12771,10 @@
       <c r="I289" s="10"/>
       <c r="J289" s="10"/>
       <c r="K289" s="10" t="s">
-        <v>858</v>
+        <v>895</v>
       </c>
       <c r="L289" s="10" t="s">
-        <v>501</v>
+        <v>895</v>
       </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
@@ -12755,16 +12782,16 @@
         <v>4</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>497</v>
+        <v>97</v>
       </c>
       <c r="C290" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D290" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E290" s="12">
-        <v>0</v>
+        <v>1.33</v>
       </c>
       <c r="F290" s="11" t="s">
         <v>21</v>
@@ -12772,18 +12799,14 @@
       <c r="G290" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H290" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I290" s="10" t="s">
-        <v>520</v>
-      </c>
+      <c r="H290" s="10"/>
+      <c r="I290" s="10"/>
       <c r="J290" s="10"/>
-      <c r="K290" s="10" t="s">
-        <v>498</v>
+      <c r="K290" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="L290" s="10" t="s">
-        <v>499</v>
+        <v>98</v>
       </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
@@ -12791,33 +12814,31 @@
         <v>4</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>774</v>
+        <v>854</v>
       </c>
       <c r="C291" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E291" s="12">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F291" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G291" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H291" s="10" t="s">
-        <v>131</v>
-      </c>
+      <c r="H291" s="10"/>
       <c r="I291" s="10"/>
       <c r="J291" s="10"/>
       <c r="K291" s="10" t="s">
-        <v>775</v>
+        <v>857</v>
       </c>
       <c r="L291" s="10" t="s">
-        <v>776</v>
+        <v>500</v>
       </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
@@ -12825,33 +12846,31 @@
         <v>4</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>269</v>
+        <v>855</v>
       </c>
       <c r="C292" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D292" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E292" s="12">
-        <v>0</v>
-      </c>
-      <c r="F292" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="F292" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="G292" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H292" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I292" s="10" t="s">
-        <v>271</v>
-      </c>
+      <c r="H292" s="10"/>
+      <c r="I292" s="10"/>
       <c r="J292" s="10"/>
       <c r="K292" s="10" t="s">
-        <v>270</v>
+        <v>858</v>
       </c>
       <c r="L292" s="10" t="s">
-        <v>284</v>
+        <v>501</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
@@ -12859,31 +12878,35 @@
         <v>4</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>9</v>
+        <v>497</v>
       </c>
       <c r="C293" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D293" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E293" s="12">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="F293" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G293" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H293" s="10"/>
-      <c r="I293" s="10"/>
+      <c r="H293" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I293" s="10" t="s">
+        <v>520</v>
+      </c>
       <c r="J293" s="10"/>
-      <c r="K293" s="9" t="s">
-        <v>285</v>
+      <c r="K293" s="10" t="s">
+        <v>498</v>
       </c>
       <c r="L293" s="10" t="s">
-        <v>286</v>
+        <v>499</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
@@ -12891,16 +12914,16 @@
         <v>4</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>787</v>
+        <v>774</v>
       </c>
       <c r="C294" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E294" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F294" s="11" t="s">
         <v>21</v>
@@ -12908,14 +12931,16 @@
       <c r="G294" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H294" s="10"/>
+      <c r="H294" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="I294" s="10"/>
       <c r="J294" s="10"/>
       <c r="K294" s="10" t="s">
-        <v>788</v>
+        <v>775</v>
       </c>
       <c r="L294" s="10" t="s">
-        <v>789</v>
+        <v>776</v>
       </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
@@ -12923,7 +12948,7 @@
         <v>4</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>533</v>
+        <v>269</v>
       </c>
       <c r="C295" s="9" t="s">
         <v>815</v>
@@ -12942,14 +12967,14 @@
         <v>131</v>
       </c>
       <c r="I295" s="10" t="s">
-        <v>534</v>
+        <v>271</v>
       </c>
       <c r="J295" s="10"/>
       <c r="K295" s="10" t="s">
-        <v>537</v>
+        <v>270</v>
       </c>
       <c r="L295" s="10" t="s">
-        <v>540</v>
+        <v>284</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
@@ -12957,7 +12982,7 @@
         <v>4</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>541</v>
+        <v>9</v>
       </c>
       <c r="C296" s="9" t="s">
         <v>815</v>
@@ -12966,10 +12991,10 @@
         <v>806</v>
       </c>
       <c r="E296" s="12">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="F296" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G296" s="11" t="b">
         <v>1</v>
@@ -12977,11 +13002,11 @@
       <c r="H296" s="10"/>
       <c r="I296" s="10"/>
       <c r="J296" s="10"/>
-      <c r="K296" s="10" t="s">
-        <v>542</v>
+      <c r="K296" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="L296" s="10" t="s">
-        <v>543</v>
+        <v>286</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.25">
@@ -12989,7 +13014,7 @@
         <v>4</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>620</v>
+        <v>787</v>
       </c>
       <c r="C297" s="9" t="s">
         <v>815</v>
@@ -12998,7 +13023,7 @@
         <v>806</v>
       </c>
       <c r="E297" s="12">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="F297" s="11" t="s">
         <v>21</v>
@@ -13010,10 +13035,10 @@
       <c r="I297" s="10"/>
       <c r="J297" s="10"/>
       <c r="K297" s="10" t="s">
-        <v>630</v>
+        <v>788</v>
       </c>
       <c r="L297" s="10" t="s">
-        <v>635</v>
+        <v>789</v>
       </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.25">
@@ -13021,31 +13046,33 @@
         <v>4</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>903</v>
+        <v>533</v>
       </c>
       <c r="C298" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D298" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E298" s="12">
-        <v>100</v>
-      </c>
-      <c r="F298" s="11" t="s">
-        <v>906</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F298" s="11"/>
       <c r="G298" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H298" s="10"/>
-      <c r="I298" s="10"/>
+      <c r="H298" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I298" s="10" t="s">
+        <v>534</v>
+      </c>
       <c r="J298" s="10"/>
       <c r="K298" s="10" t="s">
-        <v>905</v>
+        <v>537</v>
       </c>
       <c r="L298" s="10" t="s">
-        <v>904</v>
+        <v>540</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
@@ -13053,31 +13080,31 @@
         <v>4</v>
       </c>
       <c r="B299" s="9" t="s">
-        <v>828</v>
+        <v>541</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D299" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E299" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F299" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G299" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H299" s="10"/>
       <c r="I299" s="10"/>
       <c r="J299" s="10"/>
       <c r="K299" s="10" t="s">
-        <v>831</v>
+        <v>542</v>
       </c>
       <c r="L299" s="10" t="s">
-        <v>832</v>
+        <v>543</v>
       </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.25">
@@ -13085,31 +13112,31 @@
         <v>4</v>
       </c>
       <c r="B300" s="9" t="s">
-        <v>827</v>
+        <v>620</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D300" s="9" t="s">
         <v>806</v>
       </c>
       <c r="E300" s="12">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F300" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G300" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H300" s="10"/>
       <c r="I300" s="10"/>
       <c r="J300" s="10"/>
       <c r="K300" s="10" t="s">
-        <v>801</v>
+        <v>630</v>
       </c>
       <c r="L300" s="10" t="s">
-        <v>833</v>
+        <v>635</v>
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.25">
@@ -13117,29 +13144,31 @@
         <v>4</v>
       </c>
       <c r="B301" s="9" t="s">
-        <v>389</v>
+        <v>903</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D301" s="9" t="s">
-        <v>813</v>
-      </c>
-      <c r="E301" s="12"/>
+        <v>806</v>
+      </c>
+      <c r="E301" s="12">
+        <v>100</v>
+      </c>
       <c r="F301" s="11" t="s">
-        <v>21</v>
+        <v>906</v>
       </c>
       <c r="G301" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H301" s="10"/>
       <c r="I301" s="10"/>
       <c r="J301" s="10"/>
       <c r="K301" s="10" t="s">
-        <v>390</v>
+        <v>905</v>
       </c>
       <c r="L301" s="10" t="s">
-        <v>390</v>
+        <v>904</v>
       </c>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.25">
@@ -13147,7 +13176,7 @@
         <v>4</v>
       </c>
       <c r="B302" s="9" t="s">
-        <v>856</v>
+        <v>828</v>
       </c>
       <c r="C302" s="9" t="s">
         <v>816</v>
@@ -13159,7 +13188,7 @@
         <v>0</v>
       </c>
       <c r="F302" s="11" t="s">
-        <v>56</v>
+        <v>308</v>
       </c>
       <c r="G302" s="11" t="b">
         <v>0</v>
@@ -13168,10 +13197,10 @@
       <c r="I302" s="10"/>
       <c r="J302" s="10"/>
       <c r="K302" s="10" t="s">
-        <v>859</v>
+        <v>831</v>
       </c>
       <c r="L302" s="10" t="s">
-        <v>859</v>
+        <v>832</v>
       </c>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.25">
@@ -13179,7 +13208,7 @@
         <v>4</v>
       </c>
       <c r="B303" s="9" t="s">
-        <v>861</v>
+        <v>827</v>
       </c>
       <c r="C303" s="9" t="s">
         <v>816</v>
@@ -13191,7 +13220,7 @@
         <v>0</v>
       </c>
       <c r="F303" s="11" t="s">
-        <v>56</v>
+        <v>308</v>
       </c>
       <c r="G303" s="11" t="b">
         <v>0</v>
@@ -13200,9 +13229,103 @@
       <c r="I303" s="10"/>
       <c r="J303" s="10"/>
       <c r="K303" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="L303" s="10" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A304" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B304" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C304" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D304" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="E304" s="12"/>
+      <c r="F304" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G304" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H304" s="10"/>
+      <c r="I304" s="10"/>
+      <c r="J304" s="10"/>
+      <c r="K304" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="L304" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A305" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B305" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="C305" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D305" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E305" s="12">
+        <v>0</v>
+      </c>
+      <c r="F305" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G305" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H305" s="10"/>
+      <c r="I305" s="10"/>
+      <c r="J305" s="10"/>
+      <c r="K305" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="L305" s="10" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A306" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B306" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="C306" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D306" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="E306" s="12">
+        <v>0</v>
+      </c>
+      <c r="F306" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G306" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H306" s="10"/>
+      <c r="I306" s="10"/>
+      <c r="J306" s="10"/>
+      <c r="K306" s="10" t="s">
         <v>860</v>
       </c>
-      <c r="L303" s="10" t="s">
+      <c r="L306" s="10" t="s">
         <v>860</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding interface components for user flux profiles
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC15772F-F37C-45BD-BADF-28C2661F38C9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B5D784-AF4D-4DFC-9BD2-D88A3798A3DD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="942">
   <si>
     <t>String name</t>
   </si>
@@ -2823,6 +2823,24 @@
   </si>
   <si>
     <t>Save field image (User)</t>
+  </si>
+  <si>
+    <t>Uniform=0;User=1</t>
+  </si>
+  <si>
+    <t>Desired receiver flux profile</t>
+  </si>
+  <si>
+    <t>Desired receiver flux profile type, Image Size Priority mode only</t>
+  </si>
+  <si>
+    <t>flux_profile_type</t>
+  </si>
+  <si>
+    <t>user_flux_profile</t>
+  </si>
+  <si>
+    <t>User flux profile data</t>
   </si>
 </sst>
 </file>
@@ -3061,10 +3079,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L306" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L306" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:L316">
-    <sortCondition ref="A1:A316"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L308" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L308" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L318">
+    <sortCondition ref="A1:A318"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain" dataDxfId="11"/>
@@ -3405,11 +3423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L306"/>
+  <dimension ref="A1:L308"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E231" sqref="E231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10861,16 +10879,16 @@
         <v>8</v>
       </c>
       <c r="B231" s="9" t="s">
-        <v>905</v>
+        <v>939</v>
       </c>
       <c r="C231" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E231" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F231" s="11" t="s">
         <v>21</v>
@@ -10878,14 +10896,18 @@
       <c r="G231" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H231" s="10"/>
-      <c r="I231" s="10"/>
+      <c r="H231" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I231" s="10" t="s">
+        <v>936</v>
+      </c>
       <c r="J231" s="10"/>
       <c r="K231" s="10" t="s">
-        <v>906</v>
+        <v>937</v>
       </c>
       <c r="L231" s="10" t="s">
-        <v>907</v>
+        <v>938</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
@@ -10893,31 +10915,29 @@
         <v>8</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>307</v>
+        <v>940</v>
       </c>
       <c r="C232" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E232" s="12">
-        <v>10.199999999999999</v>
-      </c>
+        <v>804</v>
+      </c>
+      <c r="E232" s="12"/>
       <c r="F232" s="11" t="s">
-        <v>567</v>
+        <v>21</v>
       </c>
       <c r="G232" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H232" s="10"/>
       <c r="I232" s="10"/>
       <c r="J232" s="10"/>
       <c r="K232" s="10" t="s">
-        <v>568</v>
+        <v>941</v>
       </c>
       <c r="L232" s="10" t="s">
-        <v>569</v>
+        <v>941</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
@@ -10925,7 +10945,7 @@
         <v>8</v>
       </c>
       <c r="B233" s="9" t="s">
-        <v>570</v>
+        <v>905</v>
       </c>
       <c r="C233" s="9" t="s">
         <v>814</v>
@@ -10934,10 +10954,10 @@
         <v>805</v>
       </c>
       <c r="E233" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F233" s="11" t="s">
-        <v>558</v>
+        <v>21</v>
       </c>
       <c r="G233" s="11" t="b">
         <v>1</v>
@@ -10946,10 +10966,10 @@
       <c r="I233" s="10"/>
       <c r="J233" s="10"/>
       <c r="K233" s="10" t="s">
-        <v>571</v>
+        <v>906</v>
       </c>
       <c r="L233" s="10" t="s">
-        <v>572</v>
+        <v>907</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
@@ -10957,7 +10977,7 @@
         <v>8</v>
       </c>
       <c r="B234" s="9" t="s">
-        <v>15</v>
+        <v>307</v>
       </c>
       <c r="C234" s="9" t="s">
         <v>814</v>
@@ -10966,10 +10986,10 @@
         <v>805</v>
       </c>
       <c r="E234" s="12">
-        <v>0</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F234" s="11" t="s">
-        <v>56</v>
+        <v>567</v>
       </c>
       <c r="G234" s="11" t="b">
         <v>1</v>
@@ -10977,11 +10997,11 @@
       <c r="H234" s="10"/>
       <c r="I234" s="10"/>
       <c r="J234" s="10"/>
-      <c r="K234" s="9" t="s">
-        <v>145</v>
+      <c r="K234" s="10" t="s">
+        <v>568</v>
       </c>
       <c r="L234" s="10" t="s">
-        <v>422</v>
+        <v>569</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
@@ -10989,7 +11009,7 @@
         <v>8</v>
       </c>
       <c r="B235" s="9" t="s">
-        <v>298</v>
+        <v>570</v>
       </c>
       <c r="C235" s="9" t="s">
         <v>814</v>
@@ -11001,21 +11021,19 @@
         <v>0</v>
       </c>
       <c r="F235" s="11" t="s">
-        <v>23</v>
+        <v>558</v>
       </c>
       <c r="G235" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H235" s="10"/>
       <c r="I235" s="10"/>
-      <c r="J235" s="10" t="s">
-        <v>640</v>
-      </c>
+      <c r="J235" s="10"/>
       <c r="K235" s="10" t="s">
-        <v>300</v>
+        <v>571</v>
       </c>
       <c r="L235" s="10" t="s">
-        <v>301</v>
+        <v>572</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
@@ -11023,7 +11041,7 @@
         <v>8</v>
       </c>
       <c r="B236" s="9" t="s">
-        <v>297</v>
+        <v>15</v>
       </c>
       <c r="C236" s="9" t="s">
         <v>814</v>
@@ -11032,24 +11050,22 @@
         <v>805</v>
       </c>
       <c r="E236" s="12">
-        <v>7.75</v>
+        <v>0</v>
       </c>
       <c r="F236" s="11" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G236" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H236" s="10"/>
       <c r="I236" s="10"/>
-      <c r="J236" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="K236" s="10" t="s">
-        <v>299</v>
+      <c r="J236" s="10"/>
+      <c r="K236" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="L236" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
@@ -11057,7 +11073,7 @@
         <v>8</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>11</v>
+        <v>298</v>
       </c>
       <c r="C237" s="9" t="s">
         <v>814</v>
@@ -11066,7 +11082,7 @@
         <v>805</v>
       </c>
       <c r="E237" s="12">
-        <v>17.649999999999999</v>
+        <v>0</v>
       </c>
       <c r="F237" s="11" t="s">
         <v>23</v>
@@ -11076,12 +11092,14 @@
       </c>
       <c r="H237" s="10"/>
       <c r="I237" s="10"/>
-      <c r="J237" s="10"/>
-      <c r="K237" s="9" t="s">
-        <v>119</v>
+      <c r="J237" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K237" s="10" t="s">
+        <v>300</v>
       </c>
       <c r="L237" s="10" t="s">
-        <v>142</v>
+        <v>301</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.25">
@@ -11089,7 +11107,7 @@
         <v>8</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>431</v>
+        <v>297</v>
       </c>
       <c r="C238" s="9" t="s">
         <v>814</v>
@@ -11098,22 +11116,24 @@
         <v>805</v>
       </c>
       <c r="E238" s="12">
-        <v>0</v>
+        <v>7.75</v>
       </c>
       <c r="F238" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G238" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H238" s="10"/>
       <c r="I238" s="10"/>
-      <c r="J238" s="10"/>
-      <c r="K238" s="9" t="s">
-        <v>429</v>
+      <c r="J238" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K238" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="L238" s="10" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
@@ -11121,7 +11141,7 @@
         <v>8</v>
       </c>
       <c r="B239" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C239" s="9" t="s">
         <v>814</v>
@@ -11130,7 +11150,7 @@
         <v>805</v>
       </c>
       <c r="E239" s="12">
-        <v>21.6</v>
+        <v>17.649999999999999</v>
       </c>
       <c r="F239" s="11" t="s">
         <v>23</v>
@@ -11142,10 +11162,10 @@
       <c r="I239" s="10"/>
       <c r="J239" s="10"/>
       <c r="K239" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L239" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
@@ -11153,29 +11173,31 @@
         <v>8</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>313</v>
+        <v>431</v>
       </c>
       <c r="C240" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E240" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="F240" s="11"/>
+        <v>805</v>
+      </c>
+      <c r="E240" s="12">
+        <v>0</v>
+      </c>
+      <c r="F240" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="G240" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H240" s="10"/>
       <c r="I240" s="10"/>
       <c r="J240" s="10"/>
-      <c r="K240" s="10" t="s">
-        <v>315</v>
+      <c r="K240" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="L240" s="10" t="s">
-        <v>315</v>
+        <v>430</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
@@ -11183,7 +11205,7 @@
         <v>8</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C241" s="9" t="s">
         <v>814</v>
@@ -11192,7 +11214,7 @@
         <v>805</v>
       </c>
       <c r="E241" s="12">
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="F241" s="11" t="s">
         <v>23</v>
@@ -11204,10 +11226,10 @@
       <c r="I241" s="10"/>
       <c r="J241" s="10"/>
       <c r="K241" s="9" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="L241" s="10" t="s">
-        <v>929</v>
+        <v>143</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
@@ -11215,31 +11237,29 @@
         <v>8</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>17</v>
+        <v>313</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E242" s="12">
-        <v>0</v>
-      </c>
-      <c r="F242" s="11" t="s">
-        <v>23</v>
-      </c>
+        <v>804</v>
+      </c>
+      <c r="E242" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="F242" s="11"/>
       <c r="G242" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H242" s="10"/>
       <c r="I242" s="10"/>
       <c r="J242" s="10"/>
-      <c r="K242" s="9" t="s">
-        <v>147</v>
+      <c r="K242" s="10" t="s">
+        <v>315</v>
       </c>
       <c r="L242" s="10" t="s">
-        <v>930</v>
+        <v>315</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
@@ -11247,7 +11267,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>302</v>
+        <v>16</v>
       </c>
       <c r="C243" s="9" t="s">
         <v>814</v>
@@ -11268,10 +11288,10 @@
       <c r="I243" s="10"/>
       <c r="J243" s="10"/>
       <c r="K243" s="9" t="s">
-        <v>303</v>
+        <v>146</v>
       </c>
       <c r="L243" s="10" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
@@ -11279,35 +11299,31 @@
         <v>8</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>914</v>
+        <v>17</v>
       </c>
       <c r="C244" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E244" s="12">
         <v>0</v>
       </c>
       <c r="F244" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G244" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H244" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I244" s="10" t="s">
-        <v>932</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H244" s="10"/>
+      <c r="I244" s="10"/>
       <c r="J244" s="10"/>
-      <c r="K244" s="10" t="s">
-        <v>915</v>
+      <c r="K244" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="L244" s="10" t="s">
-        <v>916</v>
+        <v>930</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
@@ -11315,35 +11331,31 @@
         <v>8</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>20</v>
+        <v>302</v>
       </c>
       <c r="C245" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E245" s="12">
         <v>0</v>
       </c>
       <c r="F245" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G245" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H245" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I245" s="10" t="s">
-        <v>770</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H245" s="10"/>
+      <c r="I245" s="10"/>
       <c r="J245" s="10"/>
       <c r="K245" s="9" t="s">
-        <v>24</v>
+        <v>303</v>
       </c>
       <c r="L245" s="10" t="s">
-        <v>150</v>
+        <v>931</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
@@ -11351,31 +11363,35 @@
         <v>8</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>10</v>
+        <v>914</v>
       </c>
       <c r="C246" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E246" s="12">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F246" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G246" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H246" s="10"/>
-      <c r="I246" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H246" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I246" s="10" t="s">
+        <v>932</v>
+      </c>
       <c r="J246" s="10"/>
-      <c r="K246" s="9" t="s">
-        <v>118</v>
+      <c r="K246" s="10" t="s">
+        <v>915</v>
       </c>
       <c r="L246" s="10" t="s">
-        <v>141</v>
+        <v>916</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
@@ -11383,33 +11399,35 @@
         <v>8</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>417</v>
+        <v>20</v>
       </c>
       <c r="C247" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D247" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E247" s="12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F247" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G247" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H247" s="10"/>
-      <c r="I247" s="10"/>
-      <c r="J247" s="10" t="s">
-        <v>640</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H247" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I247" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="J247" s="10"/>
       <c r="K247" s="9" t="s">
-        <v>420</v>
+        <v>24</v>
       </c>
       <c r="L247" s="10" t="s">
-        <v>421</v>
+        <v>150</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
@@ -11417,7 +11435,7 @@
         <v>8</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>416</v>
+        <v>10</v>
       </c>
       <c r="C248" s="9" t="s">
         <v>814</v>
@@ -11426,24 +11444,22 @@
         <v>805</v>
       </c>
       <c r="E248" s="12">
-        <v>-180</v>
+        <v>17</v>
       </c>
       <c r="F248" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G248" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H248" s="10"/>
       <c r="I248" s="10"/>
-      <c r="J248" s="10" t="s">
-        <v>640</v>
-      </c>
+      <c r="J248" s="10"/>
       <c r="K248" s="9" t="s">
-        <v>418</v>
+        <v>118</v>
       </c>
       <c r="L248" s="10" t="s">
-        <v>419</v>
+        <v>141</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
@@ -11451,7 +11467,7 @@
         <v>8</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>561</v>
+        <v>417</v>
       </c>
       <c r="C249" s="9" t="s">
         <v>814</v>
@@ -11460,22 +11476,24 @@
         <v>805</v>
       </c>
       <c r="E249" s="12">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="F249" s="11" t="s">
-        <v>291</v>
+        <v>56</v>
       </c>
       <c r="G249" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H249" s="10"/>
       <c r="I249" s="10"/>
-      <c r="J249" s="10"/>
-      <c r="K249" s="10" t="s">
-        <v>562</v>
+      <c r="J249" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K249" s="9" t="s">
+        <v>420</v>
       </c>
       <c r="L249" s="10" t="s">
-        <v>563</v>
+        <v>421</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
@@ -11483,31 +11501,33 @@
         <v>8</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>564</v>
+        <v>416</v>
       </c>
       <c r="C250" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>802</v>
-      </c>
-      <c r="E250" s="10" t="s">
-        <v>309</v>
+        <v>805</v>
+      </c>
+      <c r="E250" s="12">
+        <v>-180</v>
       </c>
       <c r="F250" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G250" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H250" s="10"/>
       <c r="I250" s="10"/>
-      <c r="J250" s="10"/>
-      <c r="K250" s="10" t="s">
-        <v>565</v>
+      <c r="J250" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="K250" s="9" t="s">
+        <v>418</v>
       </c>
       <c r="L250" s="10" t="s">
-        <v>305</v>
+        <v>419</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
@@ -11515,31 +11535,31 @@
         <v>8</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>304</v>
+        <v>561</v>
       </c>
       <c r="C251" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>802</v>
-      </c>
-      <c r="E251" s="10" t="s">
-        <v>309</v>
+        <v>805</v>
+      </c>
+      <c r="E251" s="12">
+        <v>30</v>
       </c>
       <c r="F251" s="11" t="s">
-        <v>21</v>
+        <v>291</v>
       </c>
       <c r="G251" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H251" s="10"/>
       <c r="I251" s="10"/>
       <c r="J251" s="10"/>
       <c r="K251" s="10" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="L251" s="10" t="s">
-        <v>306</v>
+        <v>563</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
@@ -11547,19 +11567,19 @@
         <v>8</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>310</v>
+        <v>564</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E252" s="12">
-        <v>0</v>
+        <v>802</v>
+      </c>
+      <c r="E252" s="10" t="s">
+        <v>309</v>
       </c>
       <c r="F252" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G252" s="11" t="b">
         <v>0</v>
@@ -11568,10 +11588,10 @@
       <c r="I252" s="10"/>
       <c r="J252" s="10"/>
       <c r="K252" s="10" t="s">
-        <v>311</v>
+        <v>565</v>
       </c>
       <c r="L252" s="10" t="s">
-        <v>424</v>
+        <v>305</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
@@ -11579,19 +11599,19 @@
         <v>8</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>25</v>
+        <v>304</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E253" s="12">
-        <v>195</v>
+        <v>802</v>
+      </c>
+      <c r="E253" s="10" t="s">
+        <v>309</v>
       </c>
       <c r="F253" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G253" s="11" t="b">
         <v>0</v>
@@ -11599,11 +11619,11 @@
       <c r="H253" s="10"/>
       <c r="I253" s="10"/>
       <c r="J253" s="10"/>
-      <c r="K253" s="9" t="s">
-        <v>140</v>
+      <c r="K253" s="10" t="s">
+        <v>566</v>
       </c>
       <c r="L253" s="10" t="s">
-        <v>425</v>
+        <v>306</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
@@ -11611,7 +11631,7 @@
         <v>8</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>577</v>
+        <v>310</v>
       </c>
       <c r="C254" s="9" t="s">
         <v>815</v>
@@ -11623,7 +11643,7 @@
         <v>0</v>
       </c>
       <c r="F254" s="11" t="s">
-        <v>574</v>
+        <v>308</v>
       </c>
       <c r="G254" s="11" t="b">
         <v>0</v>
@@ -11632,10 +11652,10 @@
       <c r="I254" s="10"/>
       <c r="J254" s="10"/>
       <c r="K254" s="10" t="s">
-        <v>578</v>
+        <v>311</v>
       </c>
       <c r="L254" s="10" t="s">
-        <v>579</v>
+        <v>424</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">
@@ -11643,7 +11663,7 @@
         <v>8</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>294</v>
+        <v>25</v>
       </c>
       <c r="C255" s="9" t="s">
         <v>815</v>
@@ -11652,22 +11672,22 @@
         <v>805</v>
       </c>
       <c r="E255" s="12">
-        <v>1.2</v>
+        <v>195</v>
       </c>
       <c r="F255" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G255" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H255" s="10"/>
       <c r="I255" s="10"/>
       <c r="J255" s="10"/>
-      <c r="K255" s="10" t="s">
-        <v>295</v>
+      <c r="K255" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="L255" s="10" t="s">
-        <v>296</v>
+        <v>425</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
@@ -11675,7 +11695,7 @@
         <v>8</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>823</v>
+        <v>577</v>
       </c>
       <c r="C256" s="9" t="s">
         <v>815</v>
@@ -11687,7 +11707,7 @@
         <v>0</v>
       </c>
       <c r="F256" s="11" t="s">
-        <v>21</v>
+        <v>574</v>
       </c>
       <c r="G256" s="11" t="b">
         <v>0</v>
@@ -11696,10 +11716,10 @@
       <c r="I256" s="10"/>
       <c r="J256" s="10"/>
       <c r="K256" s="10" t="s">
-        <v>824</v>
+        <v>578</v>
       </c>
       <c r="L256" s="10" t="s">
-        <v>824</v>
+        <v>579</v>
       </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
@@ -11707,7 +11727,7 @@
         <v>8</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>573</v>
+        <v>294</v>
       </c>
       <c r="C257" s="9" t="s">
         <v>815</v>
@@ -11716,22 +11736,22 @@
         <v>805</v>
       </c>
       <c r="E257" s="12">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F257" s="11" t="s">
-        <v>574</v>
+        <v>21</v>
       </c>
       <c r="G257" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H257" s="10"/>
       <c r="I257" s="10"/>
       <c r="J257" s="10"/>
       <c r="K257" s="10" t="s">
-        <v>575</v>
+        <v>295</v>
       </c>
       <c r="L257" s="10" t="s">
-        <v>576</v>
+        <v>296</v>
       </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
@@ -11739,7 +11759,7 @@
         <v>8</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>911</v>
+        <v>823</v>
       </c>
       <c r="C258" s="9" t="s">
         <v>815</v>
@@ -11751,7 +11771,7 @@
         <v>0</v>
       </c>
       <c r="F258" s="11" t="s">
-        <v>574</v>
+        <v>21</v>
       </c>
       <c r="G258" s="11" t="b">
         <v>0</v>
@@ -11760,10 +11780,10 @@
       <c r="I258" s="10"/>
       <c r="J258" s="10"/>
       <c r="K258" s="10" t="s">
-        <v>912</v>
+        <v>824</v>
       </c>
       <c r="L258" s="10" t="s">
-        <v>913</v>
+        <v>824</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
@@ -11771,7 +11791,7 @@
         <v>8</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>924</v>
+        <v>573</v>
       </c>
       <c r="C259" s="9" t="s">
         <v>815</v>
@@ -11783,7 +11803,7 @@
         <v>0</v>
       </c>
       <c r="F259" s="11" t="s">
-        <v>23</v>
+        <v>574</v>
       </c>
       <c r="G259" s="11" t="b">
         <v>0</v>
@@ -11791,11 +11811,11 @@
       <c r="H259" s="10"/>
       <c r="I259" s="10"/>
       <c r="J259" s="10"/>
-      <c r="K259" s="9" t="s">
-        <v>926</v>
+      <c r="K259" s="10" t="s">
+        <v>575</v>
       </c>
       <c r="L259" s="10" t="s">
-        <v>148</v>
+        <v>576</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
@@ -11803,7 +11823,7 @@
         <v>8</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>923</v>
+        <v>911</v>
       </c>
       <c r="C260" s="9" t="s">
         <v>815</v>
@@ -11815,7 +11835,7 @@
         <v>0</v>
       </c>
       <c r="F260" s="11" t="s">
-        <v>23</v>
+        <v>574</v>
       </c>
       <c r="G260" s="11" t="b">
         <v>0</v>
@@ -11823,11 +11843,11 @@
       <c r="H260" s="10"/>
       <c r="I260" s="10"/>
       <c r="J260" s="10"/>
-      <c r="K260" s="9" t="s">
-        <v>927</v>
+      <c r="K260" s="10" t="s">
+        <v>912</v>
       </c>
       <c r="L260" s="10" t="s">
-        <v>149</v>
+        <v>913</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
@@ -11835,7 +11855,7 @@
         <v>8</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C261" s="9" t="s">
         <v>815</v>
@@ -11856,74 +11876,74 @@
       <c r="I261" s="10"/>
       <c r="J261" s="10"/>
       <c r="K261" s="9" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="L261" s="10" t="s">
-        <v>426</v>
+        <v>148</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>19</v>
+        <v>923</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>805</v>
       </c>
       <c r="E262" s="12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F262" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G262" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H262" s="10"/>
       <c r="I262" s="10"/>
       <c r="J262" s="10"/>
-      <c r="K262" s="10" t="s">
-        <v>138</v>
+      <c r="K262" s="9" t="s">
+        <v>927</v>
       </c>
       <c r="L262" s="10" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>18</v>
+        <v>925</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>805</v>
       </c>
       <c r="E263" s="12">
-        <v>-180</v>
+        <v>0</v>
       </c>
       <c r="F263" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G263" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H263" s="10"/>
       <c r="I263" s="10"/>
       <c r="J263" s="10"/>
-      <c r="K263" s="10" t="s">
-        <v>139</v>
+      <c r="K263" s="9" t="s">
+        <v>928</v>
       </c>
       <c r="L263" s="10" t="s">
-        <v>111</v>
+        <v>426</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
@@ -11931,7 +11951,7 @@
         <v>4</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="C264" s="9" t="s">
         <v>814</v>
@@ -11940,10 +11960,10 @@
         <v>805</v>
       </c>
       <c r="E264" s="12">
-        <v>2</v>
+        <v>180</v>
       </c>
       <c r="F264" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G264" s="11" t="b">
         <v>1</v>
@@ -11951,11 +11971,11 @@
       <c r="H264" s="10"/>
       <c r="I264" s="10"/>
       <c r="J264" s="10"/>
-      <c r="K264" s="9" t="s">
-        <v>127</v>
+      <c r="K264" s="10" t="s">
+        <v>138</v>
       </c>
       <c r="L264" s="10" t="s">
-        <v>213</v>
+        <v>110</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
@@ -11963,31 +11983,31 @@
         <v>4</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>545</v>
+        <v>18</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D265" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E265" s="12" t="s">
-        <v>546</v>
+        <v>805</v>
+      </c>
+      <c r="E265" s="12">
+        <v>-180</v>
       </c>
       <c r="F265" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G265" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H265" s="10"/>
       <c r="I265" s="10"/>
       <c r="J265" s="10"/>
       <c r="K265" s="10" t="s">
-        <v>547</v>
+        <v>139</v>
       </c>
       <c r="L265" s="10" t="s">
-        <v>547</v>
+        <v>111</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
@@ -11995,16 +12015,16 @@
         <v>4</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D266" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E266" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F266" s="11" t="s">
         <v>21</v>
@@ -12012,18 +12032,14 @@
       <c r="G266" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H266" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I266" s="10" t="s">
-        <v>556</v>
-      </c>
+      <c r="H266" s="10"/>
+      <c r="I266" s="10"/>
       <c r="J266" s="10"/>
       <c r="K266" s="9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L266" s="10" t="s">
-        <v>105</v>
+        <v>213</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
@@ -12031,31 +12047,31 @@
         <v>4</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>192</v>
+        <v>545</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>803</v>
-      </c>
-      <c r="E267" s="12">
-        <v>4</v>
+        <v>804</v>
+      </c>
+      <c r="E267" s="12" t="s">
+        <v>546</v>
       </c>
       <c r="F267" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G267" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H267" s="10"/>
       <c r="I267" s="10"/>
       <c r="J267" s="10"/>
       <c r="K267" s="10" t="s">
-        <v>193</v>
+        <v>547</v>
       </c>
       <c r="L267" s="10" t="s">
-        <v>194</v>
+        <v>547</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
@@ -12063,16 +12079,16 @@
         <v>4</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>582</v>
+        <v>104</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E268" s="12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F268" s="11" t="s">
         <v>21</v>
@@ -12080,14 +12096,18 @@
       <c r="G268" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H268" s="10"/>
-      <c r="I268" s="10"/>
+      <c r="H268" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I268" s="10" t="s">
+        <v>556</v>
+      </c>
       <c r="J268" s="10"/>
-      <c r="K268" s="10" t="s">
-        <v>583</v>
+      <c r="K268" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="L268" s="10" t="s">
-        <v>584</v>
+        <v>105</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
@@ -12095,19 +12115,19 @@
         <v>4</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C269" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E269" s="12">
-        <v>950</v>
+        <v>4</v>
       </c>
       <c r="F269" s="11" t="s">
-        <v>189</v>
+        <v>21</v>
       </c>
       <c r="G269" s="11" t="b">
         <v>1</v>
@@ -12116,10 +12136,10 @@
       <c r="I269" s="10"/>
       <c r="J269" s="10"/>
       <c r="K269" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L269" s="10" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
@@ -12127,16 +12147,16 @@
         <v>4</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>521</v>
+        <v>582</v>
       </c>
       <c r="C270" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E270" s="12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F270" s="11" t="s">
         <v>21</v>
@@ -12144,18 +12164,14 @@
       <c r="G270" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H270" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I270" s="10" t="s">
-        <v>523</v>
-      </c>
+      <c r="H270" s="10"/>
+      <c r="I270" s="10"/>
       <c r="J270" s="10"/>
       <c r="K270" s="10" t="s">
-        <v>555</v>
+        <v>583</v>
       </c>
       <c r="L270" s="10" t="s">
-        <v>522</v>
+        <v>584</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
@@ -12163,33 +12179,31 @@
         <v>4</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>889</v>
+        <v>188</v>
       </c>
       <c r="C271" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E271" s="12" t="b">
-        <v>0</v>
+        <v>805</v>
+      </c>
+      <c r="E271" s="12">
+        <v>950</v>
       </c>
       <c r="F271" s="11" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="G271" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H271" s="10" t="s">
-        <v>202</v>
-      </c>
+      <c r="H271" s="10"/>
       <c r="I271" s="10"/>
       <c r="J271" s="10"/>
       <c r="K271" s="10" t="s">
-        <v>890</v>
+        <v>190</v>
       </c>
       <c r="L271" s="10" t="s">
-        <v>891</v>
+        <v>191</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
@@ -12197,33 +12211,35 @@
         <v>4</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>636</v>
+        <v>521</v>
       </c>
       <c r="C272" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E272" s="12" t="b">
-        <v>1</v>
+        <v>804</v>
+      </c>
+      <c r="E272" s="12">
+        <v>7</v>
       </c>
       <c r="F272" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G272" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H272" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="I272" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="I272" s="10" t="s">
+        <v>523</v>
+      </c>
       <c r="J272" s="10"/>
       <c r="K272" s="10" t="s">
-        <v>637</v>
+        <v>555</v>
       </c>
       <c r="L272" s="10" t="s">
-        <v>638</v>
+        <v>522</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
@@ -12231,7 +12247,7 @@
         <v>4</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>612</v>
+        <v>889</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>814</v>
@@ -12254,10 +12270,10 @@
       <c r="I273" s="10"/>
       <c r="J273" s="10"/>
       <c r="K273" s="10" t="s">
-        <v>610</v>
+        <v>890</v>
       </c>
       <c r="L273" s="10" t="s">
-        <v>611</v>
+        <v>891</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
@@ -12265,7 +12281,7 @@
         <v>4</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>209</v>
+        <v>636</v>
       </c>
       <c r="C274" s="9" t="s">
         <v>814</v>
@@ -12288,10 +12304,10 @@
       <c r="I274" s="10"/>
       <c r="J274" s="10"/>
       <c r="K274" s="10" t="s">
-        <v>210</v>
+        <v>637</v>
       </c>
       <c r="L274" s="10" t="s">
-        <v>211</v>
+        <v>638</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">
@@ -12299,7 +12315,7 @@
         <v>4</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>908</v>
+        <v>612</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>814</v>
@@ -12322,10 +12338,10 @@
       <c r="I275" s="10"/>
       <c r="J275" s="10"/>
       <c r="K275" s="10" t="s">
-        <v>909</v>
+        <v>610</v>
       </c>
       <c r="L275" s="10" t="s">
-        <v>910</v>
+        <v>611</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
@@ -12333,27 +12349,33 @@
         <v>4</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>387</v>
+        <v>209</v>
       </c>
       <c r="C276" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D276" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E276" s="12"/>
-      <c r="F276" s="11"/>
+        <v>806</v>
+      </c>
+      <c r="E276" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F276" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G276" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H276" s="10"/>
+      <c r="H276" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I276" s="10"/>
       <c r="J276" s="10"/>
       <c r="K276" s="10" t="s">
-        <v>388</v>
+        <v>210</v>
       </c>
       <c r="L276" s="10" t="s">
-        <v>388</v>
+        <v>211</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
@@ -12361,35 +12383,33 @@
         <v>4</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>6</v>
+        <v>908</v>
       </c>
       <c r="C277" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E277" s="12">
+        <v>806</v>
+      </c>
+      <c r="E277" s="12" t="b">
         <v>0</v>
       </c>
       <c r="F277" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G277" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H277" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I277" s="10" t="s">
-        <v>132</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="I277" s="10"/>
       <c r="J277" s="10"/>
-      <c r="K277" s="9" t="s">
-        <v>133</v>
+      <c r="K277" s="10" t="s">
+        <v>909</v>
       </c>
       <c r="L277" s="10" t="s">
-        <v>65</v>
+        <v>910</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
@@ -12397,31 +12417,27 @@
         <v>4</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>623</v>
+        <v>387</v>
       </c>
       <c r="C278" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D278" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E278" s="12">
-        <v>1</v>
-      </c>
-      <c r="F278" s="11" t="s">
-        <v>625</v>
-      </c>
+        <v>804</v>
+      </c>
+      <c r="E278" s="12"/>
+      <c r="F278" s="11"/>
       <c r="G278" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H278" s="10"/>
       <c r="I278" s="10"/>
       <c r="J278" s="10"/>
       <c r="K278" s="10" t="s">
-        <v>627</v>
+        <v>388</v>
       </c>
       <c r="L278" s="10" t="s">
-        <v>632</v>
+        <v>388</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
@@ -12429,31 +12445,35 @@
         <v>4</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>621</v>
+        <v>6</v>
       </c>
       <c r="C279" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D279" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E279" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F279" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G279" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H279" s="10"/>
-      <c r="I279" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H279" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I279" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="J279" s="10"/>
-      <c r="K279" s="10" t="s">
-        <v>626</v>
+      <c r="K279" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="L279" s="10" t="s">
-        <v>631</v>
+        <v>65</v>
       </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.25">
@@ -12461,7 +12481,7 @@
         <v>4</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>814</v>
@@ -12470,7 +12490,7 @@
         <v>805</v>
       </c>
       <c r="E280" s="12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F280" s="11" t="s">
         <v>625</v>
@@ -12482,10 +12502,10 @@
       <c r="I280" s="10"/>
       <c r="J280" s="10"/>
       <c r="K280" s="10" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L280" s="10" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">
@@ -12493,7 +12513,7 @@
         <v>4</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C281" s="9" t="s">
         <v>814</v>
@@ -12502,7 +12522,7 @@
         <v>805</v>
       </c>
       <c r="E281" s="12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F281" s="11" t="s">
         <v>625</v>
@@ -12514,10 +12534,10 @@
       <c r="I281" s="10"/>
       <c r="J281" s="10"/>
       <c r="K281" s="10" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="L281" s="10" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.25">
@@ -12525,7 +12545,7 @@
         <v>4</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>613</v>
+        <v>624</v>
       </c>
       <c r="C282" s="9" t="s">
         <v>814</v>
@@ -12534,10 +12554,10 @@
         <v>805</v>
       </c>
       <c r="E282" s="12">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F282" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G282" s="11" t="b">
         <v>1</v>
@@ -12546,10 +12566,10 @@
       <c r="I282" s="10"/>
       <c r="J282" s="10"/>
       <c r="K282" s="10" t="s">
-        <v>614</v>
+        <v>629</v>
       </c>
       <c r="L282" s="10" t="s">
-        <v>615</v>
+        <v>634</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.25">
@@ -12557,7 +12577,7 @@
         <v>4</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>5</v>
+        <v>622</v>
       </c>
       <c r="C283" s="9" t="s">
         <v>814</v>
@@ -12566,10 +12586,10 @@
         <v>805</v>
       </c>
       <c r="E283" s="12">
-        <v>670</v>
+        <v>0.1</v>
       </c>
       <c r="F283" s="11" t="s">
-        <v>212</v>
+        <v>625</v>
       </c>
       <c r="G283" s="11" t="b">
         <v>1</v>
@@ -12577,11 +12597,11 @@
       <c r="H283" s="10"/>
       <c r="I283" s="10"/>
       <c r="J283" s="10"/>
-      <c r="K283" s="9" t="s">
-        <v>126</v>
+      <c r="K283" s="10" t="s">
+        <v>628</v>
       </c>
       <c r="L283" s="10" t="s">
-        <v>64</v>
+        <v>633</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.25">
@@ -12589,16 +12609,16 @@
         <v>4</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>100</v>
+        <v>613</v>
       </c>
       <c r="C284" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D284" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E284" s="12">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F284" s="11" t="s">
         <v>21</v>
@@ -12606,18 +12626,14 @@
       <c r="G284" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H284" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I284" s="10" t="s">
-        <v>785</v>
-      </c>
+      <c r="H284" s="10"/>
+      <c r="I284" s="10"/>
       <c r="J284" s="10"/>
-      <c r="K284" s="9" t="s">
-        <v>134</v>
+      <c r="K284" s="10" t="s">
+        <v>614</v>
       </c>
       <c r="L284" s="10" t="s">
-        <v>101</v>
+        <v>615</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.25">
@@ -12625,7 +12641,7 @@
         <v>4</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>531</v>
+        <v>5</v>
       </c>
       <c r="C285" s="9" t="s">
         <v>814</v>
@@ -12634,10 +12650,10 @@
         <v>805</v>
       </c>
       <c r="E285" s="12">
-        <v>1.1000000000000001</v>
+        <v>670</v>
       </c>
       <c r="F285" s="11" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="G285" s="11" t="b">
         <v>1</v>
@@ -12645,11 +12661,11 @@
       <c r="H285" s="10"/>
       <c r="I285" s="10"/>
       <c r="J285" s="10"/>
-      <c r="K285" s="10" t="s">
-        <v>535</v>
+      <c r="K285" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="L285" s="10" t="s">
-        <v>538</v>
+        <v>64</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
@@ -12657,16 +12673,16 @@
         <v>4</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>532</v>
+        <v>100</v>
       </c>
       <c r="C286" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E286" s="12">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F286" s="11" t="s">
         <v>21</v>
@@ -12674,14 +12690,18 @@
       <c r="G286" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H286" s="10"/>
-      <c r="I286" s="10"/>
+      <c r="H286" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I286" s="10" t="s">
+        <v>785</v>
+      </c>
       <c r="J286" s="10"/>
-      <c r="K286" s="10" t="s">
-        <v>536</v>
+      <c r="K286" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="L286" s="10" t="s">
-        <v>539</v>
+        <v>101</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
@@ -12689,7 +12709,7 @@
         <v>4</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>14</v>
+        <v>531</v>
       </c>
       <c r="C287" s="9" t="s">
         <v>814</v>
@@ -12698,22 +12718,22 @@
         <v>805</v>
       </c>
       <c r="E287" s="12">
-        <v>195</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F287" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G287" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H287" s="10"/>
       <c r="I287" s="10"/>
       <c r="J287" s="10"/>
-      <c r="K287" s="9" t="s">
-        <v>137</v>
+      <c r="K287" s="10" t="s">
+        <v>535</v>
       </c>
       <c r="L287" s="10" t="s">
-        <v>68</v>
+        <v>538</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
@@ -12721,7 +12741,7 @@
         <v>4</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>13</v>
+        <v>532</v>
       </c>
       <c r="C288" s="9" t="s">
         <v>814</v>
@@ -12730,22 +12750,22 @@
         <v>805</v>
       </c>
       <c r="E288" s="12">
-        <v>16</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F288" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G288" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H288" s="10"/>
       <c r="I288" s="10"/>
       <c r="J288" s="10"/>
-      <c r="K288" s="9" t="s">
-        <v>136</v>
+      <c r="K288" s="10" t="s">
+        <v>536</v>
       </c>
       <c r="L288" s="10" t="s">
-        <v>67</v>
+        <v>539</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -12753,7 +12773,7 @@
         <v>4</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>892</v>
+        <v>14</v>
       </c>
       <c r="C289" s="9" t="s">
         <v>814</v>
@@ -12762,22 +12782,22 @@
         <v>805</v>
       </c>
       <c r="E289" s="12">
-        <v>0.5</v>
+        <v>195</v>
       </c>
       <c r="F289" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G289" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H289" s="10"/>
       <c r="I289" s="10"/>
       <c r="J289" s="10"/>
-      <c r="K289" s="10" t="s">
-        <v>893</v>
+      <c r="K289" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="L289" s="10" t="s">
-        <v>893</v>
+        <v>68</v>
       </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
@@ -12785,7 +12805,7 @@
         <v>4</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C290" s="9" t="s">
         <v>814</v>
@@ -12794,22 +12814,22 @@
         <v>805</v>
       </c>
       <c r="E290" s="12">
-        <v>1.33</v>
+        <v>16</v>
       </c>
       <c r="F290" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G290" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H290" s="10"/>
       <c r="I290" s="10"/>
       <c r="J290" s="10"/>
       <c r="K290" s="9" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="L290" s="10" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
@@ -12817,7 +12837,7 @@
         <v>4</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>853</v>
+        <v>892</v>
       </c>
       <c r="C291" s="9" t="s">
         <v>814</v>
@@ -12826,10 +12846,10 @@
         <v>805</v>
       </c>
       <c r="E291" s="12">
-        <v>180</v>
+        <v>0.5</v>
       </c>
       <c r="F291" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G291" s="11" t="b">
         <v>1</v>
@@ -12838,10 +12858,10 @@
       <c r="I291" s="10"/>
       <c r="J291" s="10"/>
       <c r="K291" s="10" t="s">
-        <v>856</v>
+        <v>893</v>
       </c>
       <c r="L291" s="10" t="s">
-        <v>500</v>
+        <v>893</v>
       </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
@@ -12849,7 +12869,7 @@
         <v>4</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>854</v>
+        <v>97</v>
       </c>
       <c r="C292" s="9" t="s">
         <v>814</v>
@@ -12858,10 +12878,10 @@
         <v>805</v>
       </c>
       <c r="E292" s="12">
-        <v>85</v>
+        <v>1.33</v>
       </c>
       <c r="F292" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G292" s="11" t="b">
         <v>1</v>
@@ -12869,11 +12889,11 @@
       <c r="H292" s="10"/>
       <c r="I292" s="10"/>
       <c r="J292" s="10"/>
-      <c r="K292" s="10" t="s">
-        <v>857</v>
+      <c r="K292" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="L292" s="10" t="s">
-        <v>501</v>
+        <v>98</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
@@ -12881,35 +12901,31 @@
         <v>4</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>497</v>
+        <v>853</v>
       </c>
       <c r="C293" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D293" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E293" s="12">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F293" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G293" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H293" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I293" s="10" t="s">
-        <v>520</v>
-      </c>
+      <c r="H293" s="10"/>
+      <c r="I293" s="10"/>
       <c r="J293" s="10"/>
       <c r="K293" s="10" t="s">
-        <v>498</v>
+        <v>856</v>
       </c>
       <c r="L293" s="10" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
@@ -12917,33 +12933,31 @@
         <v>4</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>773</v>
+        <v>854</v>
       </c>
       <c r="C294" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E294" s="12">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F294" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G294" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H294" s="10" t="s">
-        <v>131</v>
-      </c>
+      <c r="H294" s="10"/>
       <c r="I294" s="10"/>
       <c r="J294" s="10"/>
       <c r="K294" s="10" t="s">
-        <v>774</v>
+        <v>857</v>
       </c>
       <c r="L294" s="10" t="s">
-        <v>775</v>
+        <v>501</v>
       </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
@@ -12951,7 +12965,7 @@
         <v>4</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>269</v>
+        <v>497</v>
       </c>
       <c r="C295" s="9" t="s">
         <v>814</v>
@@ -12962,7 +12976,9 @@
       <c r="E295" s="12">
         <v>0</v>
       </c>
-      <c r="F295" s="11"/>
+      <c r="F295" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G295" s="11" t="b">
         <v>1</v>
       </c>
@@ -12970,14 +12986,14 @@
         <v>131</v>
       </c>
       <c r="I295" s="10" t="s">
-        <v>271</v>
+        <v>520</v>
       </c>
       <c r="J295" s="10"/>
       <c r="K295" s="10" t="s">
-        <v>270</v>
+        <v>498</v>
       </c>
       <c r="L295" s="10" t="s">
-        <v>284</v>
+        <v>499</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
@@ -12985,31 +13001,33 @@
         <v>4</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>9</v>
+        <v>773</v>
       </c>
       <c r="C296" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D296" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E296" s="12">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="F296" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G296" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H296" s="10"/>
+      <c r="H296" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="I296" s="10"/>
       <c r="J296" s="10"/>
-      <c r="K296" s="9" t="s">
-        <v>285</v>
+      <c r="K296" s="10" t="s">
+        <v>774</v>
       </c>
       <c r="L296" s="10" t="s">
-        <v>286</v>
+        <v>775</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.25">
@@ -13017,31 +13035,33 @@
         <v>4</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>786</v>
+        <v>269</v>
       </c>
       <c r="C297" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D297" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E297" s="12">
-        <v>1</v>
-      </c>
-      <c r="F297" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F297" s="11"/>
       <c r="G297" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H297" s="10"/>
-      <c r="I297" s="10"/>
+      <c r="H297" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I297" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="J297" s="10"/>
       <c r="K297" s="10" t="s">
-        <v>787</v>
+        <v>270</v>
       </c>
       <c r="L297" s="10" t="s">
-        <v>788</v>
+        <v>284</v>
       </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.25">
@@ -13049,33 +13069,31 @@
         <v>4</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>533</v>
+        <v>9</v>
       </c>
       <c r="C298" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D298" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E298" s="12">
-        <v>0</v>
-      </c>
-      <c r="F298" s="11"/>
+        <v>195</v>
+      </c>
+      <c r="F298" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G298" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H298" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I298" s="10" t="s">
-        <v>534</v>
-      </c>
+      <c r="H298" s="10"/>
+      <c r="I298" s="10"/>
       <c r="J298" s="10"/>
-      <c r="K298" s="10" t="s">
-        <v>537</v>
+      <c r="K298" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="L298" s="10" t="s">
-        <v>540</v>
+        <v>286</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
@@ -13083,7 +13101,7 @@
         <v>4</v>
       </c>
       <c r="B299" s="9" t="s">
-        <v>541</v>
+        <v>786</v>
       </c>
       <c r="C299" s="9" t="s">
         <v>814</v>
@@ -13104,10 +13122,10 @@
       <c r="I299" s="10"/>
       <c r="J299" s="10"/>
       <c r="K299" s="10" t="s">
-        <v>542</v>
+        <v>787</v>
       </c>
       <c r="L299" s="10" t="s">
-        <v>543</v>
+        <v>788</v>
       </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.25">
@@ -13115,31 +13133,33 @@
         <v>4</v>
       </c>
       <c r="B300" s="9" t="s">
-        <v>620</v>
+        <v>533</v>
       </c>
       <c r="C300" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D300" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E300" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="F300" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F300" s="11"/>
       <c r="G300" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H300" s="10"/>
-      <c r="I300" s="10"/>
+      <c r="H300" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I300" s="10" t="s">
+        <v>534</v>
+      </c>
       <c r="J300" s="10"/>
       <c r="K300" s="10" t="s">
-        <v>630</v>
+        <v>537</v>
       </c>
       <c r="L300" s="10" t="s">
-        <v>635</v>
+        <v>540</v>
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.25">
@@ -13147,7 +13167,7 @@
         <v>4</v>
       </c>
       <c r="B301" s="9" t="s">
-        <v>901</v>
+        <v>541</v>
       </c>
       <c r="C301" s="9" t="s">
         <v>814</v>
@@ -13156,10 +13176,10 @@
         <v>805</v>
       </c>
       <c r="E301" s="12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F301" s="11" t="s">
-        <v>904</v>
+        <v>21</v>
       </c>
       <c r="G301" s="11" t="b">
         <v>1</v>
@@ -13168,10 +13188,10 @@
       <c r="I301" s="10"/>
       <c r="J301" s="10"/>
       <c r="K301" s="10" t="s">
-        <v>903</v>
+        <v>542</v>
       </c>
       <c r="L301" s="10" t="s">
-        <v>902</v>
+        <v>543</v>
       </c>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.25">
@@ -13179,31 +13199,31 @@
         <v>4</v>
       </c>
       <c r="B302" s="9" t="s">
-        <v>827</v>
+        <v>620</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D302" s="9" t="s">
         <v>805</v>
       </c>
       <c r="E302" s="12">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F302" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G302" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H302" s="10"/>
       <c r="I302" s="10"/>
       <c r="J302" s="10"/>
       <c r="K302" s="10" t="s">
-        <v>830</v>
+        <v>630</v>
       </c>
       <c r="L302" s="10" t="s">
-        <v>831</v>
+        <v>635</v>
       </c>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.25">
@@ -13211,31 +13231,31 @@
         <v>4</v>
       </c>
       <c r="B303" s="9" t="s">
-        <v>826</v>
+        <v>901</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D303" s="9" t="s">
         <v>805</v>
       </c>
       <c r="E303" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F303" s="11" t="s">
-        <v>308</v>
+        <v>904</v>
       </c>
       <c r="G303" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H303" s="10"/>
       <c r="I303" s="10"/>
       <c r="J303" s="10"/>
       <c r="K303" s="10" t="s">
-        <v>800</v>
+        <v>903</v>
       </c>
       <c r="L303" s="10" t="s">
-        <v>832</v>
+        <v>902</v>
       </c>
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.25">
@@ -13243,17 +13263,19 @@
         <v>4</v>
       </c>
       <c r="B304" s="9" t="s">
-        <v>389</v>
+        <v>827</v>
       </c>
       <c r="C304" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D304" s="9" t="s">
-        <v>812</v>
-      </c>
-      <c r="E304" s="12"/>
+        <v>805</v>
+      </c>
+      <c r="E304" s="12">
+        <v>0</v>
+      </c>
       <c r="F304" s="11" t="s">
-        <v>21</v>
+        <v>308</v>
       </c>
       <c r="G304" s="11" t="b">
         <v>0</v>
@@ -13262,10 +13284,10 @@
       <c r="I304" s="10"/>
       <c r="J304" s="10"/>
       <c r="K304" s="10" t="s">
-        <v>390</v>
+        <v>830</v>
       </c>
       <c r="L304" s="10" t="s">
-        <v>390</v>
+        <v>831</v>
       </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.25">
@@ -13273,7 +13295,7 @@
         <v>4</v>
       </c>
       <c r="B305" s="9" t="s">
-        <v>855</v>
+        <v>826</v>
       </c>
       <c r="C305" s="9" t="s">
         <v>815</v>
@@ -13285,7 +13307,7 @@
         <v>0</v>
       </c>
       <c r="F305" s="11" t="s">
-        <v>56</v>
+        <v>308</v>
       </c>
       <c r="G305" s="11" t="b">
         <v>0</v>
@@ -13294,10 +13316,10 @@
       <c r="I305" s="10"/>
       <c r="J305" s="10"/>
       <c r="K305" s="10" t="s">
-        <v>858</v>
+        <v>800</v>
       </c>
       <c r="L305" s="10" t="s">
-        <v>858</v>
+        <v>832</v>
       </c>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.25">
@@ -13305,19 +13327,17 @@
         <v>4</v>
       </c>
       <c r="B306" s="9" t="s">
-        <v>860</v>
+        <v>389</v>
       </c>
       <c r="C306" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D306" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E306" s="12">
-        <v>0</v>
-      </c>
+        <v>812</v>
+      </c>
+      <c r="E306" s="12"/>
       <c r="F306" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G306" s="11" t="b">
         <v>0</v>
@@ -13326,9 +13346,73 @@
       <c r="I306" s="10"/>
       <c r="J306" s="10"/>
       <c r="K306" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="L306" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A307" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B307" s="9" t="s">
+        <v>855</v>
+      </c>
+      <c r="C307" s="9" t="s">
+        <v>815</v>
+      </c>
+      <c r="D307" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="E307" s="12">
+        <v>0</v>
+      </c>
+      <c r="F307" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G307" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H307" s="10"/>
+      <c r="I307" s="10"/>
+      <c r="J307" s="10"/>
+      <c r="K307" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="L307" s="10" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A308" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B308" s="9" t="s">
+        <v>860</v>
+      </c>
+      <c r="C308" s="9" t="s">
+        <v>815</v>
+      </c>
+      <c r="D308" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="E308" s="12">
+        <v>0</v>
+      </c>
+      <c r="F308" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G308" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H308" s="10"/>
+      <c r="I308" s="10"/>
+      <c r="J308" s="10"/>
+      <c r="K308" s="10" t="s">
         <v>859</v>
       </c>
-      <c r="L306" s="10" t="s">
+      <c r="L308" s="10" t="s">
         <v>859</v>
       </c>
     </row>

</xml_diff>

<commit_message>
functioning interface components for user flux profiles
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -3,19 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B5D784-AF4D-4DFC-9BD2-D88A3798A3DD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D4A7C9-3B34-48B9-919D-CBB5169D518A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="943">
   <si>
     <t>String name</t>
   </si>
@@ -2841,6 +2849,9 @@
   </si>
   <si>
     <t>User flux profile data</t>
+  </si>
+  <si>
+    <t>1,1,1,1,1;1,1,1,1,1;1,1,1,1,1;1,1,1,1,1;1,1,1,1,1</t>
   </si>
 </sst>
 </file>
@@ -3426,8 +3437,8 @@
   <dimension ref="A1:L308"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E231" sqref="E231"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I252" sqref="I252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10921,9 +10932,11 @@
         <v>814</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E232" s="12"/>
+        <v>802</v>
+      </c>
+      <c r="E232" s="12" t="s">
+        <v>942</v>
+      </c>
       <c r="F232" s="11" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
image size profile functionality working for flat plate receivers
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D4A7C9-3B34-48B9-919D-CBB5169D518A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D193B1DB-AD7A-45FE-8192-2B5D9758AD41}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="945">
   <si>
     <t>String name</t>
   </si>
@@ -2852,6 +2852,12 @@
   </si>
   <si>
     <t>1,1,1,1,1;1,1,1,1,1;1,1,1,1,1;1,1,1,1,1;1,1,1,1,1</t>
+  </si>
+  <si>
+    <t>Normalized user flux profile</t>
+  </si>
+  <si>
+    <t>n_user_flux_profile</t>
   </si>
 </sst>
 </file>
@@ -3090,10 +3096,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L308" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L308" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L318">
-    <sortCondition ref="A1:A318"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L309" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L309" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L319">
+    <sortCondition ref="A1:A319"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain" dataDxfId="11"/>
@@ -3434,11 +3440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L308"/>
+  <dimension ref="A1:L309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I252" sqref="I252"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B254" sqref="B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11644,19 +11650,17 @@
         <v>8</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>310</v>
+        <v>944</v>
       </c>
       <c r="C254" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D254" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E254" s="12">
-        <v>0</v>
-      </c>
+        <v>802</v>
+      </c>
+      <c r="E254" s="12"/>
       <c r="F254" s="11" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
       <c r="G254" s="11" t="b">
         <v>0</v>
@@ -11665,10 +11669,10 @@
       <c r="I254" s="10"/>
       <c r="J254" s="10"/>
       <c r="K254" s="10" t="s">
-        <v>311</v>
+        <v>943</v>
       </c>
       <c r="L254" s="10" t="s">
-        <v>424</v>
+        <v>943</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">
@@ -11676,7 +11680,7 @@
         <v>8</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>25</v>
+        <v>310</v>
       </c>
       <c r="C255" s="9" t="s">
         <v>815</v>
@@ -11685,10 +11689,10 @@
         <v>805</v>
       </c>
       <c r="E255" s="12">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="F255" s="11" t="s">
-        <v>23</v>
+        <v>308</v>
       </c>
       <c r="G255" s="11" t="b">
         <v>0</v>
@@ -11696,11 +11700,11 @@
       <c r="H255" s="10"/>
       <c r="I255" s="10"/>
       <c r="J255" s="10"/>
-      <c r="K255" s="9" t="s">
-        <v>140</v>
+      <c r="K255" s="10" t="s">
+        <v>311</v>
       </c>
       <c r="L255" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
@@ -11708,7 +11712,7 @@
         <v>8</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>577</v>
+        <v>25</v>
       </c>
       <c r="C256" s="9" t="s">
         <v>815</v>
@@ -11717,10 +11721,10 @@
         <v>805</v>
       </c>
       <c r="E256" s="12">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="F256" s="11" t="s">
-        <v>574</v>
+        <v>23</v>
       </c>
       <c r="G256" s="11" t="b">
         <v>0</v>
@@ -11728,11 +11732,11 @@
       <c r="H256" s="10"/>
       <c r="I256" s="10"/>
       <c r="J256" s="10"/>
-      <c r="K256" s="10" t="s">
-        <v>578</v>
+      <c r="K256" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="L256" s="10" t="s">
-        <v>579</v>
+        <v>425</v>
       </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
@@ -11740,7 +11744,7 @@
         <v>8</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>294</v>
+        <v>577</v>
       </c>
       <c r="C257" s="9" t="s">
         <v>815</v>
@@ -11749,22 +11753,22 @@
         <v>805</v>
       </c>
       <c r="E257" s="12">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="F257" s="11" t="s">
-        <v>21</v>
+        <v>574</v>
       </c>
       <c r="G257" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H257" s="10"/>
       <c r="I257" s="10"/>
       <c r="J257" s="10"/>
       <c r="K257" s="10" t="s">
-        <v>295</v>
+        <v>578</v>
       </c>
       <c r="L257" s="10" t="s">
-        <v>296</v>
+        <v>579</v>
       </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
@@ -11772,7 +11776,7 @@
         <v>8</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>823</v>
+        <v>294</v>
       </c>
       <c r="C258" s="9" t="s">
         <v>815</v>
@@ -11781,22 +11785,22 @@
         <v>805</v>
       </c>
       <c r="E258" s="12">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F258" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G258" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H258" s="10"/>
       <c r="I258" s="10"/>
       <c r="J258" s="10"/>
       <c r="K258" s="10" t="s">
-        <v>824</v>
+        <v>295</v>
       </c>
       <c r="L258" s="10" t="s">
-        <v>824</v>
+        <v>296</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
@@ -11804,7 +11808,7 @@
         <v>8</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>573</v>
+        <v>823</v>
       </c>
       <c r="C259" s="9" t="s">
         <v>815</v>
@@ -11816,7 +11820,7 @@
         <v>0</v>
       </c>
       <c r="F259" s="11" t="s">
-        <v>574</v>
+        <v>21</v>
       </c>
       <c r="G259" s="11" t="b">
         <v>0</v>
@@ -11825,10 +11829,10 @@
       <c r="I259" s="10"/>
       <c r="J259" s="10"/>
       <c r="K259" s="10" t="s">
-        <v>575</v>
+        <v>824</v>
       </c>
       <c r="L259" s="10" t="s">
-        <v>576</v>
+        <v>824</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
@@ -11836,7 +11840,7 @@
         <v>8</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>911</v>
+        <v>573</v>
       </c>
       <c r="C260" s="9" t="s">
         <v>815</v>
@@ -11857,10 +11861,10 @@
       <c r="I260" s="10"/>
       <c r="J260" s="10"/>
       <c r="K260" s="10" t="s">
-        <v>912</v>
+        <v>575</v>
       </c>
       <c r="L260" s="10" t="s">
-        <v>913</v>
+        <v>576</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
@@ -11868,7 +11872,7 @@
         <v>8</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>924</v>
+        <v>911</v>
       </c>
       <c r="C261" s="9" t="s">
         <v>815</v>
@@ -11880,7 +11884,7 @@
         <v>0</v>
       </c>
       <c r="F261" s="11" t="s">
-        <v>23</v>
+        <v>574</v>
       </c>
       <c r="G261" s="11" t="b">
         <v>0</v>
@@ -11888,11 +11892,11 @@
       <c r="H261" s="10"/>
       <c r="I261" s="10"/>
       <c r="J261" s="10"/>
-      <c r="K261" s="9" t="s">
-        <v>926</v>
+      <c r="K261" s="10" t="s">
+        <v>912</v>
       </c>
       <c r="L261" s="10" t="s">
-        <v>148</v>
+        <v>913</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
@@ -11900,7 +11904,7 @@
         <v>8</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C262" s="9" t="s">
         <v>815</v>
@@ -11921,10 +11925,10 @@
       <c r="I262" s="10"/>
       <c r="J262" s="10"/>
       <c r="K262" s="9" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="L262" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
@@ -11932,7 +11936,7 @@
         <v>8</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C263" s="9" t="s">
         <v>815</v>
@@ -11953,42 +11957,42 @@
       <c r="I263" s="10"/>
       <c r="J263" s="10"/>
       <c r="K263" s="9" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="L263" s="10" t="s">
-        <v>426</v>
+        <v>149</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>19</v>
+        <v>925</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>805</v>
       </c>
       <c r="E264" s="12">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F264" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="G264" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H264" s="10"/>
       <c r="I264" s="10"/>
       <c r="J264" s="10"/>
-      <c r="K264" s="10" t="s">
-        <v>138</v>
+      <c r="K264" s="9" t="s">
+        <v>928</v>
       </c>
       <c r="L264" s="10" t="s">
-        <v>110</v>
+        <v>426</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
@@ -11996,7 +12000,7 @@
         <v>4</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>814</v>
@@ -12005,7 +12009,7 @@
         <v>805</v>
       </c>
       <c r="E265" s="12">
-        <v>-180</v>
+        <v>180</v>
       </c>
       <c r="F265" s="11" t="s">
         <v>56</v>
@@ -12017,10 +12021,10 @@
       <c r="I265" s="10"/>
       <c r="J265" s="10"/>
       <c r="K265" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L265" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
@@ -12028,7 +12032,7 @@
         <v>4</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>814</v>
@@ -12037,10 +12041,10 @@
         <v>805</v>
       </c>
       <c r="E266" s="12">
-        <v>2</v>
+        <v>-180</v>
       </c>
       <c r="F266" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G266" s="11" t="b">
         <v>1</v>
@@ -12048,11 +12052,11 @@
       <c r="H266" s="10"/>
       <c r="I266" s="10"/>
       <c r="J266" s="10"/>
-      <c r="K266" s="9" t="s">
-        <v>127</v>
+      <c r="K266" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="L266" s="10" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
@@ -12060,31 +12064,31 @@
         <v>4</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>545</v>
+        <v>99</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E267" s="12" t="s">
-        <v>546</v>
+        <v>805</v>
+      </c>
+      <c r="E267" s="12">
+        <v>2</v>
       </c>
       <c r="F267" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G267" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H267" s="10"/>
       <c r="I267" s="10"/>
       <c r="J267" s="10"/>
-      <c r="K267" s="10" t="s">
-        <v>547</v>
+      <c r="K267" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="L267" s="10" t="s">
-        <v>547</v>
+        <v>213</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
@@ -12092,7 +12096,7 @@
         <v>4</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>104</v>
+        <v>545</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>814</v>
@@ -12100,27 +12104,23 @@
       <c r="D268" s="9" t="s">
         <v>804</v>
       </c>
-      <c r="E268" s="12">
-        <v>5</v>
+      <c r="E268" s="12" t="s">
+        <v>546</v>
       </c>
       <c r="F268" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G268" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H268" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I268" s="10" t="s">
-        <v>556</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H268" s="10"/>
+      <c r="I268" s="10"/>
       <c r="J268" s="10"/>
-      <c r="K268" s="9" t="s">
-        <v>135</v>
+      <c r="K268" s="10" t="s">
+        <v>547</v>
       </c>
       <c r="L268" s="10" t="s">
-        <v>105</v>
+        <v>547</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
@@ -12128,16 +12128,16 @@
         <v>4</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
       <c r="C269" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E269" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F269" s="11" t="s">
         <v>21</v>
@@ -12145,14 +12145,18 @@
       <c r="G269" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H269" s="10"/>
-      <c r="I269" s="10"/>
+      <c r="H269" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I269" s="10" t="s">
+        <v>556</v>
+      </c>
       <c r="J269" s="10"/>
-      <c r="K269" s="10" t="s">
-        <v>193</v>
+      <c r="K269" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="L269" s="10" t="s">
-        <v>194</v>
+        <v>105</v>
       </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
@@ -12160,7 +12164,7 @@
         <v>4</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>582</v>
+        <v>192</v>
       </c>
       <c r="C270" s="9" t="s">
         <v>814</v>
@@ -12169,7 +12173,7 @@
         <v>803</v>
       </c>
       <c r="E270" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F270" s="11" t="s">
         <v>21</v>
@@ -12181,10 +12185,10 @@
       <c r="I270" s="10"/>
       <c r="J270" s="10"/>
       <c r="K270" s="10" t="s">
-        <v>583</v>
+        <v>193</v>
       </c>
       <c r="L270" s="10" t="s">
-        <v>584</v>
+        <v>194</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
@@ -12192,19 +12196,19 @@
         <v>4</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>188</v>
+        <v>582</v>
       </c>
       <c r="C271" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E271" s="12">
-        <v>950</v>
+        <v>2</v>
       </c>
       <c r="F271" s="11" t="s">
-        <v>189</v>
+        <v>21</v>
       </c>
       <c r="G271" s="11" t="b">
         <v>1</v>
@@ -12213,10 +12217,10 @@
       <c r="I271" s="10"/>
       <c r="J271" s="10"/>
       <c r="K271" s="10" t="s">
-        <v>190</v>
+        <v>583</v>
       </c>
       <c r="L271" s="10" t="s">
-        <v>191</v>
+        <v>584</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
@@ -12224,35 +12228,31 @@
         <v>4</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>521</v>
+        <v>188</v>
       </c>
       <c r="C272" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E272" s="12">
-        <v>7</v>
+        <v>950</v>
       </c>
       <c r="F272" s="11" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="G272" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H272" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I272" s="10" t="s">
-        <v>523</v>
-      </c>
+      <c r="H272" s="10"/>
+      <c r="I272" s="10"/>
       <c r="J272" s="10"/>
       <c r="K272" s="10" t="s">
-        <v>555</v>
+        <v>190</v>
       </c>
       <c r="L272" s="10" t="s">
-        <v>522</v>
+        <v>191</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
@@ -12260,16 +12260,16 @@
         <v>4</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>889</v>
+        <v>521</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>806</v>
-      </c>
-      <c r="E273" s="12" t="b">
-        <v>0</v>
+        <v>804</v>
+      </c>
+      <c r="E273" s="12">
+        <v>7</v>
       </c>
       <c r="F273" s="11" t="s">
         <v>21</v>
@@ -12278,15 +12278,17 @@
         <v>1</v>
       </c>
       <c r="H273" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="I273" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="I273" s="10" t="s">
+        <v>523</v>
+      </c>
       <c r="J273" s="10"/>
       <c r="K273" s="10" t="s">
-        <v>890</v>
+        <v>555</v>
       </c>
       <c r="L273" s="10" t="s">
-        <v>891</v>
+        <v>522</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
@@ -12294,7 +12296,7 @@
         <v>4</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>636</v>
+        <v>889</v>
       </c>
       <c r="C274" s="9" t="s">
         <v>814</v>
@@ -12303,13 +12305,13 @@
         <v>806</v>
       </c>
       <c r="E274" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F274" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G274" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H274" s="10" t="s">
         <v>202</v>
@@ -12317,10 +12319,10 @@
       <c r="I274" s="10"/>
       <c r="J274" s="10"/>
       <c r="K274" s="10" t="s">
-        <v>637</v>
+        <v>890</v>
       </c>
       <c r="L274" s="10" t="s">
-        <v>638</v>
+        <v>891</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">
@@ -12328,7 +12330,7 @@
         <v>4</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>612</v>
+        <v>636</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>814</v>
@@ -12337,13 +12339,13 @@
         <v>806</v>
       </c>
       <c r="E275" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F275" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G275" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H275" s="10" t="s">
         <v>202</v>
@@ -12351,10 +12353,10 @@
       <c r="I275" s="10"/>
       <c r="J275" s="10"/>
       <c r="K275" s="10" t="s">
-        <v>610</v>
+        <v>637</v>
       </c>
       <c r="L275" s="10" t="s">
-        <v>611</v>
+        <v>638</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
@@ -12362,7 +12364,7 @@
         <v>4</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>209</v>
+        <v>612</v>
       </c>
       <c r="C276" s="9" t="s">
         <v>814</v>
@@ -12371,13 +12373,13 @@
         <v>806</v>
       </c>
       <c r="E276" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F276" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G276" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H276" s="10" t="s">
         <v>202</v>
@@ -12385,10 +12387,10 @@
       <c r="I276" s="10"/>
       <c r="J276" s="10"/>
       <c r="K276" s="10" t="s">
-        <v>210</v>
+        <v>610</v>
       </c>
       <c r="L276" s="10" t="s">
-        <v>211</v>
+        <v>611</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
@@ -12396,7 +12398,7 @@
         <v>4</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>908</v>
+        <v>209</v>
       </c>
       <c r="C277" s="9" t="s">
         <v>814</v>
@@ -12405,13 +12407,13 @@
         <v>806</v>
       </c>
       <c r="E277" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F277" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G277" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H277" s="10" t="s">
         <v>202</v>
@@ -12419,10 +12421,10 @@
       <c r="I277" s="10"/>
       <c r="J277" s="10"/>
       <c r="K277" s="10" t="s">
-        <v>909</v>
+        <v>210</v>
       </c>
       <c r="L277" s="10" t="s">
-        <v>910</v>
+        <v>211</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
@@ -12430,27 +12432,33 @@
         <v>4</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>387</v>
+        <v>908</v>
       </c>
       <c r="C278" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D278" s="9" t="s">
-        <v>804</v>
-      </c>
-      <c r="E278" s="12"/>
-      <c r="F278" s="11"/>
+        <v>806</v>
+      </c>
+      <c r="E278" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F278" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G278" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H278" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="H278" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="I278" s="10"/>
       <c r="J278" s="10"/>
       <c r="K278" s="10" t="s">
-        <v>388</v>
+        <v>909</v>
       </c>
       <c r="L278" s="10" t="s">
-        <v>388</v>
+        <v>910</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
@@ -12458,7 +12466,7 @@
         <v>4</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>6</v>
+        <v>387</v>
       </c>
       <c r="C279" s="9" t="s">
         <v>814</v>
@@ -12466,27 +12474,19 @@
       <c r="D279" s="9" t="s">
         <v>804</v>
       </c>
-      <c r="E279" s="12">
-        <v>0</v>
-      </c>
-      <c r="F279" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="E279" s="12"/>
+      <c r="F279" s="11"/>
       <c r="G279" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="H279" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I279" s="10" t="s">
-        <v>132</v>
-      </c>
+      <c r="H279" s="10"/>
+      <c r="I279" s="10"/>
       <c r="J279" s="10"/>
-      <c r="K279" s="9" t="s">
-        <v>133</v>
+      <c r="K279" s="10" t="s">
+        <v>388</v>
       </c>
       <c r="L279" s="10" t="s">
-        <v>65</v>
+        <v>388</v>
       </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.25">
@@ -12494,31 +12494,35 @@
         <v>4</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>623</v>
+        <v>6</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D280" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E280" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F280" s="11" t="s">
-        <v>625</v>
+        <v>21</v>
       </c>
       <c r="G280" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H280" s="10"/>
-      <c r="I280" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="H280" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I280" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="J280" s="10"/>
-      <c r="K280" s="10" t="s">
-        <v>627</v>
+      <c r="K280" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="L280" s="10" t="s">
-        <v>632</v>
+        <v>65</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">
@@ -12526,7 +12530,7 @@
         <v>4</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="C281" s="9" t="s">
         <v>814</v>
@@ -12547,10 +12551,10 @@
       <c r="I281" s="10"/>
       <c r="J281" s="10"/>
       <c r="K281" s="10" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="L281" s="10" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.25">
@@ -12558,7 +12562,7 @@
         <v>4</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C282" s="9" t="s">
         <v>814</v>
@@ -12567,7 +12571,7 @@
         <v>805</v>
       </c>
       <c r="E282" s="12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F282" s="11" t="s">
         <v>625</v>
@@ -12579,10 +12583,10 @@
       <c r="I282" s="10"/>
       <c r="J282" s="10"/>
       <c r="K282" s="10" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="L282" s="10" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.25">
@@ -12590,7 +12594,7 @@
         <v>4</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="C283" s="9" t="s">
         <v>814</v>
@@ -12611,10 +12615,10 @@
       <c r="I283" s="10"/>
       <c r="J283" s="10"/>
       <c r="K283" s="10" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="L283" s="10" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.25">
@@ -12622,7 +12626,7 @@
         <v>4</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="C284" s="9" t="s">
         <v>814</v>
@@ -12631,10 +12635,10 @@
         <v>805</v>
       </c>
       <c r="E284" s="12">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F284" s="11" t="s">
-        <v>21</v>
+        <v>625</v>
       </c>
       <c r="G284" s="11" t="b">
         <v>1</v>
@@ -12643,10 +12647,10 @@
       <c r="I284" s="10"/>
       <c r="J284" s="10"/>
       <c r="K284" s="10" t="s">
-        <v>614</v>
+        <v>628</v>
       </c>
       <c r="L284" s="10" t="s">
-        <v>615</v>
+        <v>633</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.25">
@@ -12654,7 +12658,7 @@
         <v>4</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>5</v>
+        <v>613</v>
       </c>
       <c r="C285" s="9" t="s">
         <v>814</v>
@@ -12663,10 +12667,10 @@
         <v>805</v>
       </c>
       <c r="E285" s="12">
-        <v>670</v>
+        <v>0.03</v>
       </c>
       <c r="F285" s="11" t="s">
-        <v>212</v>
+        <v>21</v>
       </c>
       <c r="G285" s="11" t="b">
         <v>1</v>
@@ -12674,11 +12678,11 @@
       <c r="H285" s="10"/>
       <c r="I285" s="10"/>
       <c r="J285" s="10"/>
-      <c r="K285" s="9" t="s">
-        <v>126</v>
+      <c r="K285" s="10" t="s">
+        <v>614</v>
       </c>
       <c r="L285" s="10" t="s">
-        <v>64</v>
+        <v>615</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
@@ -12686,35 +12690,31 @@
         <v>4</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C286" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E286" s="12">
-        <v>0</v>
+        <v>670</v>
       </c>
       <c r="F286" s="11" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="G286" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H286" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I286" s="10" t="s">
-        <v>785</v>
-      </c>
+      <c r="H286" s="10"/>
+      <c r="I286" s="10"/>
       <c r="J286" s="10"/>
       <c r="K286" s="9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="L286" s="10" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
@@ -12722,16 +12722,16 @@
         <v>4</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>531</v>
+        <v>100</v>
       </c>
       <c r="C287" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E287" s="12">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F287" s="11" t="s">
         <v>21</v>
@@ -12739,14 +12739,18 @@
       <c r="G287" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H287" s="10"/>
-      <c r="I287" s="10"/>
+      <c r="H287" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I287" s="10" t="s">
+        <v>785</v>
+      </c>
       <c r="J287" s="10"/>
-      <c r="K287" s="10" t="s">
-        <v>535</v>
+      <c r="K287" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="L287" s="10" t="s">
-        <v>538</v>
+        <v>101</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
@@ -12754,7 +12758,7 @@
         <v>4</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C288" s="9" t="s">
         <v>814</v>
@@ -12775,10 +12779,10 @@
       <c r="I288" s="10"/>
       <c r="J288" s="10"/>
       <c r="K288" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L288" s="10" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -12786,7 +12790,7 @@
         <v>4</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>14</v>
+        <v>532</v>
       </c>
       <c r="C289" s="9" t="s">
         <v>814</v>
@@ -12795,22 +12799,22 @@
         <v>805</v>
       </c>
       <c r="E289" s="12">
-        <v>195</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F289" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G289" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H289" s="10"/>
       <c r="I289" s="10"/>
       <c r="J289" s="10"/>
-      <c r="K289" s="9" t="s">
-        <v>137</v>
+      <c r="K289" s="10" t="s">
+        <v>536</v>
       </c>
       <c r="L289" s="10" t="s">
-        <v>68</v>
+        <v>539</v>
       </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
@@ -12818,7 +12822,7 @@
         <v>4</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C290" s="9" t="s">
         <v>814</v>
@@ -12827,7 +12831,7 @@
         <v>805</v>
       </c>
       <c r="E290" s="12">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="F290" s="11" t="s">
         <v>23</v>
@@ -12839,10 +12843,10 @@
       <c r="I290" s="10"/>
       <c r="J290" s="10"/>
       <c r="K290" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L290" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
@@ -12850,7 +12854,7 @@
         <v>4</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>892</v>
+        <v>13</v>
       </c>
       <c r="C291" s="9" t="s">
         <v>814</v>
@@ -12859,22 +12863,22 @@
         <v>805</v>
       </c>
       <c r="E291" s="12">
-        <v>0.5</v>
+        <v>16</v>
       </c>
       <c r="F291" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G291" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H291" s="10"/>
       <c r="I291" s="10"/>
       <c r="J291" s="10"/>
-      <c r="K291" s="10" t="s">
-        <v>893</v>
+      <c r="K291" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="L291" s="10" t="s">
-        <v>893</v>
+        <v>67</v>
       </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
@@ -12882,7 +12886,7 @@
         <v>4</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>97</v>
+        <v>892</v>
       </c>
       <c r="C292" s="9" t="s">
         <v>814</v>
@@ -12891,7 +12895,7 @@
         <v>805</v>
       </c>
       <c r="E292" s="12">
-        <v>1.33</v>
+        <v>0.5</v>
       </c>
       <c r="F292" s="11" t="s">
         <v>21</v>
@@ -12902,11 +12906,11 @@
       <c r="H292" s="10"/>
       <c r="I292" s="10"/>
       <c r="J292" s="10"/>
-      <c r="K292" s="9" t="s">
-        <v>128</v>
+      <c r="K292" s="10" t="s">
+        <v>893</v>
       </c>
       <c r="L292" s="10" t="s">
-        <v>98</v>
+        <v>893</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
@@ -12914,7 +12918,7 @@
         <v>4</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>853</v>
+        <v>97</v>
       </c>
       <c r="C293" s="9" t="s">
         <v>814</v>
@@ -12923,10 +12927,10 @@
         <v>805</v>
       </c>
       <c r="E293" s="12">
-        <v>180</v>
+        <v>1.33</v>
       </c>
       <c r="F293" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G293" s="11" t="b">
         <v>1</v>
@@ -12934,11 +12938,11 @@
       <c r="H293" s="10"/>
       <c r="I293" s="10"/>
       <c r="J293" s="10"/>
-      <c r="K293" s="10" t="s">
-        <v>856</v>
+      <c r="K293" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="L293" s="10" t="s">
-        <v>500</v>
+        <v>98</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
@@ -12946,7 +12950,7 @@
         <v>4</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C294" s="9" t="s">
         <v>814</v>
@@ -12955,7 +12959,7 @@
         <v>805</v>
       </c>
       <c r="E294" s="12">
-        <v>85</v>
+        <v>180</v>
       </c>
       <c r="F294" s="11" t="s">
         <v>56</v>
@@ -12967,10 +12971,10 @@
       <c r="I294" s="10"/>
       <c r="J294" s="10"/>
       <c r="K294" s="10" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="L294" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
@@ -12978,35 +12982,31 @@
         <v>4</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>497</v>
+        <v>854</v>
       </c>
       <c r="C295" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E295" s="12">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F295" s="11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G295" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H295" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I295" s="10" t="s">
-        <v>520</v>
-      </c>
+      <c r="H295" s="10"/>
+      <c r="I295" s="10"/>
       <c r="J295" s="10"/>
       <c r="K295" s="10" t="s">
-        <v>498</v>
+        <v>857</v>
       </c>
       <c r="L295" s="10" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
@@ -13014,7 +13014,7 @@
         <v>4</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>773</v>
+        <v>497</v>
       </c>
       <c r="C296" s="9" t="s">
         <v>814</v>
@@ -13034,13 +13034,15 @@
       <c r="H296" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="I296" s="10"/>
+      <c r="I296" s="10" t="s">
+        <v>520</v>
+      </c>
       <c r="J296" s="10"/>
       <c r="K296" s="10" t="s">
-        <v>774</v>
+        <v>498</v>
       </c>
       <c r="L296" s="10" t="s">
-        <v>775</v>
+        <v>499</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.25">
@@ -13048,7 +13050,7 @@
         <v>4</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>269</v>
+        <v>773</v>
       </c>
       <c r="C297" s="9" t="s">
         <v>814</v>
@@ -13059,22 +13061,22 @@
       <c r="E297" s="12">
         <v>0</v>
       </c>
-      <c r="F297" s="11"/>
+      <c r="F297" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G297" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H297" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="I297" s="10" t="s">
-        <v>271</v>
-      </c>
+      <c r="I297" s="10"/>
       <c r="J297" s="10"/>
       <c r="K297" s="10" t="s">
-        <v>270</v>
+        <v>774</v>
       </c>
       <c r="L297" s="10" t="s">
-        <v>284</v>
+        <v>775</v>
       </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.25">
@@ -13082,31 +13084,33 @@
         <v>4</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>9</v>
+        <v>269</v>
       </c>
       <c r="C298" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D298" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E298" s="12">
-        <v>195</v>
-      </c>
-      <c r="F298" s="11" t="s">
-        <v>23</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F298" s="11"/>
       <c r="G298" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H298" s="10"/>
-      <c r="I298" s="10"/>
+      <c r="H298" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I298" s="10" t="s">
+        <v>271</v>
+      </c>
       <c r="J298" s="10"/>
-      <c r="K298" s="9" t="s">
-        <v>285</v>
+      <c r="K298" s="10" t="s">
+        <v>270</v>
       </c>
       <c r="L298" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
@@ -13114,7 +13118,7 @@
         <v>4</v>
       </c>
       <c r="B299" s="9" t="s">
-        <v>786</v>
+        <v>9</v>
       </c>
       <c r="C299" s="9" t="s">
         <v>814</v>
@@ -13123,10 +13127,10 @@
         <v>805</v>
       </c>
       <c r="E299" s="12">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="F299" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G299" s="11" t="b">
         <v>1</v>
@@ -13134,11 +13138,11 @@
       <c r="H299" s="10"/>
       <c r="I299" s="10"/>
       <c r="J299" s="10"/>
-      <c r="K299" s="10" t="s">
-        <v>787</v>
+      <c r="K299" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="L299" s="10" t="s">
-        <v>788</v>
+        <v>286</v>
       </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.25">
@@ -13146,33 +13150,31 @@
         <v>4</v>
       </c>
       <c r="B300" s="9" t="s">
-        <v>533</v>
+        <v>786</v>
       </c>
       <c r="C300" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D300" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E300" s="12">
-        <v>0</v>
-      </c>
-      <c r="F300" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="F300" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G300" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H300" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I300" s="10" t="s">
-        <v>534</v>
-      </c>
+      <c r="H300" s="10"/>
+      <c r="I300" s="10"/>
       <c r="J300" s="10"/>
       <c r="K300" s="10" t="s">
-        <v>537</v>
+        <v>787</v>
       </c>
       <c r="L300" s="10" t="s">
-        <v>540</v>
+        <v>788</v>
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.25">
@@ -13180,31 +13182,33 @@
         <v>4</v>
       </c>
       <c r="B301" s="9" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="C301" s="9" t="s">
         <v>814</v>
       </c>
       <c r="D301" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E301" s="12">
-        <v>1</v>
-      </c>
-      <c r="F301" s="11" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F301" s="11"/>
       <c r="G301" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="H301" s="10"/>
-      <c r="I301" s="10"/>
+      <c r="H301" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I301" s="10" t="s">
+        <v>534</v>
+      </c>
       <c r="J301" s="10"/>
       <c r="K301" s="10" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="L301" s="10" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.25">
@@ -13212,7 +13216,7 @@
         <v>4</v>
       </c>
       <c r="B302" s="9" t="s">
-        <v>620</v>
+        <v>541</v>
       </c>
       <c r="C302" s="9" t="s">
         <v>814</v>
@@ -13221,7 +13225,7 @@
         <v>805</v>
       </c>
       <c r="E302" s="12">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="F302" s="11" t="s">
         <v>21</v>
@@ -13233,10 +13237,10 @@
       <c r="I302" s="10"/>
       <c r="J302" s="10"/>
       <c r="K302" s="10" t="s">
-        <v>630</v>
+        <v>542</v>
       </c>
       <c r="L302" s="10" t="s">
-        <v>635</v>
+        <v>543</v>
       </c>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.25">
@@ -13244,7 +13248,7 @@
         <v>4</v>
       </c>
       <c r="B303" s="9" t="s">
-        <v>901</v>
+        <v>620</v>
       </c>
       <c r="C303" s="9" t="s">
         <v>814</v>
@@ -13253,10 +13257,10 @@
         <v>805</v>
       </c>
       <c r="E303" s="12">
-        <v>100</v>
+        <v>1E-3</v>
       </c>
       <c r="F303" s="11" t="s">
-        <v>904</v>
+        <v>21</v>
       </c>
       <c r="G303" s="11" t="b">
         <v>1</v>
@@ -13265,10 +13269,10 @@
       <c r="I303" s="10"/>
       <c r="J303" s="10"/>
       <c r="K303" s="10" t="s">
-        <v>903</v>
+        <v>630</v>
       </c>
       <c r="L303" s="10" t="s">
-        <v>902</v>
+        <v>635</v>
       </c>
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.25">
@@ -13276,31 +13280,31 @@
         <v>4</v>
       </c>
       <c r="B304" s="9" t="s">
-        <v>827</v>
+        <v>901</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D304" s="9" t="s">
         <v>805</v>
       </c>
       <c r="E304" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F304" s="11" t="s">
-        <v>308</v>
+        <v>904</v>
       </c>
       <c r="G304" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H304" s="10"/>
       <c r="I304" s="10"/>
       <c r="J304" s="10"/>
       <c r="K304" s="10" t="s">
-        <v>830</v>
+        <v>903</v>
       </c>
       <c r="L304" s="10" t="s">
-        <v>831</v>
+        <v>902</v>
       </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.25">
@@ -13308,7 +13312,7 @@
         <v>4</v>
       </c>
       <c r="B305" s="9" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C305" s="9" t="s">
         <v>815</v>
@@ -13329,10 +13333,10 @@
       <c r="I305" s="10"/>
       <c r="J305" s="10"/>
       <c r="K305" s="10" t="s">
-        <v>800</v>
+        <v>830</v>
       </c>
       <c r="L305" s="10" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.25">
@@ -13340,17 +13344,19 @@
         <v>4</v>
       </c>
       <c r="B306" s="9" t="s">
-        <v>389</v>
+        <v>826</v>
       </c>
       <c r="C306" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D306" s="9" t="s">
-        <v>812</v>
-      </c>
-      <c r="E306" s="12"/>
+        <v>805</v>
+      </c>
+      <c r="E306" s="12">
+        <v>0</v>
+      </c>
       <c r="F306" s="11" t="s">
-        <v>21</v>
+        <v>308</v>
       </c>
       <c r="G306" s="11" t="b">
         <v>0</v>
@@ -13359,10 +13365,10 @@
       <c r="I306" s="10"/>
       <c r="J306" s="10"/>
       <c r="K306" s="10" t="s">
-        <v>390</v>
+        <v>800</v>
       </c>
       <c r="L306" s="10" t="s">
-        <v>390</v>
+        <v>832</v>
       </c>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.25">
@@ -13370,19 +13376,17 @@
         <v>4</v>
       </c>
       <c r="B307" s="9" t="s">
-        <v>855</v>
+        <v>389</v>
       </c>
       <c r="C307" s="9" t="s">
         <v>815</v>
       </c>
       <c r="D307" s="9" t="s">
-        <v>805</v>
-      </c>
-      <c r="E307" s="12">
-        <v>0</v>
-      </c>
+        <v>812</v>
+      </c>
+      <c r="E307" s="12"/>
       <c r="F307" s="11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G307" s="11" t="b">
         <v>0</v>
@@ -13391,10 +13395,10 @@
       <c r="I307" s="10"/>
       <c r="J307" s="10"/>
       <c r="K307" s="10" t="s">
-        <v>858</v>
+        <v>390</v>
       </c>
       <c r="L307" s="10" t="s">
-        <v>858</v>
+        <v>390</v>
       </c>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.25">
@@ -13402,7 +13406,7 @@
         <v>4</v>
       </c>
       <c r="B308" s="9" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
       <c r="C308" s="9" t="s">
         <v>815</v>
@@ -13423,9 +13427,41 @@
       <c r="I308" s="10"/>
       <c r="J308" s="10"/>
       <c r="K308" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="L308" s="10" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A309" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B309" s="9" t="s">
+        <v>860</v>
+      </c>
+      <c r="C309" s="9" t="s">
+        <v>815</v>
+      </c>
+      <c r="D309" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="E309" s="12">
+        <v>0</v>
+      </c>
+      <c r="F309" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G309" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H309" s="10"/>
+      <c r="I309" s="10"/>
+      <c r="J309" s="10"/>
+      <c r="K309" s="10" t="s">
         <v>859</v>
       </c>
-      <c r="L308" s="10" t="s">
+      <c r="L309" s="10" t="s">
         <v>859</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes to receiver acceptance angles
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D193B1DB-AD7A-45FE-8192-2B5D9758AD41}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE9834E-415A-46D6-9701-802C76B9C6DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="8220" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3443,8 +3443,8 @@
   <dimension ref="A1:L309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B254" sqref="B254"/>
+      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10483,7 +10483,7 @@
         <v>805</v>
       </c>
       <c r="E218" s="12">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="F218" s="11" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
field plot receiver color support
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwagner\Documents\NREL\projects\SolarPILOT\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD95DE2-4884-48F4-B22B-4828B95AAF74}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C78A1B-BC61-429A-9242-C7566D876F54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="961">
   <si>
     <t>Domain</t>
   </si>
@@ -2902,6 +2902,18 @@
   </si>
   <si>
     <t>Correction of circumsolar ratio based on energy balance</t>
+  </si>
+  <si>
+    <t>map_color</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>Specified receiver map color</t>
+  </si>
+  <si>
+    <t>Specified receiver map color (hex)</t>
   </si>
 </sst>
 </file>
@@ -2998,8 +3010,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L313" totalsRowShown="0">
-  <autoFilter ref="A1:L313" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L314" totalsRowShown="0">
+  <autoFilter ref="A1:L314" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="String name"/>
@@ -3315,11 +3327,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L313"/>
+  <dimension ref="A1:L314"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G262" sqref="G262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11224,26 +11236,28 @@
         <v>666</v>
       </c>
       <c r="B258" t="s">
-        <v>780</v>
+        <v>957</v>
       </c>
       <c r="C258" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="D258" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>958</v>
       </c>
       <c r="F258" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G258" s="2" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="K258" s="3" t="s">
-        <v>781</v>
+        <v>959</v>
       </c>
       <c r="L258" s="3" t="s">
-        <v>781</v>
+        <v>960</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
@@ -11251,29 +11265,26 @@
         <v>666</v>
       </c>
       <c r="B259" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C259" t="s">
         <v>90</v>
       </c>
       <c r="D259" t="s">
-        <v>30</v>
-      </c>
-      <c r="E259" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F259" s="2" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="G259" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="K259" s="3" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="L259" s="3" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
@@ -11281,7 +11292,7 @@
         <v>666</v>
       </c>
       <c r="B260" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C260" t="s">
         <v>90</v>
@@ -11290,20 +11301,20 @@
         <v>30</v>
       </c>
       <c r="E260" s="1">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="F260" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="G260" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K260" t="s">
-        <v>786</v>
+      <c r="K260" s="3" t="s">
+        <v>783</v>
       </c>
       <c r="L260" s="3" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
@@ -11311,7 +11322,7 @@
         <v>666</v>
       </c>
       <c r="B261" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C261" t="s">
         <v>90</v>
@@ -11320,20 +11331,20 @@
         <v>30</v>
       </c>
       <c r="E261" s="1">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="F261" s="2" t="s">
-        <v>789</v>
+        <v>43</v>
       </c>
       <c r="G261" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K261" s="3" t="s">
-        <v>790</v>
+      <c r="K261" t="s">
+        <v>786</v>
       </c>
       <c r="L261" s="3" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
@@ -11341,7 +11352,7 @@
         <v>666</v>
       </c>
       <c r="B262" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C262" t="s">
         <v>90</v>
@@ -11350,20 +11361,20 @@
         <v>30</v>
       </c>
       <c r="E262" s="1">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="F262" s="2" t="s">
-        <v>17</v>
+        <v>789</v>
       </c>
       <c r="G262" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K262" s="3" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="L262" s="3" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
@@ -11371,7 +11382,7 @@
         <v>666</v>
       </c>
       <c r="B263" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C263" t="s">
         <v>90</v>
@@ -11380,20 +11391,20 @@
         <v>30</v>
       </c>
       <c r="E263" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F263" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G263" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K263" s="3" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="L263" s="3" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
@@ -11401,7 +11412,7 @@
         <v>666</v>
       </c>
       <c r="B264" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C264" t="s">
         <v>90</v>
@@ -11413,17 +11424,17 @@
         <v>0</v>
       </c>
       <c r="F264" s="2" t="s">
-        <v>789</v>
+        <v>17</v>
       </c>
       <c r="G264" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="K264" s="3" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="L264" s="3" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
@@ -11431,7 +11442,7 @@
         <v>666</v>
       </c>
       <c r="B265" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="C265" t="s">
         <v>90</v>
@@ -11450,10 +11461,10 @@
         <v>0</v>
       </c>
       <c r="K265" s="3" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="L265" s="3" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
@@ -11461,7 +11472,7 @@
         <v>666</v>
       </c>
       <c r="B266" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="C266" t="s">
         <v>90</v>
@@ -11473,17 +11484,17 @@
         <v>0</v>
       </c>
       <c r="F266" s="2" t="s">
-        <v>43</v>
+        <v>789</v>
       </c>
       <c r="G266" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K266" t="s">
-        <v>804</v>
+      <c r="K266" s="3" t="s">
+        <v>801</v>
       </c>
       <c r="L266" s="3" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
@@ -11491,7 +11502,7 @@
         <v>666</v>
       </c>
       <c r="B267" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="C267" t="s">
         <v>90</v>
@@ -11510,10 +11521,10 @@
         <v>0</v>
       </c>
       <c r="K267" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="L267" s="3" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
@@ -11521,7 +11532,7 @@
         <v>666</v>
       </c>
       <c r="B268" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C268" t="s">
         <v>90</v>
@@ -11540,40 +11551,40 @@
         <v>0</v>
       </c>
       <c r="K268" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="L268" s="3" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>812</v>
+        <v>666</v>
       </c>
       <c r="B269" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="C269" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="D269" t="s">
         <v>30</v>
       </c>
       <c r="E269" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F269" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G269" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K269" s="3" t="s">
-        <v>814</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K269" t="s">
+        <v>810</v>
       </c>
       <c r="L269" s="3" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
@@ -11581,7 +11592,7 @@
         <v>812</v>
       </c>
       <c r="B270" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C270" t="s">
         <v>14</v>
@@ -11590,7 +11601,7 @@
         <v>30</v>
       </c>
       <c r="E270" s="1">
-        <v>-180</v>
+        <v>180</v>
       </c>
       <c r="F270" s="2" t="s">
         <v>51</v>
@@ -11600,10 +11611,10 @@
         <v>1</v>
       </c>
       <c r="K270" s="3" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="L270" s="3" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
@@ -11611,7 +11622,7 @@
         <v>812</v>
       </c>
       <c r="B271" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="C271" t="s">
         <v>14</v>
@@ -11620,20 +11631,20 @@
         <v>30</v>
       </c>
       <c r="E271" s="1">
-        <v>2</v>
+        <v>-180</v>
       </c>
       <c r="F271" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G271" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K271" t="s">
-        <v>820</v>
+      <c r="K271" s="3" t="s">
+        <v>817</v>
       </c>
       <c r="L271" s="3" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
@@ -11641,29 +11652,29 @@
         <v>812</v>
       </c>
       <c r="B272" t="s">
-        <v>26</v>
+        <v>819</v>
       </c>
       <c r="C272" t="s">
         <v>14</v>
       </c>
       <c r="D272" t="s">
-        <v>21</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>822</v>
+        <v>30</v>
+      </c>
+      <c r="E272" s="1">
+        <v>2</v>
       </c>
       <c r="F272" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G272" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K272" s="3" t="s">
-        <v>28</v>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K272" t="s">
+        <v>820</v>
       </c>
       <c r="L272" s="3" t="s">
-        <v>28</v>
+        <v>821</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
@@ -11671,7 +11682,7 @@
         <v>812</v>
       </c>
       <c r="B273" t="s">
-        <v>823</v>
+        <v>26</v>
       </c>
       <c r="C273" t="s">
         <v>14</v>
@@ -11679,27 +11690,21 @@
       <c r="D273" t="s">
         <v>21</v>
       </c>
-      <c r="E273" s="1">
-        <v>5</v>
+      <c r="E273" s="1" t="s">
+        <v>822</v>
       </c>
       <c r="F273" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G273" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H273" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I273" s="3" t="s">
-        <v>824</v>
-      </c>
-      <c r="K273" t="s">
-        <v>825</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K273" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="L273" s="3" t="s">
-        <v>826</v>
+        <v>28</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
@@ -11707,16 +11712,16 @@
         <v>812</v>
       </c>
       <c r="B274" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C274" t="s">
         <v>14</v>
       </c>
       <c r="D274" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
       <c r="E274" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F274" s="2" t="s">
         <v>17</v>
@@ -11725,11 +11730,17 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K274" s="3" t="s">
-        <v>828</v>
+      <c r="H274" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I274" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="K274" t="s">
+        <v>825</v>
       </c>
       <c r="L274" s="3" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">
@@ -11737,7 +11748,7 @@
         <v>812</v>
       </c>
       <c r="B275" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C275" t="s">
         <v>14</v>
@@ -11746,7 +11757,7 @@
         <v>228</v>
       </c>
       <c r="E275" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F275" s="2" t="s">
         <v>17</v>
@@ -11756,10 +11767,10 @@
         <v>1</v>
       </c>
       <c r="K275" s="3" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="L275" s="3" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
@@ -11767,29 +11778,29 @@
         <v>812</v>
       </c>
       <c r="B276" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="C276" t="s">
         <v>14</v>
       </c>
       <c r="D276" t="s">
-        <v>30</v>
+        <v>228</v>
       </c>
       <c r="E276" s="1">
-        <v>950</v>
+        <v>2</v>
       </c>
       <c r="F276" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G276" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K276" s="3" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="L276" s="3" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
@@ -11797,35 +11808,29 @@
         <v>812</v>
       </c>
       <c r="B277" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C277" t="s">
         <v>14</v>
       </c>
       <c r="D277" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E277" s="1">
-        <v>7</v>
+        <v>950</v>
       </c>
       <c r="F277" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="G277" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H277" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I277" s="3" t="s">
-        <v>837</v>
-      </c>
       <c r="K277" s="3" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="L277" s="3" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
@@ -11833,17 +11838,16 @@
         <v>812</v>
       </c>
       <c r="B278" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C278" t="s">
         <v>14</v>
       </c>
       <c r="D278" t="s">
-        <v>111</v>
-      </c>
-      <c r="E278" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="E278" s="1">
+        <v>7</v>
       </c>
       <c r="F278" s="2" t="s">
         <v>17</v>
@@ -11853,13 +11857,16 @@
         <v>1</v>
       </c>
       <c r="H278" s="3" t="s">
-        <v>112</v>
+        <v>22</v>
+      </c>
+      <c r="I278" s="3" t="s">
+        <v>837</v>
       </c>
       <c r="K278" s="3" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="L278" s="3" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
@@ -11867,7 +11874,7 @@
         <v>812</v>
       </c>
       <c r="B279" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C279" t="s">
         <v>14</v>
@@ -11876,24 +11883,24 @@
         <v>111</v>
       </c>
       <c r="E279" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F279" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G279" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H279" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K279" s="3" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="L279" s="3" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.25">
@@ -11901,7 +11908,7 @@
         <v>812</v>
       </c>
       <c r="B280" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C280" t="s">
         <v>14</v>
@@ -11910,24 +11917,24 @@
         <v>111</v>
       </c>
       <c r="E280" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F280" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G280" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H280" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K280" s="3" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="L280" s="3" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">
@@ -11935,7 +11942,7 @@
         <v>812</v>
       </c>
       <c r="B281" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="C281" t="s">
         <v>14</v>
@@ -11944,24 +11951,24 @@
         <v>111</v>
       </c>
       <c r="E281" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F281" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G281" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H281" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K281" s="3" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="L281" s="3" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.25">
@@ -11969,7 +11976,7 @@
         <v>812</v>
       </c>
       <c r="B282" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="C282" t="s">
         <v>14</v>
@@ -11978,24 +11985,24 @@
         <v>111</v>
       </c>
       <c r="E282" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F282" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G282" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H282" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K282" s="3" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="L282" s="3" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.25">
@@ -12003,23 +12010,33 @@
         <v>812</v>
       </c>
       <c r="B283" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="C283" t="s">
         <v>14</v>
       </c>
       <c r="D283" t="s">
-        <v>21</v>
+        <v>111</v>
+      </c>
+      <c r="E283" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F283" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G283" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H283" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="K283" s="3" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="L283" s="3" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.25">
@@ -12027,7 +12044,7 @@
         <v>812</v>
       </c>
       <c r="B284" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C284" t="s">
         <v>14</v>
@@ -12035,27 +12052,15 @@
       <c r="D284" t="s">
         <v>21</v>
       </c>
-      <c r="E284" s="1">
-        <v>0</v>
-      </c>
-      <c r="F284" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G284" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H284" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I284" s="3" t="s">
-        <v>858</v>
-      </c>
-      <c r="K284" t="s">
-        <v>859</v>
+      <c r="K284" s="3" t="s">
+        <v>856</v>
       </c>
       <c r="L284" s="3" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.25">
@@ -12063,29 +12068,35 @@
         <v>812</v>
       </c>
       <c r="B285" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="C285" t="s">
         <v>14</v>
       </c>
       <c r="D285" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E285" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F285" s="2" t="s">
-        <v>862</v>
+        <v>17</v>
       </c>
       <c r="G285" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K285" s="3" t="s">
-        <v>863</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H285" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I285" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="K285" t="s">
+        <v>859</v>
       </c>
       <c r="L285" s="3" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
@@ -12093,7 +12104,7 @@
         <v>812</v>
       </c>
       <c r="B286" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="C286" t="s">
         <v>14</v>
@@ -12112,10 +12123,10 @@
         <v>1</v>
       </c>
       <c r="K286" s="3" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="L286" s="3" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
@@ -12123,7 +12134,7 @@
         <v>812</v>
       </c>
       <c r="B287" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="C287" t="s">
         <v>14</v>
@@ -12132,7 +12143,7 @@
         <v>30</v>
       </c>
       <c r="E287" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F287" s="2" t="s">
         <v>862</v>
@@ -12142,10 +12153,10 @@
         <v>1</v>
       </c>
       <c r="K287" s="3" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="L287" s="3" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
@@ -12153,7 +12164,7 @@
         <v>812</v>
       </c>
       <c r="B288" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="C288" t="s">
         <v>14</v>
@@ -12172,10 +12183,10 @@
         <v>1</v>
       </c>
       <c r="K288" s="3" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="L288" s="3" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -12183,7 +12194,7 @@
         <v>812</v>
       </c>
       <c r="B289" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="C289" t="s">
         <v>14</v>
@@ -12192,20 +12203,20 @@
         <v>30</v>
       </c>
       <c r="E289" s="1">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F289" s="2" t="s">
-        <v>17</v>
+        <v>862</v>
       </c>
       <c r="G289" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K289" s="3" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="L289" s="3" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
@@ -12213,7 +12224,7 @@
         <v>812</v>
       </c>
       <c r="B290" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="C290" t="s">
         <v>14</v>
@@ -12222,20 +12233,20 @@
         <v>30</v>
       </c>
       <c r="E290" s="1">
-        <v>670</v>
+        <v>0.03</v>
       </c>
       <c r="F290" s="2" t="s">
-        <v>878</v>
+        <v>17</v>
       </c>
       <c r="G290" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K290" t="s">
-        <v>879</v>
+      <c r="K290" s="3" t="s">
+        <v>875</v>
       </c>
       <c r="L290" s="3" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
@@ -12243,35 +12254,29 @@
         <v>812</v>
       </c>
       <c r="B291" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="C291" t="s">
         <v>14</v>
       </c>
       <c r="D291" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E291" s="1">
-        <v>0</v>
+        <v>670</v>
       </c>
       <c r="F291" s="2" t="s">
-        <v>17</v>
+        <v>878</v>
       </c>
       <c r="G291" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H291" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I291" s="3" t="s">
-        <v>882</v>
-      </c>
       <c r="K291" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="L291" s="3" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
@@ -12279,16 +12284,16 @@
         <v>812</v>
       </c>
       <c r="B292" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="C292" t="s">
         <v>14</v>
       </c>
       <c r="D292" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E292" s="1">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F292" s="2" t="s">
         <v>17</v>
@@ -12297,11 +12302,17 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K292" s="3" t="s">
-        <v>886</v>
+      <c r="H292" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I292" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="K292" t="s">
+        <v>883</v>
       </c>
       <c r="L292" s="3" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
@@ -12309,7 +12320,7 @@
         <v>812</v>
       </c>
       <c r="B293" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="C293" t="s">
         <v>14</v>
@@ -12328,10 +12339,10 @@
         <v>1</v>
       </c>
       <c r="K293" s="3" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="L293" s="3" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
@@ -12339,7 +12350,7 @@
         <v>812</v>
       </c>
       <c r="B294" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="C294" t="s">
         <v>14</v>
@@ -12348,20 +12359,20 @@
         <v>30</v>
       </c>
       <c r="E294" s="1">
-        <v>195</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F294" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G294" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K294" t="s">
-        <v>892</v>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K294" s="3" t="s">
+        <v>889</v>
       </c>
       <c r="L294" s="3" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
@@ -12369,7 +12380,7 @@
         <v>812</v>
       </c>
       <c r="B295" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="C295" t="s">
         <v>14</v>
@@ -12378,7 +12389,7 @@
         <v>30</v>
       </c>
       <c r="E295" s="1">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="F295" s="2" t="s">
         <v>43</v>
@@ -12388,10 +12399,10 @@
         <v>0</v>
       </c>
       <c r="K295" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="L295" s="3" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
@@ -12399,7 +12410,7 @@
         <v>812</v>
       </c>
       <c r="B296" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="C296" t="s">
         <v>14</v>
@@ -12408,20 +12419,20 @@
         <v>30</v>
       </c>
       <c r="E296" s="1">
-        <v>0.5</v>
+        <v>16</v>
       </c>
       <c r="F296" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G296" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K296" s="3" t="s">
-        <v>898</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K296" t="s">
+        <v>895</v>
       </c>
       <c r="L296" s="3" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.25">
@@ -12429,7 +12440,7 @@
         <v>812</v>
       </c>
       <c r="B297" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C297" t="s">
         <v>14</v>
@@ -12438,7 +12449,7 @@
         <v>30</v>
       </c>
       <c r="E297" s="1">
-        <v>1.33</v>
+        <v>0.5</v>
       </c>
       <c r="F297" s="2" t="s">
         <v>17</v>
@@ -12447,11 +12458,11 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K297" t="s">
-        <v>900</v>
+      <c r="K297" s="3" t="s">
+        <v>898</v>
       </c>
       <c r="L297" s="3" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.25">
@@ -12459,7 +12470,7 @@
         <v>812</v>
       </c>
       <c r="B298" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="C298" t="s">
         <v>14</v>
@@ -12468,20 +12479,20 @@
         <v>30</v>
       </c>
       <c r="E298" s="1">
-        <v>180</v>
+        <v>1.33</v>
       </c>
       <c r="F298" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="G298" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K298" s="3" t="s">
-        <v>903</v>
+      <c r="K298" t="s">
+        <v>900</v>
       </c>
       <c r="L298" s="3" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
@@ -12489,7 +12500,7 @@
         <v>812</v>
       </c>
       <c r="B299" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C299" t="s">
         <v>14</v>
@@ -12498,7 +12509,7 @@
         <v>30</v>
       </c>
       <c r="E299" s="1">
-        <v>85</v>
+        <v>180</v>
       </c>
       <c r="F299" s="2" t="s">
         <v>51</v>
@@ -12508,10 +12519,10 @@
         <v>1</v>
       </c>
       <c r="K299" s="3" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="L299" s="3" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.25">
@@ -12519,35 +12530,29 @@
         <v>812</v>
       </c>
       <c r="B300" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="C300" t="s">
         <v>14</v>
       </c>
       <c r="D300" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E300" s="1">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F300" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G300" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H300" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I300" s="3" t="s">
-        <v>909</v>
-      </c>
       <c r="K300" s="3" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="L300" s="3" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.25">
@@ -12555,7 +12560,7 @@
         <v>812</v>
       </c>
       <c r="B301" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="C301" t="s">
         <v>14</v>
@@ -12576,11 +12581,14 @@
       <c r="H301" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="I301" s="3" t="s">
+        <v>909</v>
+      </c>
       <c r="K301" s="3" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="L301" s="3" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.25">
@@ -12588,7 +12596,7 @@
         <v>812</v>
       </c>
       <c r="B302" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="C302" t="s">
         <v>14</v>
@@ -12599,6 +12607,9 @@
       <c r="E302" s="1">
         <v>0</v>
       </c>
+      <c r="F302" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G302" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
@@ -12606,14 +12617,11 @@
       <c r="H302" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I302" s="3" t="s">
-        <v>916</v>
-      </c>
       <c r="K302" s="3" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="L302" s="3" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.25">
@@ -12621,29 +12629,32 @@
         <v>812</v>
       </c>
       <c r="B303" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="C303" t="s">
         <v>14</v>
       </c>
       <c r="D303" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E303" s="1">
-        <v>195</v>
-      </c>
-      <c r="F303" s="2" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="G303" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K303" t="s">
-        <v>920</v>
+      <c r="H303" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I303" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="K303" s="3" t="s">
+        <v>917</v>
       </c>
       <c r="L303" s="3" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.25">
@@ -12651,7 +12662,7 @@
         <v>812</v>
       </c>
       <c r="B304" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="C304" t="s">
         <v>14</v>
@@ -12660,20 +12671,20 @@
         <v>30</v>
       </c>
       <c r="E304" s="1">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="F304" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G304" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K304" s="3" t="s">
-        <v>923</v>
+      <c r="K304" t="s">
+        <v>920</v>
       </c>
       <c r="L304" s="3" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.25">
@@ -12681,32 +12692,29 @@
         <v>812</v>
       </c>
       <c r="B305" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="C305" t="s">
         <v>14</v>
       </c>
       <c r="D305" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E305" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F305" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G305" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H305" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I305" s="3" t="s">
-        <v>926</v>
-      </c>
       <c r="K305" s="3" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="L305" s="3" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.25">
@@ -12714,29 +12722,32 @@
         <v>812</v>
       </c>
       <c r="B306" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="C306" t="s">
         <v>14</v>
       </c>
       <c r="D306" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E306" s="1">
-        <v>1</v>
-      </c>
-      <c r="F306" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G306" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H306" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I306" s="3" t="s">
+        <v>926</v>
+      </c>
       <c r="K306" s="3" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="L306" s="3" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.25">
@@ -12744,7 +12755,7 @@
         <v>812</v>
       </c>
       <c r="B307" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="C307" t="s">
         <v>14</v>
@@ -12753,7 +12764,7 @@
         <v>30</v>
       </c>
       <c r="E307" s="1">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="F307" s="2" t="s">
         <v>17</v>
@@ -12763,10 +12774,10 @@
         <v>1</v>
       </c>
       <c r="K307" s="3" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="L307" s="3" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.25">
@@ -12774,7 +12785,7 @@
         <v>812</v>
       </c>
       <c r="B308" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C308" t="s">
         <v>14</v>
@@ -12783,20 +12794,20 @@
         <v>30</v>
       </c>
       <c r="E308" s="1">
-        <v>100</v>
+        <v>1E-3</v>
       </c>
       <c r="F308" s="2" t="s">
-        <v>936</v>
+        <v>17</v>
       </c>
       <c r="G308" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K308" s="3" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="L308" s="3" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.25">
@@ -12804,29 +12815,29 @@
         <v>812</v>
       </c>
       <c r="B309" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="C309" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="D309" t="s">
         <v>30</v>
       </c>
       <c r="E309" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F309" s="2" t="s">
-        <v>128</v>
+        <v>936</v>
       </c>
       <c r="G309" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K309" s="3" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="L309" s="3" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.25">
@@ -12834,7 +12845,7 @@
         <v>812</v>
       </c>
       <c r="B310" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="C310" t="s">
         <v>90</v>
@@ -12853,10 +12864,10 @@
         <v>0</v>
       </c>
       <c r="K310" s="3" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="L310" s="3" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.25">
@@ -12864,26 +12875,29 @@
         <v>812</v>
       </c>
       <c r="B311" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="C311" t="s">
         <v>90</v>
       </c>
       <c r="D311" t="s">
-        <v>87</v>
+        <v>30</v>
+      </c>
+      <c r="E311" s="1">
+        <v>0</v>
       </c>
       <c r="F311" s="2" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="G311" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="K311" s="3" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="L311" s="3" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.25">
@@ -12891,29 +12905,26 @@
         <v>812</v>
       </c>
       <c r="B312" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C312" t="s">
         <v>90</v>
       </c>
       <c r="D312" t="s">
-        <v>30</v>
-      </c>
-      <c r="E312" s="1">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="F312" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="G312" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="K312" s="3" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="L312" s="3" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.25">
@@ -12921,7 +12932,7 @@
         <v>812</v>
       </c>
       <c r="B313" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C313" t="s">
         <v>90</v>
@@ -12940,9 +12951,39 @@
         <v>0</v>
       </c>
       <c r="K313" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="L313" s="3" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>812</v>
+      </c>
+      <c r="B314" t="s">
+        <v>949</v>
+      </c>
+      <c r="C314" t="s">
+        <v>90</v>
+      </c>
+      <c r="D314" t="s">
+        <v>30</v>
+      </c>
+      <c r="E314" s="1">
+        <v>0</v>
+      </c>
+      <c r="F314" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G314" s="2" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K314" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="L313" s="3" t="s">
+      <c r="L314" s="3" t="s">
         <v>950</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testing modify_heliostat function after updates
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwagner\Documents\NREL\projects\SolarPILOT\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WHamilt2\Documents\solarPILOT_build\SolarPILOT\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C78A1B-BC61-429A-9242-C7566D876F54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF09015-F0DF-4886-92C0-54242CCE2AFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="963">
   <si>
     <t>Domain</t>
   </si>
@@ -2914,6 +2916,12 @@
   </si>
   <si>
     <t>Specified receiver map color (hex)</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>SolarPILOT code base version number</t>
   </si>
 </sst>
 </file>
@@ -3010,8 +3018,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L314" totalsRowShown="0">
-  <autoFilter ref="A1:L314" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L315" totalsRowShown="0">
+  <autoFilter ref="A1:L315" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Domain"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="String name"/>
@@ -3327,31 +3335,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L314"/>
+  <dimension ref="A1:L315"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G262" sqref="G262"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="114.42578125" customWidth="1"/>
-    <col min="13" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="39.54296875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="114.453125" customWidth="1"/>
+    <col min="13" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3389,7 +3397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3422,7 +3430,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3458,7 +3466,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3488,7 +3496,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3518,7 +3526,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3548,7 +3556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3578,7 +3586,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3608,7 +3616,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3644,7 +3652,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3674,7 +3682,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3704,7 +3712,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3734,7 +3742,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3764,7 +3772,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3794,7 +3802,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3821,7 +3829,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3851,7 +3859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3887,7 +3895,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3917,7 +3925,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3944,7 +3952,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3974,7 +3982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4001,7 +4009,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4030,7 +4038,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -4060,7 +4068,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4090,7 +4098,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -4120,7 +4128,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -4150,7 +4158,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -4180,7 +4188,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -4210,7 +4218,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -4241,7 +4249,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -4271,7 +4279,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -4301,7 +4309,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -4331,7 +4339,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -4361,7 +4369,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -4391,7 +4399,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -4421,7 +4429,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -4451,7 +4459,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -4481,7 +4489,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -4511,7 +4519,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -4541,7 +4549,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -4568,7 +4576,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -4595,7 +4603,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -4625,7 +4633,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -4655,7 +4663,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -4685,7 +4693,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>97</v>
       </c>
@@ -4715,7 +4723,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -4745,7 +4753,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -4775,7 +4783,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -4805,7 +4813,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -4835,7 +4843,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -4865,7 +4873,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -4895,7 +4903,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -4925,7 +4933,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -4955,7 +4963,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>97</v>
       </c>
@@ -4985,7 +4993,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>97</v>
       </c>
@@ -5015,7 +5023,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>190</v>
       </c>
@@ -5048,7 +5056,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>190</v>
       </c>
@@ -5078,7 +5086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -5108,7 +5116,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>190</v>
       </c>
@@ -5138,7 +5146,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>190</v>
       </c>
@@ -5168,7 +5176,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>190</v>
       </c>
@@ -5198,7 +5206,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>190</v>
       </c>
@@ -5225,7 +5233,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>190</v>
       </c>
@@ -5252,7 +5260,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -5285,7 +5293,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>190</v>
       </c>
@@ -5315,7 +5323,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -5345,7 +5353,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>190</v>
       </c>
@@ -5369,7 +5377,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>190</v>
       </c>
@@ -5396,7 +5404,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>190</v>
       </c>
@@ -5429,7 +5437,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -5459,7 +5467,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>190</v>
       </c>
@@ -5489,7 +5497,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -5525,7 +5533,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>190</v>
       </c>
@@ -5552,7 +5560,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>190</v>
       </c>
@@ -5579,7 +5587,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>190</v>
       </c>
@@ -5606,7 +5614,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>190</v>
       </c>
@@ -5642,7 +5650,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>190</v>
       </c>
@@ -5676,7 +5684,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>190</v>
       </c>
@@ -5707,7 +5715,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>190</v>
       </c>
@@ -5738,7 +5746,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -5769,7 +5777,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>190</v>
       </c>
@@ -5800,7 +5808,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>190</v>
       </c>
@@ -5837,7 +5845,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -5868,7 +5876,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -5905,7 +5913,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>190</v>
       </c>
@@ -5936,7 +5944,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>190</v>
       </c>
@@ -5966,7 +5974,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>190</v>
       </c>
@@ -5996,7 +6004,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>190</v>
       </c>
@@ -6023,7 +6031,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>190</v>
       </c>
@@ -6053,7 +6061,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>190</v>
       </c>
@@ -6083,7 +6091,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>190</v>
       </c>
@@ -6119,7 +6127,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>190</v>
       </c>
@@ -6150,7 +6158,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -6177,7 +6185,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>190</v>
       </c>
@@ -6207,7 +6215,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>190</v>
       </c>
@@ -6234,7 +6242,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -6264,7 +6272,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -6291,10 +6299,10 @@
         <v>323</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>190</v>
       </c>
@@ -6321,10 +6329,10 @@
         <v>326</v>
       </c>
       <c r="L98" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>190</v>
       </c>
@@ -6353,7 +6361,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>190</v>
       </c>
@@ -6383,7 +6391,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>190</v>
       </c>
@@ -6413,7 +6421,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>332</v>
       </c>
@@ -6443,7 +6451,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>332</v>
       </c>
@@ -6473,7 +6481,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>332</v>
       </c>
@@ -6509,7 +6517,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>332</v>
       </c>
@@ -6539,7 +6547,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>332</v>
       </c>
@@ -6569,7 +6577,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>332</v>
       </c>
@@ -6599,7 +6607,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>332</v>
       </c>
@@ -6629,7 +6637,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>332</v>
       </c>
@@ -6659,7 +6667,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>332</v>
       </c>
@@ -6689,7 +6697,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>332</v>
       </c>
@@ -6719,7 +6727,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>332</v>
       </c>
@@ -6749,7 +6757,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>332</v>
       </c>
@@ -6779,7 +6787,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>332</v>
       </c>
@@ -6809,7 +6817,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>332</v>
       </c>
@@ -6839,7 +6847,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>332</v>
       </c>
@@ -6869,7 +6877,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>332</v>
       </c>
@@ -6899,7 +6907,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>332</v>
       </c>
@@ -6929,7 +6937,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>332</v>
       </c>
@@ -6965,7 +6973,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>332</v>
       </c>
@@ -7001,7 +7009,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>332</v>
       </c>
@@ -7031,7 +7039,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>332</v>
       </c>
@@ -7058,7 +7066,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>332</v>
       </c>
@@ -7088,7 +7096,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>332</v>
       </c>
@@ -7119,7 +7127,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>332</v>
       </c>
@@ -7153,7 +7161,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>332</v>
       </c>
@@ -7181,7 +7189,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>332</v>
       </c>
@@ -7215,7 +7223,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>332</v>
       </c>
@@ -7249,7 +7257,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>332</v>
       </c>
@@ -7285,7 +7293,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>332</v>
       </c>
@@ -7319,7 +7327,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>332</v>
       </c>
@@ -7353,7 +7361,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>332</v>
       </c>
@@ -7380,7 +7388,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>332</v>
       </c>
@@ -7407,7 +7415,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>332</v>
       </c>
@@ -7437,7 +7445,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>332</v>
       </c>
@@ -7467,7 +7475,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>332</v>
       </c>
@@ -7497,7 +7505,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>332</v>
       </c>
@@ -7527,7 +7535,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>332</v>
       </c>
@@ -7557,7 +7565,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>332</v>
       </c>
@@ -7587,7 +7595,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>332</v>
       </c>
@@ -7617,7 +7625,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>332</v>
       </c>
@@ -7647,7 +7655,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>332</v>
       </c>
@@ -7677,7 +7685,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>332</v>
       </c>
@@ -7707,7 +7715,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>332</v>
       </c>
@@ -7746,7 +7754,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>332</v>
       </c>
@@ -7779,7 +7787,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>332</v>
       </c>
@@ -7806,7 +7814,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>332</v>
       </c>
@@ -7836,7 +7844,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>332</v>
       </c>
@@ -7866,7 +7874,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>332</v>
       </c>
@@ -7896,7 +7904,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>332</v>
       </c>
@@ -7926,7 +7934,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>332</v>
       </c>
@@ -7956,7 +7964,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>332</v>
       </c>
@@ -7986,7 +7994,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>332</v>
       </c>
@@ -8016,7 +8024,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>332</v>
       </c>
@@ -8046,7 +8054,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>332</v>
       </c>
@@ -8076,7 +8084,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>332</v>
       </c>
@@ -8106,7 +8114,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>332</v>
       </c>
@@ -8136,7 +8144,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>332</v>
       </c>
@@ -8166,7 +8174,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>332</v>
       </c>
@@ -8196,7 +8204,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>332</v>
       </c>
@@ -8226,7 +8234,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>332</v>
       </c>
@@ -8256,7 +8264,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>332</v>
       </c>
@@ -8286,7 +8294,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>332</v>
       </c>
@@ -8316,7 +8324,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>332</v>
       </c>
@@ -8346,7 +8354,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>513</v>
       </c>
@@ -8376,7 +8384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>513</v>
       </c>
@@ -8400,7 +8408,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>513</v>
       </c>
@@ -8430,7 +8438,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>513</v>
       </c>
@@ -8460,7 +8468,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>513</v>
       </c>
@@ -8491,7 +8499,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>513</v>
       </c>
@@ -8515,7 +8523,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>513</v>
       </c>
@@ -8549,7 +8557,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>513</v>
       </c>
@@ -8583,7 +8591,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>513</v>
       </c>
@@ -8617,7 +8625,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>513</v>
       </c>
@@ -8651,7 +8659,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>513</v>
       </c>
@@ -8681,7 +8689,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>513</v>
       </c>
@@ -8711,7 +8719,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>513</v>
       </c>
@@ -8741,7 +8749,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>513</v>
       </c>
@@ -8771,7 +8779,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>513</v>
       </c>
@@ -8801,7 +8809,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>513</v>
       </c>
@@ -8831,7 +8839,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>513</v>
       </c>
@@ -8861,7 +8869,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>513</v>
       </c>
@@ -8891,7 +8899,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>513</v>
       </c>
@@ -8921,7 +8929,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>513</v>
       </c>
@@ -8951,7 +8959,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>513</v>
       </c>
@@ -8981,7 +8989,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>513</v>
       </c>
@@ -9011,7 +9019,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>576</v>
       </c>
@@ -9047,7 +9055,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>576</v>
       </c>
@@ -9069,7 +9077,7 @@
       </c>
       <c r="L188" s="3"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>576</v>
       </c>
@@ -9099,7 +9107,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>576</v>
       </c>
@@ -9132,7 +9140,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>576</v>
       </c>
@@ -9165,7 +9173,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>576</v>
       </c>
@@ -9198,7 +9206,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>576</v>
       </c>
@@ -9228,7 +9236,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>576</v>
       </c>
@@ -9258,7 +9266,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>576</v>
       </c>
@@ -9288,7 +9296,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>576</v>
       </c>
@@ -9318,7 +9326,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>576</v>
       </c>
@@ -9348,7 +9356,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>576</v>
       </c>
@@ -9375,7 +9383,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>576</v>
       </c>
@@ -9405,7 +9413,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>576</v>
       </c>
@@ -9438,7 +9446,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>576</v>
       </c>
@@ -9470,7 +9478,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>619</v>
       </c>
@@ -9500,7 +9508,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>619</v>
       </c>
@@ -9527,7 +9535,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>619</v>
       </c>
@@ -9554,7 +9562,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>619</v>
       </c>
@@ -9587,7 +9595,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>619</v>
       </c>
@@ -9618,7 +9626,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>619</v>
       </c>
@@ -9652,7 +9660,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>619</v>
       </c>
@@ -9686,7 +9694,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>619</v>
       </c>
@@ -9720,7 +9728,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>619</v>
       </c>
@@ -9754,7 +9762,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>619</v>
       </c>
@@ -9788,7 +9796,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>619</v>
       </c>
@@ -9822,7 +9830,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>619</v>
       </c>
@@ -9856,7 +9864,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>619</v>
       </c>
@@ -9890,7 +9898,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>619</v>
       </c>
@@ -9924,7 +9932,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>619</v>
       </c>
@@ -9958,7 +9966,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>619</v>
       </c>
@@ -9982,7 +9990,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>619</v>
       </c>
@@ -10009,7 +10017,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>619</v>
       </c>
@@ -10045,7 +10053,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>666</v>
       </c>
@@ -10075,7 +10083,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>666</v>
       </c>
@@ -10111,7 +10119,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>666</v>
       </c>
@@ -10141,7 +10149,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>666</v>
       </c>
@@ -10171,7 +10179,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>666</v>
       </c>
@@ -10204,7 +10212,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>666</v>
       </c>
@@ -10234,7 +10242,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>666</v>
       </c>
@@ -10264,7 +10272,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>666</v>
       </c>
@@ -10291,7 +10299,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>666</v>
       </c>
@@ -10322,7 +10330,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>666</v>
       </c>
@@ -10350,7 +10358,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>666</v>
       </c>
@@ -10384,7 +10392,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>666</v>
       </c>
@@ -10418,7 +10426,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>666</v>
       </c>
@@ -10451,7 +10459,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>666</v>
       </c>
@@ -10484,7 +10492,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>666</v>
       </c>
@@ -10514,7 +10522,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>666</v>
       </c>
@@ -10550,7 +10558,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>666</v>
       </c>
@@ -10580,7 +10588,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>666</v>
       </c>
@@ -10610,7 +10618,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>666</v>
       </c>
@@ -10640,7 +10648,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>666</v>
       </c>
@@ -10670,7 +10678,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>666</v>
       </c>
@@ -10700,7 +10708,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>666</v>
       </c>
@@ -10733,7 +10741,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>666</v>
       </c>
@@ -10766,7 +10774,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>666</v>
       </c>
@@ -10796,7 +10804,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>666</v>
       </c>
@@ -10826,7 +10834,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>666</v>
       </c>
@@ -10856,7 +10864,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>666</v>
       </c>
@@ -10883,7 +10891,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>666</v>
       </c>
@@ -10913,7 +10921,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>666</v>
       </c>
@@ -10943,7 +10951,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>666</v>
       </c>
@@ -10973,7 +10981,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>666</v>
       </c>
@@ -11009,7 +11017,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>666</v>
       </c>
@@ -11045,7 +11053,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>666</v>
       </c>
@@ -11075,7 +11083,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>666</v>
       </c>
@@ -11108,7 +11116,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>666</v>
       </c>
@@ -11141,7 +11149,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>666</v>
       </c>
@@ -11171,7 +11179,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>666</v>
       </c>
@@ -11201,7 +11209,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>666</v>
       </c>
@@ -11231,7 +11239,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>666</v>
       </c>
@@ -11260,7 +11268,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>666</v>
       </c>
@@ -11287,7 +11295,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>666</v>
       </c>
@@ -11317,7 +11325,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>666</v>
       </c>
@@ -11347,7 +11355,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>666</v>
       </c>
@@ -11377,7 +11385,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>666</v>
       </c>
@@ -11407,7 +11415,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>666</v>
       </c>
@@ -11437,7 +11445,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>666</v>
       </c>
@@ -11467,7 +11475,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>666</v>
       </c>
@@ -11497,7 +11505,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>666</v>
       </c>
@@ -11527,7 +11535,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>666</v>
       </c>
@@ -11557,7 +11565,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>666</v>
       </c>
@@ -11587,42 +11595,35 @@
         <v>811</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>812</v>
       </c>
       <c r="B270" t="s">
-        <v>813</v>
+        <v>961</v>
       </c>
       <c r="C270" t="s">
         <v>14</v>
       </c>
       <c r="D270" t="s">
-        <v>30</v>
-      </c>
-      <c r="E270" s="1">
-        <v>180</v>
-      </c>
-      <c r="F270" s="2" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G270" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K270" s="3" t="s">
-        <v>814</v>
-      </c>
-      <c r="L270" s="3" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K270" t="s">
+        <v>962</v>
+      </c>
+      <c r="L270" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>812</v>
       </c>
       <c r="B271" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C271" t="s">
         <v>14</v>
@@ -11631,7 +11632,7 @@
         <v>30</v>
       </c>
       <c r="E271" s="1">
-        <v>-180</v>
+        <v>180</v>
       </c>
       <c r="F271" s="2" t="s">
         <v>51</v>
@@ -11641,18 +11642,18 @@
         <v>1</v>
       </c>
       <c r="K271" s="3" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="L271" s="3" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>812</v>
       </c>
       <c r="B272" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="C272" t="s">
         <v>14</v>
@@ -11661,58 +11662,58 @@
         <v>30</v>
       </c>
       <c r="E272" s="1">
-        <v>2</v>
+        <v>-180</v>
       </c>
       <c r="F272" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G272" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K272" t="s">
-        <v>820</v>
+      <c r="K272" s="3" t="s">
+        <v>817</v>
       </c>
       <c r="L272" s="3" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>812</v>
       </c>
       <c r="B273" t="s">
-        <v>26</v>
+        <v>819</v>
       </c>
       <c r="C273" t="s">
         <v>14</v>
       </c>
       <c r="D273" t="s">
-        <v>21</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>822</v>
+        <v>30</v>
+      </c>
+      <c r="E273" s="1">
+        <v>2</v>
       </c>
       <c r="F273" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G273" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K273" s="3" t="s">
-        <v>28</v>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K273" t="s">
+        <v>820</v>
       </c>
       <c r="L273" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>812</v>
       </c>
       <c r="B274" t="s">
-        <v>823</v>
+        <v>26</v>
       </c>
       <c r="C274" t="s">
         <v>14</v>
@@ -11720,44 +11721,38 @@
       <c r="D274" t="s">
         <v>21</v>
       </c>
-      <c r="E274" s="1">
-        <v>5</v>
+      <c r="E274" s="1" t="s">
+        <v>822</v>
       </c>
       <c r="F274" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G274" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H274" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I274" s="3" t="s">
-        <v>824</v>
-      </c>
-      <c r="K274" t="s">
-        <v>825</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K274" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="L274" s="3" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>812</v>
       </c>
       <c r="B275" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C275" t="s">
         <v>14</v>
       </c>
       <c r="D275" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
       <c r="E275" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F275" s="2" t="s">
         <v>17</v>
@@ -11766,19 +11761,25 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K275" s="3" t="s">
-        <v>828</v>
+      <c r="H275" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I275" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="K275" t="s">
+        <v>825</v>
       </c>
       <c r="L275" s="3" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>812</v>
       </c>
       <c r="B276" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C276" t="s">
         <v>14</v>
@@ -11787,7 +11788,7 @@
         <v>228</v>
       </c>
       <c r="E276" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F276" s="2" t="s">
         <v>17</v>
@@ -11797,94 +11798,87 @@
         <v>1</v>
       </c>
       <c r="K276" s="3" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="L276" s="3" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>812</v>
       </c>
       <c r="B277" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="C277" t="s">
         <v>14</v>
       </c>
       <c r="D277" t="s">
-        <v>30</v>
+        <v>228</v>
       </c>
       <c r="E277" s="1">
-        <v>950</v>
+        <v>2</v>
       </c>
       <c r="F277" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G277" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K277" s="3" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="L277" s="3" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>812</v>
       </c>
       <c r="B278" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C278" t="s">
         <v>14</v>
       </c>
       <c r="D278" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E278" s="1">
-        <v>7</v>
+        <v>950</v>
       </c>
       <c r="F278" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="G278" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H278" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I278" s="3" t="s">
-        <v>837</v>
-      </c>
       <c r="K278" s="3" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="L278" s="3" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>812</v>
       </c>
       <c r="B279" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C279" t="s">
         <v>14</v>
       </c>
       <c r="D279" t="s">
-        <v>111</v>
-      </c>
-      <c r="E279" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="E279" s="1">
+        <v>7</v>
       </c>
       <c r="F279" s="2" t="s">
         <v>17</v>
@@ -11894,21 +11888,24 @@
         <v>1</v>
       </c>
       <c r="H279" s="3" t="s">
-        <v>112</v>
+        <v>22</v>
+      </c>
+      <c r="I279" s="3" t="s">
+        <v>837</v>
       </c>
       <c r="K279" s="3" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="L279" s="3" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>812</v>
       </c>
       <c r="B280" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C280" t="s">
         <v>14</v>
@@ -11917,32 +11914,32 @@
         <v>111</v>
       </c>
       <c r="E280" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F280" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G280" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H280" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K280" s="3" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="L280" s="3" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>812</v>
       </c>
       <c r="B281" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C281" t="s">
         <v>14</v>
@@ -11951,32 +11948,32 @@
         <v>111</v>
       </c>
       <c r="E281" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F281" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G281" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H281" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K281" s="3" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="L281" s="3" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>812</v>
       </c>
       <c r="B282" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="C282" t="s">
         <v>14</v>
@@ -11985,32 +11982,32 @@
         <v>111</v>
       </c>
       <c r="E282" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F282" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G282" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H282" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K282" s="3" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="L282" s="3" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>812</v>
       </c>
       <c r="B283" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="C283" t="s">
         <v>14</v>
@@ -12019,56 +12016,66 @@
         <v>111</v>
       </c>
       <c r="E283" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F283" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G283" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H283" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K283" s="3" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="L283" s="3" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>812</v>
       </c>
       <c r="B284" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="C284" t="s">
         <v>14</v>
       </c>
       <c r="D284" t="s">
-        <v>21</v>
+        <v>111</v>
+      </c>
+      <c r="E284" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F284" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G284" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H284" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="K284" s="3" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="L284" s="3" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>812</v>
       </c>
       <c r="B285" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C285" t="s">
         <v>14</v>
@@ -12076,65 +12083,59 @@
       <c r="D285" t="s">
         <v>21</v>
       </c>
-      <c r="E285" s="1">
-        <v>0</v>
-      </c>
-      <c r="F285" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G285" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H285" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I285" s="3" t="s">
-        <v>858</v>
-      </c>
-      <c r="K285" t="s">
-        <v>859</v>
+      <c r="K285" s="3" t="s">
+        <v>856</v>
       </c>
       <c r="L285" s="3" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>812</v>
       </c>
       <c r="B286" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="C286" t="s">
         <v>14</v>
       </c>
       <c r="D286" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E286" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F286" s="2" t="s">
-        <v>862</v>
+        <v>17</v>
       </c>
       <c r="G286" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K286" s="3" t="s">
-        <v>863</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H286" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I286" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="K286" t="s">
+        <v>859</v>
       </c>
       <c r="L286" s="3" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>812</v>
       </c>
       <c r="B287" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="C287" t="s">
         <v>14</v>
@@ -12153,18 +12154,18 @@
         <v>1</v>
       </c>
       <c r="K287" s="3" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="L287" s="3" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>812</v>
       </c>
       <c r="B288" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="C288" t="s">
         <v>14</v>
@@ -12173,7 +12174,7 @@
         <v>30</v>
       </c>
       <c r="E288" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F288" s="2" t="s">
         <v>862</v>
@@ -12183,18 +12184,18 @@
         <v>1</v>
       </c>
       <c r="K288" s="3" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="L288" s="3" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>812</v>
       </c>
       <c r="B289" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="C289" t="s">
         <v>14</v>
@@ -12213,18 +12214,18 @@
         <v>1</v>
       </c>
       <c r="K289" s="3" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="L289" s="3" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>812</v>
       </c>
       <c r="B290" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="C290" t="s">
         <v>14</v>
@@ -12233,28 +12234,28 @@
         <v>30</v>
       </c>
       <c r="E290" s="1">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F290" s="2" t="s">
-        <v>17</v>
+        <v>862</v>
       </c>
       <c r="G290" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K290" s="3" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="L290" s="3" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>812</v>
       </c>
       <c r="B291" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="C291" t="s">
         <v>14</v>
@@ -12263,73 +12264,67 @@
         <v>30</v>
       </c>
       <c r="E291" s="1">
-        <v>670</v>
+        <v>0.03</v>
       </c>
       <c r="F291" s="2" t="s">
-        <v>878</v>
+        <v>17</v>
       </c>
       <c r="G291" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K291" t="s">
-        <v>879</v>
+      <c r="K291" s="3" t="s">
+        <v>875</v>
       </c>
       <c r="L291" s="3" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>812</v>
       </c>
       <c r="B292" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="C292" t="s">
         <v>14</v>
       </c>
       <c r="D292" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E292" s="1">
-        <v>0</v>
+        <v>670</v>
       </c>
       <c r="F292" s="2" t="s">
-        <v>17</v>
+        <v>878</v>
       </c>
       <c r="G292" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H292" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I292" s="3" t="s">
-        <v>882</v>
-      </c>
       <c r="K292" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="L292" s="3" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>812</v>
       </c>
       <c r="B293" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="C293" t="s">
         <v>14</v>
       </c>
       <c r="D293" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E293" s="1">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F293" s="2" t="s">
         <v>17</v>
@@ -12338,19 +12333,25 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K293" s="3" t="s">
-        <v>886</v>
+      <c r="H293" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I293" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="K293" t="s">
+        <v>883</v>
       </c>
       <c r="L293" s="3" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>812</v>
       </c>
       <c r="B294" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="C294" t="s">
         <v>14</v>
@@ -12369,18 +12370,18 @@
         <v>1</v>
       </c>
       <c r="K294" s="3" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="L294" s="3" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>812</v>
       </c>
       <c r="B295" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="C295" t="s">
         <v>14</v>
@@ -12389,28 +12390,28 @@
         <v>30</v>
       </c>
       <c r="E295" s="1">
-        <v>195</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F295" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G295" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K295" t="s">
-        <v>892</v>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K295" s="3" t="s">
+        <v>889</v>
       </c>
       <c r="L295" s="3" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>812</v>
       </c>
       <c r="B296" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="C296" t="s">
         <v>14</v>
@@ -12419,7 +12420,7 @@
         <v>30</v>
       </c>
       <c r="E296" s="1">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="F296" s="2" t="s">
         <v>43</v>
@@ -12429,18 +12430,18 @@
         <v>0</v>
       </c>
       <c r="K296" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="L296" s="3" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>812</v>
       </c>
       <c r="B297" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="C297" t="s">
         <v>14</v>
@@ -12449,28 +12450,28 @@
         <v>30</v>
       </c>
       <c r="E297" s="1">
-        <v>0.5</v>
+        <v>16</v>
       </c>
       <c r="F297" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G297" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K297" s="3" t="s">
-        <v>898</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K297" t="s">
+        <v>895</v>
       </c>
       <c r="L297" s="3" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>812</v>
       </c>
       <c r="B298" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C298" t="s">
         <v>14</v>
@@ -12479,7 +12480,7 @@
         <v>30</v>
       </c>
       <c r="E298" s="1">
-        <v>1.33</v>
+        <v>0.5</v>
       </c>
       <c r="F298" s="2" t="s">
         <v>17</v>
@@ -12488,19 +12489,19 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K298" t="s">
-        <v>900</v>
+      <c r="K298" s="3" t="s">
+        <v>898</v>
       </c>
       <c r="L298" s="3" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>812</v>
       </c>
       <c r="B299" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="C299" t="s">
         <v>14</v>
@@ -12509,28 +12510,28 @@
         <v>30</v>
       </c>
       <c r="E299" s="1">
-        <v>180</v>
+        <v>1.33</v>
       </c>
       <c r="F299" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="G299" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K299" s="3" t="s">
-        <v>903</v>
+      <c r="K299" t="s">
+        <v>900</v>
       </c>
       <c r="L299" s="3" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>812</v>
       </c>
       <c r="B300" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C300" t="s">
         <v>14</v>
@@ -12539,7 +12540,7 @@
         <v>30</v>
       </c>
       <c r="E300" s="1">
-        <v>85</v>
+        <v>180</v>
       </c>
       <c r="F300" s="2" t="s">
         <v>51</v>
@@ -12549,54 +12550,48 @@
         <v>1</v>
       </c>
       <c r="K300" s="3" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="L300" s="3" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>812</v>
       </c>
       <c r="B301" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="C301" t="s">
         <v>14</v>
       </c>
       <c r="D301" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E301" s="1">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F301" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G301" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H301" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I301" s="3" t="s">
-        <v>909</v>
-      </c>
       <c r="K301" s="3" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="L301" s="3" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>812</v>
       </c>
       <c r="B302" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="C302" t="s">
         <v>14</v>
@@ -12617,19 +12612,22 @@
       <c r="H302" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="I302" s="3" t="s">
+        <v>909</v>
+      </c>
       <c r="K302" s="3" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="L302" s="3" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>812</v>
       </c>
       <c r="B303" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="C303" t="s">
         <v>14</v>
@@ -12640,6 +12638,9 @@
       <c r="E303" s="1">
         <v>0</v>
       </c>
+      <c r="F303" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G303" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
@@ -12647,52 +12648,52 @@
       <c r="H303" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I303" s="3" t="s">
-        <v>916</v>
-      </c>
       <c r="K303" s="3" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="L303" s="3" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>812</v>
       </c>
       <c r="B304" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="C304" t="s">
         <v>14</v>
       </c>
       <c r="D304" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E304" s="1">
-        <v>195</v>
-      </c>
-      <c r="F304" s="2" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="G304" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K304" t="s">
-        <v>920</v>
+      <c r="H304" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I304" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="K304" s="3" t="s">
+        <v>917</v>
       </c>
       <c r="L304" s="3" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>812</v>
       </c>
       <c r="B305" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="C305" t="s">
         <v>14</v>
@@ -12701,91 +12702,91 @@
         <v>30</v>
       </c>
       <c r="E305" s="1">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="F305" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G305" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K305" s="3" t="s">
-        <v>923</v>
+      <c r="K305" t="s">
+        <v>920</v>
       </c>
       <c r="L305" s="3" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>812</v>
       </c>
       <c r="B306" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="C306" t="s">
         <v>14</v>
       </c>
       <c r="D306" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E306" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F306" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G306" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H306" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I306" s="3" t="s">
-        <v>926</v>
-      </c>
       <c r="K306" s="3" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="L306" s="3" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>812</v>
       </c>
       <c r="B307" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="C307" t="s">
         <v>14</v>
       </c>
       <c r="D307" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E307" s="1">
-        <v>1</v>
-      </c>
-      <c r="F307" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G307" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H307" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I307" s="3" t="s">
+        <v>926</v>
+      </c>
       <c r="K307" s="3" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="L307" s="3" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>812</v>
       </c>
       <c r="B308" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="C308" t="s">
         <v>14</v>
@@ -12794,7 +12795,7 @@
         <v>30</v>
       </c>
       <c r="E308" s="1">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="F308" s="2" t="s">
         <v>17</v>
@@ -12804,18 +12805,18 @@
         <v>1</v>
       </c>
       <c r="K308" s="3" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="L308" s="3" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>812</v>
       </c>
       <c r="B309" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C309" t="s">
         <v>14</v>
@@ -12824,58 +12825,58 @@
         <v>30</v>
       </c>
       <c r="E309" s="1">
-        <v>100</v>
+        <v>1E-3</v>
       </c>
       <c r="F309" s="2" t="s">
-        <v>936</v>
+        <v>17</v>
       </c>
       <c r="G309" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K309" s="3" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="L309" s="3" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>812</v>
       </c>
       <c r="B310" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="C310" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="D310" t="s">
         <v>30</v>
       </c>
       <c r="E310" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F310" s="2" t="s">
-        <v>128</v>
+        <v>936</v>
       </c>
       <c r="G310" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K310" s="3" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="L310" s="3" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="311" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>812</v>
       </c>
       <c r="B311" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="C311" t="s">
         <v>90</v>
@@ -12894,75 +12895,75 @@
         <v>0</v>
       </c>
       <c r="K311" s="3" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="L311" s="3" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>812</v>
       </c>
       <c r="B312" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="C312" t="s">
         <v>90</v>
       </c>
       <c r="D312" t="s">
-        <v>87</v>
+        <v>30</v>
+      </c>
+      <c r="E312" s="1">
+        <v>0</v>
       </c>
       <c r="F312" s="2" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="G312" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="K312" s="3" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="L312" s="3" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>812</v>
       </c>
       <c r="B313" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C313" t="s">
         <v>90</v>
       </c>
       <c r="D313" t="s">
-        <v>30</v>
-      </c>
-      <c r="E313" s="1">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="F313" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="G313" s="2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="K313" s="3" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="L313" s="3" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>812</v>
       </c>
       <c r="B314" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C314" t="s">
         <v>90</v>
@@ -12981,9 +12982,39 @@
         <v>0</v>
       </c>
       <c r="K314" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="L314" s="3" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>812</v>
+      </c>
+      <c r="B315" t="s">
+        <v>949</v>
+      </c>
+      <c r="C315" t="s">
+        <v>90</v>
+      </c>
+      <c r="D315" t="s">
+        <v>30</v>
+      </c>
+      <c r="E315" s="1">
+        <v>0</v>
+      </c>
+      <c r="F315" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G315" s="2" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K315" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="L314" s="3" t="s">
+      <c r="L315" s="3" t="s">
         <v>950</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating variable names, fixing disabled n_panel controls
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\solarpilot\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ACEA10-C1ED-47A0-A9F4-1B7CEB317B88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E346A-A132-4A07-81CE-D9AD07318D65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2880,42 +2880,27 @@
     <t>rec_cav_tlip</t>
   </si>
   <si>
-    <t>Receiver cavity top lip fractional height</t>
-  </si>
-  <si>
     <t>Fraction of the total receiver height occupied by the top lip in a cavity geometry</t>
   </si>
   <si>
     <t>rec_cav_blip</t>
   </si>
   <si>
-    <t>Receiver cavity bottom lip fractional height</t>
-  </si>
-  <si>
     <t>Fraction of the total receiver height occupied by the bottom lip in a cavity geometry</t>
   </si>
   <si>
-    <t>Receiver cavity active surface radius</t>
-  </si>
-  <si>
     <t>Radius of the circle circumscribing all active absorber surfaces</t>
   </si>
   <si>
     <t>rec_cav_apwfrac</t>
   </si>
   <si>
-    <t>Receiver cavity aperture width fraction</t>
-  </si>
-  <si>
     <t>Width of cavity aperture relative to maximum width at the aperture plane</t>
   </si>
   <si>
     <t>rec_cav_apw</t>
   </si>
   <si>
-    <t>Receiver cavity aperture width</t>
-  </si>
-  <si>
     <t>Calculated aperture width based on cavity geometry and aperture width fraction</t>
   </si>
   <si>
@@ -2934,9 +2919,6 @@
     <t>rec_cav_aph</t>
   </si>
   <si>
-    <t>Receiver cavity aperture height</t>
-  </si>
-  <si>
     <t>Calculated aperture height based on receiver height and lip height fractions</t>
   </si>
   <si>
@@ -2944,6 +2926,24 @@
   </si>
   <si>
     <t>Offset of circle circumscribing cavity absorber surfaces from the aperture plane; fraction of cavity radius; positive yields greater receiver depth</t>
+  </si>
+  <si>
+    <t>Cavity active surface radius</t>
+  </si>
+  <si>
+    <t>Cavity top lip fractional height</t>
+  </si>
+  <si>
+    <t>Cavity bottom lip fractional height</t>
+  </si>
+  <si>
+    <t>Cavity aperture width fraction</t>
+  </si>
+  <si>
+    <t>Cavity aperture width</t>
+  </si>
+  <si>
+    <t>Cavity aperture height</t>
   </si>
 </sst>
 </file>
@@ -3360,8 +3360,8 @@
   <dimension ref="A1:L318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A241" sqref="A241"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K268" sqref="K268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10754,10 +10754,10 @@
         <v>1</v>
       </c>
       <c r="K241" s="3" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="L241" s="3" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.3">
@@ -10784,10 +10784,10 @@
         <v>1</v>
       </c>
       <c r="K242" s="3" t="s">
-        <v>956</v>
+        <v>967</v>
       </c>
       <c r="L242" s="3" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.3">
@@ -10813,10 +10813,10 @@
         <v>1</v>
       </c>
       <c r="K243" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="L243" s="3" t="s">
         <v>951</v>
-      </c>
-      <c r="L243" s="3" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.3">
@@ -10824,7 +10824,7 @@
         <v>666</v>
       </c>
       <c r="B244" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C244" t="s">
         <v>14</v>
@@ -10842,10 +10842,10 @@
         <v>1</v>
       </c>
       <c r="K244" s="3" t="s">
-        <v>954</v>
+        <v>969</v>
       </c>
       <c r="L244" s="3" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.3">
@@ -10853,7 +10853,7 @@
         <v>666</v>
       </c>
       <c r="B245" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="C245" t="s">
         <v>14</v>
@@ -10871,10 +10871,10 @@
         <v>1</v>
       </c>
       <c r="K245" s="3" t="s">
-        <v>959</v>
+        <v>970</v>
       </c>
       <c r="L245" s="3" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.3">
@@ -11183,7 +11183,7 @@
         <v>757</v>
       </c>
       <c r="L255" s="3" t="s">
-        <v>964</v>
+        <v>959</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.3">
@@ -11367,7 +11367,7 @@
         <v>666</v>
       </c>
       <c r="B262" t="s">
-        <v>965</v>
+        <v>960</v>
       </c>
       <c r="C262" t="s">
         <v>90</v>
@@ -11386,10 +11386,10 @@
         <v>0</v>
       </c>
       <c r="K262" s="3" t="s">
-        <v>966</v>
+        <v>961</v>
       </c>
       <c r="L262" s="3" t="s">
-        <v>967</v>
+        <v>962</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.3">
@@ -11487,7 +11487,7 @@
         <v>666</v>
       </c>
       <c r="B266" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="C266" t="s">
         <v>90</v>
@@ -11505,10 +11505,10 @@
         <v>0</v>
       </c>
       <c r="K266" s="3" t="s">
-        <v>962</v>
+        <v>971</v>
       </c>
       <c r="L266" s="3" t="s">
-        <v>963</v>
+        <v>958</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.3">
@@ -11516,7 +11516,7 @@
         <v>666</v>
       </c>
       <c r="B267" t="s">
-        <v>968</v>
+        <v>963</v>
       </c>
       <c r="C267" t="s">
         <v>90</v>
@@ -11534,10 +11534,10 @@
         <v>0</v>
       </c>
       <c r="K267" s="3" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="L267" s="3" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updating variable definitions for cavity model
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\solarpilot\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E346A-A132-4A07-81CE-D9AD07318D65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D714DA-A5AB-4EB9-9122-57C0FEC56627}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3360,8 +3360,8 @@
   <dimension ref="A1:L318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K268" sqref="K268"/>
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E248" sqref="E248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10744,7 +10744,7 @@
         <v>30</v>
       </c>
       <c r="E241" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F241" s="2" t="s">
         <v>17</v>
@@ -10774,7 +10774,7 @@
         <v>30</v>
       </c>
       <c r="E242" s="1">
-        <v>7.75</v>
+        <v>7.5</v>
       </c>
       <c r="F242" s="2" t="s">
         <v>43</v>
@@ -11134,7 +11134,7 @@
         <v>21</v>
       </c>
       <c r="E254" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F254" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
update defaults and cavity ui display
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\solarpilot\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98CE24B-A9E7-49FD-A3E8-00E2237D3933}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F36744-22DE-430E-ADA6-33FD9FFF40DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="975">
   <si>
     <t>Domain</t>
   </si>
@@ -2925,9 +2925,6 @@
     <t>Cavity absorber centroid aperture offset</t>
   </si>
   <si>
-    <t>Offset of circle circumscribing cavity absorber surfaces from the aperture plane; fraction of cavity radius; positive yields greater receiver depth</t>
-  </si>
-  <si>
     <t>Cavity active surface radius</t>
   </si>
   <si>
@@ -2950,6 +2947,9 @@
   </si>
   <si>
     <t>SolarPILOT code base version number</t>
+  </si>
+  <si>
+    <t>Offset of centroid of cavity absorber surfaces from the aperture plane (fraction of cavity radius); positive yields greater receiver depth</t>
   </si>
 </sst>
 </file>
@@ -3366,8 +3366,8 @@
   <dimension ref="A1:L319"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E255" sqref="E255"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5992,8 +5992,7 @@
         <v>17</v>
       </c>
       <c r="G86" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K86" s="3" t="s">
         <v>287</v>
@@ -6022,8 +6021,7 @@
         <v>17</v>
       </c>
       <c r="G87" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K87" s="3" t="s">
         <v>290</v>
@@ -6320,8 +6318,8 @@
         <v>17</v>
       </c>
       <c r="G97" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K97" s="3" t="s">
         <v>323</v>
@@ -6350,8 +6348,8 @@
         <v>17</v>
       </c>
       <c r="G98" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K98" s="3" t="s">
         <v>326</v>
@@ -10750,7 +10748,7 @@
         <v>30</v>
       </c>
       <c r="E241" s="1">
-        <v>0.1</v>
+        <v>-0.25</v>
       </c>
       <c r="F241" s="2" t="s">
         <v>17</v>
@@ -10763,7 +10761,7 @@
         <v>965</v>
       </c>
       <c r="L241" s="3" t="s">
-        <v>966</v>
+        <v>974</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
@@ -10780,7 +10778,7 @@
         <v>30</v>
       </c>
       <c r="E242" s="1">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="F242" s="2" t="s">
         <v>43</v>
@@ -10790,7 +10788,7 @@
         <v>1</v>
       </c>
       <c r="K242" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="L242" s="3" t="s">
         <v>954</v>
@@ -10810,7 +10808,7 @@
         <v>30</v>
       </c>
       <c r="E243" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F243" s="2" t="s">
         <v>17</v>
@@ -10818,8 +10816,11 @@
       <c r="G243" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="J243" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="K243" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="L243" s="3" t="s">
         <v>951</v>
@@ -10839,7 +10840,7 @@
         <v>30</v>
       </c>
       <c r="E244" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F244" s="2" t="s">
         <v>17</v>
@@ -10847,8 +10848,11 @@
       <c r="G244" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="J244" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="K244" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="L244" s="3" t="s">
         <v>953</v>
@@ -10876,8 +10880,11 @@
       <c r="G245" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="J245" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="K245" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="L245" s="3" t="s">
         <v>956</v>
@@ -11511,7 +11518,7 @@
         <v>0</v>
       </c>
       <c r="K266" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="L266" s="3" t="s">
         <v>958</v>
@@ -11540,7 +11547,7 @@
         <v>0</v>
       </c>
       <c r="K267" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="L267" s="3" t="s">
         <v>964</v>
@@ -11731,7 +11738,7 @@
         <v>800</v>
       </c>
       <c r="B274" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C274" t="s">
         <v>14</v>
@@ -11746,10 +11753,10 @@
         <v>0</v>
       </c>
       <c r="K274" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="L274" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update curtain width to max curtain width
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WHamilt2\Documents\solarPILOT_build\SolarPILOT\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE0BCCC-2A73-4785-85AC-E5EC68BC55AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959FADA6-DD41-4681-8D8E-29335F4840F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2978,12 +2978,6 @@
     <t>curtain_radius</t>
   </si>
   <si>
-    <t>curtain_width</t>
-  </si>
-  <si>
-    <t>Particle curtain width</t>
-  </si>
-  <si>
     <t>Particle curtain radius</t>
   </si>
   <si>
@@ -3066,6 +3060,12 @@
   </si>
   <si>
     <t>Normalized particle curtain height</t>
+  </si>
+  <si>
+    <t>max_curtain_width</t>
+  </si>
+  <si>
+    <t>Particle curtain maximum width</t>
   </si>
 </sst>
 </file>
@@ -3092,24 +3092,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3124,7 +3112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3156,15 +3144,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3510,9 +3497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L331"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K256" sqref="K256"/>
+      <selection pane="bottomLeft" activeCell="L285" sqref="L285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11122,7 +11109,7 @@
         <v>735</v>
       </c>
       <c r="L248" s="3" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.35">
@@ -11305,7 +11292,7 @@
         <v>22</v>
       </c>
       <c r="I254" s="3" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="K254" t="s">
         <v>753</v>
@@ -11314,129 +11301,132 @@
         <v>754</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
+    <row r="255" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A255" s="11" t="s">
         <v>666</v>
       </c>
       <c r="B255" s="11" t="s">
         <v>755</v>
       </c>
-      <c r="C255" t="s">
-        <v>14</v>
-      </c>
-      <c r="D255" t="s">
-        <v>30</v>
-      </c>
-      <c r="E255" s="1">
-        <v>17</v>
-      </c>
-      <c r="F255" s="2" t="s">
+      <c r="C255" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D255" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E255" s="12">
+        <v>17</v>
+      </c>
+      <c r="F255" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G255" s="2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K255" t="s">
+      <c r="G255" s="13" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H255" s="14"/>
+      <c r="I255" s="14"/>
+      <c r="J255" s="14"/>
+      <c r="K255" s="11" t="s">
         <v>756</v>
       </c>
-      <c r="L255" s="3" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="256" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A256" s="12" t="s">
+      <c r="L255" s="14" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A256" s="11" t="s">
         <v>666</v>
       </c>
-      <c r="B256" s="12" t="s">
+      <c r="B256" s="11" t="s">
+        <v>998</v>
+      </c>
+      <c r="C256" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D256" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E256" s="12">
+        <v>1</v>
+      </c>
+      <c r="F256" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G256" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H256" s="14"/>
+      <c r="I256" s="14"/>
+      <c r="J256" s="14"/>
+      <c r="K256" s="14" t="s">
+        <v>1007</v>
+      </c>
+      <c r="L256" s="11" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A257" s="11" t="s">
+        <v>666</v>
+      </c>
+      <c r="B257" s="11" t="s">
+        <v>999</v>
+      </c>
+      <c r="C257" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D257" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E257" s="12">
+        <v>1</v>
+      </c>
+      <c r="F257" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G257" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H257" s="14"/>
+      <c r="I257" s="14"/>
+      <c r="J257" s="14"/>
+      <c r="K257" s="14" t="s">
         <v>1000</v>
       </c>
-      <c r="C256" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D256" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E256" s="13">
-        <v>1</v>
-      </c>
-      <c r="F256" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G256" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H256" s="15"/>
-      <c r="I256" s="15"/>
-      <c r="J256" s="15"/>
-      <c r="K256" s="15" t="s">
-        <v>1009</v>
-      </c>
-      <c r="L256" s="12" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="257" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A257" s="12" t="s">
+      <c r="L257" s="11" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A258" s="11" t="s">
         <v>666</v>
       </c>
-      <c r="B257" s="12" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C257" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D257" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E257" s="13">
-        <v>1</v>
-      </c>
-      <c r="F257" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G257" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H257" s="15"/>
-      <c r="I257" s="15"/>
-      <c r="J257" s="15"/>
-      <c r="K257" s="15" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L257" s="12" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="258" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A258" s="12" t="s">
-        <v>666</v>
-      </c>
-      <c r="B258" s="12" t="s">
+      <c r="B258" s="11" t="s">
         <v>972</v>
       </c>
-      <c r="C258" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D258" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E258" s="13">
+      <c r="C258" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D258" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E258" s="12">
         <v>1.5</v>
       </c>
-      <c r="F258" s="14" t="s">
+      <c r="F258" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G258" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H258" s="15"/>
-      <c r="I258" s="15"/>
-      <c r="J258" s="15"/>
-      <c r="K258" s="15" t="s">
+      <c r="G258" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H258" s="14"/>
+      <c r="I258" s="14"/>
+      <c r="J258" s="14"/>
+      <c r="K258" s="14" t="s">
         <v>973</v>
       </c>
-      <c r="L258" s="12" t="s">
+      <c r="L258" s="11" t="s">
         <v>974</v>
       </c>
     </row>
@@ -11454,7 +11444,7 @@
         <v>15</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="F259" s="2" t="s">
         <v>17</v>
@@ -11463,10 +11453,10 @@
         <v>1</v>
       </c>
       <c r="K259" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="L259" s="3" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.35">
@@ -11495,7 +11485,7 @@
         <v>22</v>
       </c>
       <c r="I260" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="K260" s="3" t="s">
         <v>977</v>
@@ -11527,10 +11517,10 @@
         <v>1</v>
       </c>
       <c r="K261" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="L261" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.35">
@@ -11538,7 +11528,7 @@
         <v>666</v>
       </c>
       <c r="B262" s="11" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C262" t="s">
         <v>14</v>
@@ -11558,10 +11548,10 @@
         <v>112</v>
       </c>
       <c r="K262" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="L262" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.35">
@@ -11569,7 +11559,7 @@
         <v>666</v>
       </c>
       <c r="B263" s="11" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C263" t="s">
         <v>14</v>
@@ -11587,10 +11577,10 @@
         <v>1</v>
       </c>
       <c r="K263" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="L263" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.35">
@@ -11598,7 +11588,7 @@
         <v>666</v>
       </c>
       <c r="B264" s="11" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C264" t="s">
         <v>14</v>
@@ -11616,10 +11606,10 @@
         <v>1</v>
       </c>
       <c r="K264" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="L264" s="3" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.35">
@@ -11627,7 +11617,7 @@
         <v>666</v>
       </c>
       <c r="B265" s="11" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C265" t="s">
         <v>14</v>
@@ -11645,10 +11635,10 @@
         <v>1</v>
       </c>
       <c r="K265" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="L265" s="3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.35">
@@ -12190,7 +12180,7 @@
         <v>666</v>
       </c>
       <c r="B284" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="C284" t="s">
         <v>90</v>
@@ -12208,10 +12198,10 @@
         <v>0</v>
       </c>
       <c r="K284" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="L284" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.35">
@@ -12219,7 +12209,7 @@
         <v>666</v>
       </c>
       <c r="B285" t="s">
-        <v>980</v>
+        <v>1008</v>
       </c>
       <c r="C285" t="s">
         <v>90</v>
@@ -12237,10 +12227,10 @@
         <v>0</v>
       </c>
       <c r="K285" t="s">
-        <v>981</v>
+        <v>1009</v>
       </c>
       <c r="L285" t="s">
-        <v>981</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added aperture view option to plot flux page
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WHamilt2\Documents\solarPILOT_build\SolarPILOT\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959FADA6-DD41-4681-8D8E-29335F4840F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB70C4B6-97F2-49D8-B17F-622B9FA5F3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2960,9 +2960,6 @@
     <t>Particle curtain entrance depth</t>
   </si>
   <si>
-    <t>Particle curtain entrance depth from the aperature</t>
-  </si>
-  <si>
     <t>norm_heights_depths</t>
   </si>
   <si>
@@ -3014,9 +3011,6 @@
     <t>Horizontal SNOUT angle</t>
   </si>
   <si>
-    <t>SNOUT spanning angle defined in the aperature vertical midplane</t>
-  </si>
-  <si>
     <t>External cylindrical=0;Cavity=1;Flat plate=2;Falling particle=3</t>
   </si>
   <si>
@@ -3066,6 +3060,12 @@
   </si>
   <si>
     <t>Particle curtain maximum width</t>
+  </si>
+  <si>
+    <t>SNOUT spanning angle defined in the aperture vertical midplane</t>
+  </si>
+  <si>
+    <t>Particle curtain entrance depth from the aperture</t>
   </si>
 </sst>
 </file>
@@ -3112,7 +3112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3143,16 +3143,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3497,29 +3487,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L285" sqref="L285"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L256" sqref="L256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="39.54296875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="114.453125" customWidth="1"/>
-    <col min="13" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="39.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="114.42578125" customWidth="1"/>
+    <col min="13" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3557,7 +3547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3590,7 +3580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3626,7 +3616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3656,7 +3646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3686,7 +3676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3716,7 +3706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3746,7 +3736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3776,7 +3766,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3812,7 +3802,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3842,7 +3832,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3872,7 +3862,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3902,7 +3892,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3932,7 +3922,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3962,7 +3952,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3989,7 +3979,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -4019,7 +4009,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -4055,7 +4045,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -4085,7 +4075,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4112,7 +4102,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4142,7 +4132,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4169,7 +4159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4198,7 +4188,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -4228,7 +4218,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4258,7 +4248,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -4288,7 +4278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -4318,7 +4308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -4348,7 +4338,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -4378,7 +4368,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -4409,7 +4399,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -4439,7 +4429,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -4469,7 +4459,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -4499,7 +4489,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -4529,7 +4519,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -4559,7 +4549,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -4589,7 +4579,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -4619,7 +4609,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -4649,7 +4639,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -4679,7 +4669,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -4709,7 +4699,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -4736,7 +4726,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -4763,7 +4753,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -4793,7 +4783,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -4823,7 +4813,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -4853,7 +4843,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>97</v>
       </c>
@@ -4883,7 +4873,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -4913,7 +4903,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -4943,7 +4933,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -4973,7 +4963,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -5003,7 +4993,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -5033,7 +5023,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -5063,7 +5053,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -5093,7 +5083,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -5123,7 +5113,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>97</v>
       </c>
@@ -5153,7 +5143,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>97</v>
       </c>
@@ -5183,7 +5173,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>190</v>
       </c>
@@ -5216,7 +5206,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>190</v>
       </c>
@@ -5246,7 +5236,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -5276,7 +5266,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>190</v>
       </c>
@@ -5306,7 +5296,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>190</v>
       </c>
@@ -5336,7 +5326,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>190</v>
       </c>
@@ -5366,7 +5356,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>190</v>
       </c>
@@ -5393,7 +5383,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>190</v>
       </c>
@@ -5420,7 +5410,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -5453,7 +5443,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>190</v>
       </c>
@@ -5483,7 +5473,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -5513,7 +5503,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>190</v>
       </c>
@@ -5537,7 +5527,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>190</v>
       </c>
@@ -5564,7 +5554,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>190</v>
       </c>
@@ -5597,7 +5587,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -5627,7 +5617,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>190</v>
       </c>
@@ -5657,7 +5647,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -5693,7 +5683,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>190</v>
       </c>
@@ -5720,7 +5710,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>190</v>
       </c>
@@ -5747,7 +5737,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>190</v>
       </c>
@@ -5774,7 +5764,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>190</v>
       </c>
@@ -5810,7 +5800,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>190</v>
       </c>
@@ -5844,7 +5834,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>190</v>
       </c>
@@ -5875,7 +5865,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>190</v>
       </c>
@@ -5906,7 +5896,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -5937,7 +5927,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>190</v>
       </c>
@@ -5968,7 +5958,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>190</v>
       </c>
@@ -6005,7 +5995,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -6036,7 +6026,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -6073,7 +6063,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>190</v>
       </c>
@@ -6104,7 +6094,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>190</v>
       </c>
@@ -6133,7 +6123,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>190</v>
       </c>
@@ -6162,7 +6152,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>190</v>
       </c>
@@ -6189,7 +6179,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>190</v>
       </c>
@@ -6219,7 +6209,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>190</v>
       </c>
@@ -6249,7 +6239,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>190</v>
       </c>
@@ -6285,7 +6275,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>190</v>
       </c>
@@ -6316,7 +6306,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -6343,7 +6333,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>190</v>
       </c>
@@ -6373,7 +6363,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>190</v>
       </c>
@@ -6400,7 +6390,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -6430,7 +6420,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -6460,7 +6450,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>190</v>
       </c>
@@ -6490,7 +6480,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>190</v>
       </c>
@@ -6519,7 +6509,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>190</v>
       </c>
@@ -6549,7 +6539,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>190</v>
       </c>
@@ -6579,7 +6569,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>332</v>
       </c>
@@ -6609,7 +6599,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>332</v>
       </c>
@@ -6639,7 +6629,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>332</v>
       </c>
@@ -6675,7 +6665,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>332</v>
       </c>
@@ -6705,7 +6695,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>332</v>
       </c>
@@ -6735,7 +6725,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>332</v>
       </c>
@@ -6765,7 +6755,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>332</v>
       </c>
@@ -6795,7 +6785,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>332</v>
       </c>
@@ -6825,7 +6815,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>332</v>
       </c>
@@ -6855,7 +6845,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>332</v>
       </c>
@@ -6885,7 +6875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>332</v>
       </c>
@@ -6915,7 +6905,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>332</v>
       </c>
@@ -6945,7 +6935,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>332</v>
       </c>
@@ -6975,7 +6965,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>332</v>
       </c>
@@ -7005,7 +6995,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>332</v>
       </c>
@@ -7035,7 +7025,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>332</v>
       </c>
@@ -7065,7 +7055,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>332</v>
       </c>
@@ -7095,7 +7085,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>332</v>
       </c>
@@ -7131,7 +7121,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>332</v>
       </c>
@@ -7167,7 +7157,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>332</v>
       </c>
@@ -7197,7 +7187,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>332</v>
       </c>
@@ -7224,7 +7214,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>332</v>
       </c>
@@ -7254,7 +7244,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>332</v>
       </c>
@@ -7285,7 +7275,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>332</v>
       </c>
@@ -7319,7 +7309,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>332</v>
       </c>
@@ -7347,7 +7337,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>332</v>
       </c>
@@ -7381,7 +7371,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>332</v>
       </c>
@@ -7415,7 +7405,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>332</v>
       </c>
@@ -7451,7 +7441,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>332</v>
       </c>
@@ -7485,7 +7475,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>332</v>
       </c>
@@ -7519,7 +7509,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>332</v>
       </c>
@@ -7546,7 +7536,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>332</v>
       </c>
@@ -7573,7 +7563,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>332</v>
       </c>
@@ -7603,7 +7593,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>332</v>
       </c>
@@ -7633,7 +7623,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>332</v>
       </c>
@@ -7663,7 +7653,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>332</v>
       </c>
@@ -7693,7 +7683,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>332</v>
       </c>
@@ -7723,7 +7713,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>332</v>
       </c>
@@ -7753,7 +7743,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>332</v>
       </c>
@@ -7783,7 +7773,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>332</v>
       </c>
@@ -7813,7 +7803,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>332</v>
       </c>
@@ -7843,7 +7833,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>332</v>
       </c>
@@ -7873,7 +7863,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>332</v>
       </c>
@@ -7912,7 +7902,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>332</v>
       </c>
@@ -7945,7 +7935,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>332</v>
       </c>
@@ -7972,7 +7962,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>332</v>
       </c>
@@ -8002,7 +7992,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>332</v>
       </c>
@@ -8032,7 +8022,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>332</v>
       </c>
@@ -8062,7 +8052,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>332</v>
       </c>
@@ -8092,7 +8082,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>332</v>
       </c>
@@ -8122,7 +8112,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>332</v>
       </c>
@@ -8152,7 +8142,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>332</v>
       </c>
@@ -8182,7 +8172,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>332</v>
       </c>
@@ -8212,7 +8202,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>332</v>
       </c>
@@ -8242,7 +8232,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>332</v>
       </c>
@@ -8272,7 +8262,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>332</v>
       </c>
@@ -8302,7 +8292,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>332</v>
       </c>
@@ -8332,7 +8322,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>332</v>
       </c>
@@ -8362,7 +8352,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>332</v>
       </c>
@@ -8392,7 +8382,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>332</v>
       </c>
@@ -8422,7 +8412,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>332</v>
       </c>
@@ -8452,7 +8442,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>332</v>
       </c>
@@ -8482,7 +8472,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>332</v>
       </c>
@@ -8512,7 +8502,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>513</v>
       </c>
@@ -8542,7 +8532,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>513</v>
       </c>
@@ -8566,7 +8556,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>513</v>
       </c>
@@ -8596,7 +8586,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>513</v>
       </c>
@@ -8626,7 +8616,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>513</v>
       </c>
@@ -8657,7 +8647,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>513</v>
       </c>
@@ -8681,7 +8671,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>513</v>
       </c>
@@ -8715,7 +8705,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>513</v>
       </c>
@@ -8749,7 +8739,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>513</v>
       </c>
@@ -8783,7 +8773,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>513</v>
       </c>
@@ -8817,7 +8807,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>513</v>
       </c>
@@ -8847,7 +8837,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>513</v>
       </c>
@@ -8877,7 +8867,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>513</v>
       </c>
@@ -8907,7 +8897,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>513</v>
       </c>
@@ -8937,7 +8927,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>513</v>
       </c>
@@ -8967,7 +8957,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>513</v>
       </c>
@@ -8997,7 +8987,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>513</v>
       </c>
@@ -9027,7 +9017,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>513</v>
       </c>
@@ -9057,7 +9047,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>513</v>
       </c>
@@ -9087,7 +9077,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>513</v>
       </c>
@@ -9117,7 +9107,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>513</v>
       </c>
@@ -9147,7 +9137,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>513</v>
       </c>
@@ -9177,7 +9167,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>576</v>
       </c>
@@ -9213,7 +9203,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>576</v>
       </c>
@@ -9235,7 +9225,7 @@
       </c>
       <c r="L188" s="3"/>
     </row>
-    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>576</v>
       </c>
@@ -9265,7 +9255,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>576</v>
       </c>
@@ -9298,7 +9288,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>576</v>
       </c>
@@ -9331,7 +9321,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>576</v>
       </c>
@@ -9364,7 +9354,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>576</v>
       </c>
@@ -9394,7 +9384,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>576</v>
       </c>
@@ -9424,7 +9414,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>576</v>
       </c>
@@ -9454,7 +9444,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>576</v>
       </c>
@@ -9484,7 +9474,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>576</v>
       </c>
@@ -9514,7 +9504,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>576</v>
       </c>
@@ -9541,7 +9531,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>576</v>
       </c>
@@ -9571,7 +9561,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>576</v>
       </c>
@@ -9604,7 +9594,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>576</v>
       </c>
@@ -9636,7 +9626,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>619</v>
       </c>
@@ -9666,7 +9656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>619</v>
       </c>
@@ -9693,7 +9683,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>619</v>
       </c>
@@ -9720,7 +9710,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>619</v>
       </c>
@@ -9753,7 +9743,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>619</v>
       </c>
@@ -9784,7 +9774,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>619</v>
       </c>
@@ -9818,7 +9808,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>619</v>
       </c>
@@ -9852,7 +9842,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>619</v>
       </c>
@@ -9886,7 +9876,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>619</v>
       </c>
@@ -9920,7 +9910,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>619</v>
       </c>
@@ -9954,7 +9944,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>619</v>
       </c>
@@ -9988,7 +9978,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>619</v>
       </c>
@@ -10022,7 +10012,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>619</v>
       </c>
@@ -10056,7 +10046,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>619</v>
       </c>
@@ -10090,7 +10080,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>619</v>
       </c>
@@ -10124,7 +10114,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>619</v>
       </c>
@@ -10148,7 +10138,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>619</v>
       </c>
@@ -10175,7 +10165,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>619</v>
       </c>
@@ -10211,7 +10201,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>666</v>
       </c>
@@ -10241,7 +10231,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>666</v>
       </c>
@@ -10277,7 +10267,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>666</v>
       </c>
@@ -10307,7 +10297,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>666</v>
       </c>
@@ -10337,7 +10327,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>666</v>
       </c>
@@ -10373,7 +10363,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>666</v>
       </c>
@@ -10403,7 +10393,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>666</v>
       </c>
@@ -10433,7 +10423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>666</v>
       </c>
@@ -10460,7 +10450,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>666</v>
       </c>
@@ -10491,7 +10481,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>666</v>
       </c>
@@ -10519,7 +10509,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>666</v>
       </c>
@@ -10553,7 +10543,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>666</v>
       </c>
@@ -10587,7 +10577,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>666</v>
       </c>
@@ -10617,7 +10607,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>666</v>
       </c>
@@ -10650,7 +10640,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>666</v>
       </c>
@@ -10680,7 +10670,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>666</v>
       </c>
@@ -10716,7 +10706,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>666</v>
       </c>
@@ -10746,7 +10736,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>666</v>
       </c>
@@ -10776,7 +10766,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>666</v>
       </c>
@@ -10806,7 +10796,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>666</v>
       </c>
@@ -10836,7 +10826,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>666</v>
       </c>
@@ -10866,7 +10856,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>666</v>
       </c>
@@ -10896,7 +10886,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>666</v>
       </c>
@@ -10926,7 +10916,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>666</v>
       </c>
@@ -10958,7 +10948,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>666</v>
       </c>
@@ -10990,7 +10980,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>666</v>
       </c>
@@ -11022,7 +11012,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>666</v>
       </c>
@@ -11052,7 +11042,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>666</v>
       </c>
@@ -11082,7 +11072,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>666</v>
       </c>
@@ -11109,10 +11099,10 @@
         <v>735</v>
       </c>
       <c r="L248" s="3" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>666</v>
       </c>
@@ -11139,7 +11129,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>666</v>
       </c>
@@ -11169,7 +11159,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>666</v>
       </c>
@@ -11199,7 +11189,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>666</v>
       </c>
@@ -11229,7 +11219,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>666</v>
       </c>
@@ -11265,7 +11255,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>666</v>
       </c>
@@ -11292,7 +11282,7 @@
         <v>22</v>
       </c>
       <c r="I254" s="3" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="K254" t="s">
         <v>753</v>
@@ -11301,141 +11291,129 @@
         <v>754</v>
       </c>
     </row>
-    <row r="255" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A255" s="11" t="s">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
         <v>666</v>
       </c>
-      <c r="B255" s="11" t="s">
+      <c r="B255" t="s">
         <v>755</v>
       </c>
-      <c r="C255" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D255" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E255" s="12">
-        <v>17</v>
-      </c>
-      <c r="F255" s="13" t="s">
+      <c r="C255" t="s">
+        <v>14</v>
+      </c>
+      <c r="D255" t="s">
+        <v>30</v>
+      </c>
+      <c r="E255" s="1">
+        <v>17</v>
+      </c>
+      <c r="F255" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G255" s="13" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H255" s="14"/>
-      <c r="I255" s="14"/>
-      <c r="J255" s="14"/>
-      <c r="K255" s="11" t="s">
+      <c r="G255" s="2" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K255" t="s">
         <v>756</v>
       </c>
-      <c r="L255" s="14" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="256" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A256" s="11" t="s">
+      <c r="L255" s="3" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>666</v>
       </c>
-      <c r="B256" s="11" t="s">
+      <c r="B256" t="s">
+        <v>996</v>
+      </c>
+      <c r="C256" t="s">
+        <v>14</v>
+      </c>
+      <c r="D256" t="s">
+        <v>30</v>
+      </c>
+      <c r="E256" s="1">
+        <v>1</v>
+      </c>
+      <c r="F256" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G256" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K256" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="L256" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>666</v>
+      </c>
+      <c r="B257" t="s">
+        <v>997</v>
+      </c>
+      <c r="C257" t="s">
+        <v>14</v>
+      </c>
+      <c r="D257" t="s">
+        <v>30</v>
+      </c>
+      <c r="E257" s="1">
+        <v>1</v>
+      </c>
+      <c r="F257" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G257" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K257" s="3" t="s">
         <v>998</v>
       </c>
-      <c r="C256" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D256" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E256" s="12">
-        <v>1</v>
-      </c>
-      <c r="F256" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G256" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H256" s="14"/>
-      <c r="I256" s="14"/>
-      <c r="J256" s="14"/>
-      <c r="K256" s="14" t="s">
-        <v>1007</v>
-      </c>
-      <c r="L256" s="11" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="257" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A257" s="11" t="s">
+      <c r="L257" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
         <v>666</v>
       </c>
-      <c r="B257" s="11" t="s">
-        <v>999</v>
-      </c>
-      <c r="C257" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D257" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E257" s="12">
-        <v>1</v>
-      </c>
-      <c r="F257" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G257" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H257" s="14"/>
-      <c r="I257" s="14"/>
-      <c r="J257" s="14"/>
-      <c r="K257" s="14" t="s">
-        <v>1000</v>
-      </c>
-      <c r="L257" s="11" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="258" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A258" s="11" t="s">
-        <v>666</v>
-      </c>
-      <c r="B258" s="11" t="s">
+      <c r="B258" t="s">
         <v>972</v>
       </c>
-      <c r="C258" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D258" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E258" s="12">
+      <c r="C258" t="s">
+        <v>14</v>
+      </c>
+      <c r="D258" t="s">
+        <v>30</v>
+      </c>
+      <c r="E258" s="1">
         <v>1.5</v>
       </c>
-      <c r="F258" s="13" t="s">
+      <c r="F258" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G258" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H258" s="14"/>
-      <c r="I258" s="14"/>
-      <c r="J258" s="14"/>
-      <c r="K258" s="14" t="s">
+      <c r="G258" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K258" s="3" t="s">
         <v>973</v>
       </c>
-      <c r="L258" s="11" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L258" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>666</v>
       </c>
-      <c r="B259" s="11" t="s">
-        <v>975</v>
+      <c r="B259" t="s">
+        <v>974</v>
       </c>
       <c r="C259" t="s">
         <v>14</v>
@@ -11444,7 +11422,7 @@
         <v>15</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="F259" s="2" t="s">
         <v>17</v>
@@ -11453,18 +11431,18 @@
         <v>1</v>
       </c>
       <c r="K259" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="L259" s="3" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>666</v>
       </c>
-      <c r="B260" s="11" t="s">
-        <v>976</v>
+      <c r="B260" t="s">
+        <v>975</v>
       </c>
       <c r="C260" t="s">
         <v>14</v>
@@ -11485,21 +11463,21 @@
         <v>22</v>
       </c>
       <c r="I260" s="3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="K260" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="L260" t="s">
         <v>977</v>
       </c>
-      <c r="L260" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>666</v>
       </c>
-      <c r="B261" s="11" t="s">
-        <v>979</v>
+      <c r="B261" t="s">
+        <v>978</v>
       </c>
       <c r="C261" t="s">
         <v>14</v>
@@ -11517,18 +11495,18 @@
         <v>1</v>
       </c>
       <c r="K261" t="s">
+        <v>979</v>
+      </c>
+      <c r="L261" s="3" t="s">
         <v>980</v>
       </c>
-      <c r="L261" s="3" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>666</v>
       </c>
-      <c r="B262" s="11" t="s">
-        <v>982</v>
+      <c r="B262" t="s">
+        <v>981</v>
       </c>
       <c r="C262" t="s">
         <v>14</v>
@@ -11548,18 +11526,18 @@
         <v>112</v>
       </c>
       <c r="K262" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="L262" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>666</v>
       </c>
-      <c r="B263" s="11" t="s">
-        <v>984</v>
+      <c r="B263" t="s">
+        <v>983</v>
       </c>
       <c r="C263" t="s">
         <v>14</v>
@@ -11577,18 +11555,18 @@
         <v>1</v>
       </c>
       <c r="K263" t="s">
+        <v>986</v>
+      </c>
+      <c r="L263" s="3" t="s">
         <v>987</v>
       </c>
-      <c r="L263" s="3" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>666</v>
       </c>
-      <c r="B264" s="11" t="s">
-        <v>985</v>
+      <c r="B264" t="s">
+        <v>984</v>
       </c>
       <c r="C264" t="s">
         <v>14</v>
@@ -11606,18 +11584,18 @@
         <v>1</v>
       </c>
       <c r="K264" t="s">
+        <v>988</v>
+      </c>
+      <c r="L264" s="3" t="s">
         <v>989</v>
       </c>
-      <c r="L264" s="3" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>666</v>
       </c>
-      <c r="B265" s="11" t="s">
-        <v>986</v>
+      <c r="B265" t="s">
+        <v>985</v>
       </c>
       <c r="C265" t="s">
         <v>14</v>
@@ -11635,13 +11613,13 @@
         <v>1</v>
       </c>
       <c r="K265" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="L265" s="3" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>666</v>
       </c>
@@ -11671,7 +11649,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>666</v>
       </c>
@@ -11701,7 +11679,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>666</v>
       </c>
@@ -11731,7 +11709,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>666</v>
       </c>
@@ -11760,7 +11738,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>666</v>
       </c>
@@ -11787,7 +11765,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>666</v>
       </c>
@@ -11817,7 +11795,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>666</v>
       </c>
@@ -11847,7 +11825,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>666</v>
       </c>
@@ -11877,7 +11855,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>666</v>
       </c>
@@ -11907,7 +11885,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>666</v>
       </c>
@@ -11937,7 +11915,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>666</v>
       </c>
@@ -11966,7 +11944,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>666</v>
       </c>
@@ -11995,7 +11973,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>666</v>
       </c>
@@ -12025,7 +12003,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>666</v>
       </c>
@@ -12055,7 +12033,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>666</v>
       </c>
@@ -12085,7 +12063,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>666</v>
       </c>
@@ -12115,7 +12093,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>666</v>
       </c>
@@ -12145,7 +12123,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>666</v>
       </c>
@@ -12175,12 +12153,12 @@
         <v>798</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>666</v>
       </c>
       <c r="B284" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C284" t="s">
         <v>90</v>
@@ -12198,18 +12176,18 @@
         <v>0</v>
       </c>
       <c r="K284" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="L284" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>666</v>
       </c>
       <c r="B285" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C285" t="s">
         <v>90</v>
@@ -12227,13 +12205,13 @@
         <v>0</v>
       </c>
       <c r="K285" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="L285" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>799</v>
       </c>
@@ -12259,7 +12237,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>799</v>
       </c>
@@ -12289,7 +12267,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>799</v>
       </c>
@@ -12319,7 +12297,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>799</v>
       </c>
@@ -12349,7 +12327,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>799</v>
       </c>
@@ -12379,7 +12357,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>799</v>
       </c>
@@ -12415,7 +12393,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>799</v>
       </c>
@@ -12445,7 +12423,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>799</v>
       </c>
@@ -12475,7 +12453,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>799</v>
       </c>
@@ -12505,7 +12483,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>799</v>
       </c>
@@ -12541,7 +12519,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>799</v>
       </c>
@@ -12575,7 +12553,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>799</v>
       </c>
@@ -12609,7 +12587,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>799</v>
       </c>
@@ -12643,7 +12621,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>799</v>
       </c>
@@ -12677,7 +12655,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>799</v>
       </c>
@@ -12711,7 +12689,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>799</v>
       </c>
@@ -12735,7 +12713,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>799</v>
       </c>
@@ -12771,7 +12749,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>799</v>
       </c>
@@ -12801,7 +12779,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>799</v>
       </c>
@@ -12831,7 +12809,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>799</v>
       </c>
@@ -12861,7 +12839,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>799</v>
       </c>
@@ -12891,7 +12869,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>799</v>
       </c>
@@ -12921,7 +12899,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>799</v>
       </c>
@@ -12951,7 +12929,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>799</v>
       </c>
@@ -12987,7 +12965,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>799</v>
       </c>
@@ -13017,7 +12995,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>799</v>
       </c>
@@ -13047,7 +13025,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>799</v>
       </c>
@@ -13077,7 +13055,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>799</v>
       </c>
@@ -13107,7 +13085,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>799</v>
       </c>
@@ -13137,7 +13115,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>799</v>
       </c>
@@ -13167,7 +13145,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="316" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>799</v>
       </c>
@@ -13197,7 +13175,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>799</v>
       </c>
@@ -13227,7 +13205,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>799</v>
       </c>
@@ -13263,7 +13241,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>799</v>
       </c>
@@ -13296,7 +13274,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>799</v>
       </c>
@@ -13329,7 +13307,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>799</v>
       </c>
@@ -13359,7 +13337,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>799</v>
       </c>
@@ -13389,7 +13367,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>799</v>
       </c>
@@ -13422,7 +13400,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>799</v>
       </c>
@@ -13452,7 +13430,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>799</v>
       </c>
@@ -13482,7 +13460,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="326" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>799</v>
       </c>
@@ -13512,7 +13490,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>799</v>
       </c>
@@ -13542,7 +13520,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="328" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>799</v>
       </c>
@@ -13572,7 +13550,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="329" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>799</v>
       </c>
@@ -13599,7 +13577,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="330" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>799</v>
       </c>
@@ -13629,7 +13607,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="331" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>799</v>
       </c>

</xml_diff>

<commit_message>
updated curved curtain default value
</commit_message>
<xml_diff>
--- a/tools/variable_map.xlsx
+++ b/tools/variable_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WHamilt2\Documents\solarPILOT_build\SolarPILOT\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB70C4B6-97F2-49D8-B17F-622B9FA5F3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7ECBAA-3B4F-4D1C-BDB7-D14AE380F768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3477,7 +3477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3487,29 +3487,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L256" sqref="L256"/>
+      <selection pane="bottomLeft" activeCell="E261" sqref="E261"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="114.42578125" customWidth="1"/>
-    <col min="13" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="39.54296875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="114.453125" customWidth="1"/>
+    <col min="13" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>97</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>97</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>97</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>190</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>190</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>190</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>190</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>190</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>190</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>190</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>190</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>190</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>190</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>190</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>190</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>190</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>190</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>190</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>190</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>190</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>190</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>190</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>190</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>190</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>190</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>190</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>190</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>190</v>
       </c>
@@ -6179,7 +6179,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>190</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>190</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>190</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>190</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>190</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>190</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>190</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>190</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>190</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>190</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>332</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>332</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>332</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>332</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>332</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>332</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>332</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>332</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>332</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>332</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>332</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>332</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>332</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>332</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>332</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>332</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>332</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>332</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>332</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>332</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>332</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>332</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>332</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>332</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>332</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>332</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>332</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>332</v>
       </c>
@@ -7441,7 +7441,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>332</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>332</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>332</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>332</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>332</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>332</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>332</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>332</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>332</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>332</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>332</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>332</v>
       </c>
@@ -7803,7 +7803,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>332</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>332</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>332</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>332</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>332</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>332</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>332</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>332</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>332</v>
       </c>
@@ -8082,7 +8082,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>332</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>332</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>332</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>332</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>332</v>
       </c>
@@ -8232,7 +8232,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>332</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>332</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>332</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>332</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>332</v>
       </c>
@@ -8382,7 +8382,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>332</v>
       </c>
@@ -8412,7 +8412,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>332</v>
       </c>
@@ -8442,7 +8442,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>332</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>332</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>513</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>513</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>513</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>513</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>513</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>513</v>
       </c>
@@ -8671,7 +8671,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>513</v>
       </c>
@@ -8705,7 +8705,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>513</v>
       </c>
@@ -8739,7 +8739,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>513</v>
       </c>
@@ -8773,7 +8773,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>513</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>513</v>
       </c>
@@ -8837,7 +8837,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>513</v>
       </c>
@@ -8867,7 +8867,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>513</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>513</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>513</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>513</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>513</v>
       </c>
@@ -9017,7 +9017,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>513</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>513</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>513</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>513</v>
       </c>
@@ -9137,7 +9137,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>513</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>576</v>
       </c>
@@ -9203,7 +9203,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>576</v>
       </c>
@@ -9225,7 +9225,7 @@
       </c>
       <c r="L188" s="3"/>
     </row>
-    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>576</v>
       </c>
@@ -9255,7 +9255,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>576</v>
       </c>
@@ -9288,7 +9288,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>576</v>
       </c>
@@ -9321,7 +9321,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>576</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>576</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>576</v>
       </c>
@@ -9414,7 +9414,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>576</v>
       </c>
@@ -9444,7 +9444,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>576</v>
       </c>
@@ -9474,7 +9474,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>576</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>576</v>
       </c>
@@ -9531,7 +9531,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>576</v>
       </c>
@@ -9561,7 +9561,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>576</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>576</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>619</v>
       </c>
@@ -9656,7 +9656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>619</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>619</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>619</v>
       </c>
@@ -9743,7 +9743,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>619</v>
       </c>
@@ -9774,7 +9774,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>619</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>619</v>
       </c>
@@ -9842,7 +9842,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>619</v>
       </c>
@@ -9876,7 +9876,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>619</v>
       </c>
@@ -9910,7 +9910,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>619</v>
       </c>
@@ -9944,7 +9944,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>619</v>
       </c>
@@ -9978,7 +9978,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>619</v>
       </c>
@@ -10012,7 +10012,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>619</v>
       </c>
@@ -10046,7 +10046,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>619</v>
       </c>
@@ -10080,7 +10080,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>619</v>
       </c>
@@ -10114,7 +10114,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>619</v>
       </c>
@@ -10138,7 +10138,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>619</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>619</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>666</v>
       </c>
@@ -10231,7 +10231,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>666</v>
       </c>
@@ -10267,7 +10267,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>666</v>
       </c>
@@ -10297,7 +10297,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>666</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>666</v>
       </c>
@@ -10363,7 +10363,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>666</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>666</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>666</v>
       </c>
@@ -10450,7 +10450,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>666</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>666</v>
       </c>
@@ -10509,7 +10509,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>666</v>
       </c>
@@ -10543,7 +10543,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>666</v>
       </c>
@@ -10577,7 +10577,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>666</v>
       </c>
@@ -10607,7 +10607,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>666</v>
       </c>
@@ -10640,7 +10640,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>666</v>
       </c>
@@ -10670,7 +10670,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>666</v>
       </c>
@@ -10706,7 +10706,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>666</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>666</v>
       </c>
@@ -10766,7 +10766,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>666</v>
       </c>
@@ -10796,7 +10796,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>666</v>
       </c>
@@ -10826,7 +10826,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>666</v>
       </c>
@@ -10856,7 +10856,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>666</v>
       </c>
@@ -10886,7 +10886,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>666</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>666</v>
       </c>
@@ -10948,7 +10948,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>666</v>
       </c>
@@ -10980,7 +10980,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>666</v>
       </c>
@@ -11012,7 +11012,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>666</v>
       </c>
@@ -11042,7 +11042,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>666</v>
       </c>
@@ -11072,7 +11072,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>666</v>
       </c>
@@ -11102,7 +11102,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>666</v>
       </c>
@@ -11129,7 +11129,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>666</v>
       </c>
@@ -11159,7 +11159,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>666</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>666</v>
       </c>
@@ -11219,7 +11219,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>666</v>
       </c>
@@ -11255,7 +11255,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>666</v>
       </c>
@@ -11291,7 +11291,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>666</v>
       </c>
@@ -11321,7 +11321,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>666</v>
       </c>
@@ -11350,7 +11350,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>666</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>666</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>666</v>
       </c>
@@ -11437,7 +11437,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>666</v>
       </c>
@@ -11472,7 +11472,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>666</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>30</v>
       </c>
       <c r="E261" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F261" s="2" t="s">
         <v>43</v>
@@ -11501,7 +11501,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>666</v>
       </c>
@@ -11532,7 +11532,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>666</v>
       </c>
@@ -11561,7 +11561,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>666</v>
       </c>
@@ -11590,7 +11590,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>666</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>666</v>
       </c>
@@ -11649,7 +11649,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>666</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>666</v>
       </c>
@@ -11709,7 +11709,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>666</v>
       </c>
@@ -11738,7 +11738,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>666</v>
       </c>
@@ -11765,7 +11765,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>666</v>
       </c>
@@ -11795,7 +11795,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>666</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>666</v>
       </c>
@@ -11855,7 +11855,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>666</v>
       </c>
@@ -11885,7 +11885,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>666</v>
       </c>
@@ -11915,7 +11915,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>666</v>
       </c>
@@ -11944,7 +11944,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>666</v>
       </c>
@@ -11973,7 +11973,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>666</v>
       </c>
@@ -12003,7 +12003,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>666</v>
       </c>
@@ -12033,7 +12033,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>666</v>
       </c>
@@ -12063,7 +12063,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>666</v>
       </c>
@@ -12093,7 +12093,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>666</v>
       </c>
@@ -12123,7 +12123,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>666</v>
       </c>
@@ -12153,7 +12153,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>666</v>
       </c>
@@ -12182,7 +12182,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>666</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>799</v>
       </c>
@@ -12237,7 +12237,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>799</v>
       </c>
@@ -12267,7 +12267,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>799</v>
       </c>
@@ -12297,7 +12297,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>799</v>
       </c>
@@ -12327,7 +12327,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>799</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>799</v>
       </c>
@@ -12393,7 +12393,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>799</v>
       </c>
@@ -12423,7 +12423,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>799</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>799</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>799</v>
       </c>
@@ -12519,7 +12519,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>799</v>
       </c>
@@ -12553,7 +12553,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>799</v>
       </c>
@@ -12587,7 +12587,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>799</v>
       </c>
@@ -12621,7 +12621,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>799</v>
       </c>
@@ -12655,7 +12655,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>799</v>
       </c>
@@ -12689,7 +12689,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>799</v>
       </c>
@@ -12713,7 +12713,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>799</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>799</v>
       </c>
@@ -12779,7 +12779,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>799</v>
       </c>
@@ -12809,7 +12809,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>799</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>799</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>799</v>
       </c>
@@ -12899,7 +12899,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>799</v>
       </c>
@@ -12929,7 +12929,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>799</v>
       </c>
@@ -12965,7 +12965,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>799</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>799</v>
       </c>
@@ -13025,7 +13025,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>799</v>
       </c>
@@ -13055,7 +13055,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>799</v>
       </c>
@@ -13085,7 +13085,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>799</v>
       </c>
@@ -13115,7 +13115,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>799</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="316" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>799</v>
       </c>
@@ -13175,7 +13175,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>799</v>
       </c>
@@ -13205,7 +13205,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>799</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>799</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>799</v>
       </c>
@@ -13307,7 +13307,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>799</v>
       </c>
@@ -13337,7 +13337,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>799</v>
       </c>
@@ -13367,7 +13367,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>799</v>
       </c>
@@ -13400,7 +13400,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>799</v>
       </c>
@@ -13430,7 +13430,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>799</v>
       </c>
@@ -13460,7 +13460,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="326" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>799</v>
       </c>
@@ -13490,7 +13490,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>799</v>
       </c>
@@ -13520,7 +13520,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="328" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>799</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="329" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>799</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="330" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>799</v>
       </c>
@@ -13607,7 +13607,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="331" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>799</v>
       </c>

</xml_diff>